<commit_message>
Update assembly instructions and parts list
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -9,10 +9,10 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1058</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1060</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="287">
   <si>
     <t xml:space="preserve">pic label</t>
   </si>
@@ -320,6 +320,15 @@
     <t xml:space="preserve">This provides mains power for the heaters. The LAB CONTROL UNIT is powered separately.</t>
   </si>
   <si>
+    <t xml:space="preserve">TC-PWC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick disconnect connectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional, but highly recommended for connecting to the inlet power module</t>
+  </si>
+  <si>
     <t xml:space="preserve">REAGENT PUMP UNIT – Linear Syringe Pumps</t>
   </si>
   <si>
@@ -669,6 +678,12 @@
   </si>
   <si>
     <t xml:space="preserve">Used to build the housing for the Reactor Unit and as support for the pumps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packing tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used to make a transparent door for the Reactor Unit housing</t>
   </si>
   <si>
     <t xml:space="preserve">Paint</t>
@@ -1271,15 +1286,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I1058"/>
+  <dimension ref="A1:I1060"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H81" activeCellId="0" sqref="H81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="H73" activeCellId="0" sqref="H73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -1914,49 +1929,48 @@
       </c>
       <c r="I35" s="22"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
+      <c r="E36" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F36" s="11"/>
-      <c r="H36" s="12"/>
+      <c r="H36" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="23"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="20"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B39" s="9" t="s">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="E38" s="23"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D39" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="12"/>
-      <c r="I39" s="15"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
@@ -1969,25 +1983,23 @@
         <v>105</v>
       </c>
       <c r="D40" s="10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="12" t="s">
+      <c r="H40" s="12"/>
+      <c r="I40" s="15"/>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="I40" s="15"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
+      <c r="B41" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="C41" s="24" t="s">
-        <v>109</v>
       </c>
       <c r="D41" s="10" t="n">
         <v>3</v>
@@ -1995,7 +2007,9 @@
       <c r="E41" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="12"/>
+      <c r="H41" s="12" t="s">
+        <v>109</v>
+      </c>
       <c r="I41" s="15"/>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,7 +2057,7 @@
       <c r="B44" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="24" t="s">
         <v>118</v>
       </c>
       <c r="D44" s="10" t="n">
@@ -2081,7 +2095,7 @@
       <c r="B46" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="9" t="s">
         <v>124</v>
       </c>
       <c r="D46" s="10" t="n">
@@ -2093,14 +2107,14 @@
       <c r="H46" s="12"/>
       <c r="I46" s="15"/>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
         <v>125</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="24" t="s">
         <v>127</v>
       </c>
       <c r="D47" s="10" t="n">
@@ -2109,24 +2123,18 @@
       <c r="E47" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="H47" s="12"/>
-      <c r="I47" s="22"/>
+      <c r="I47" s="15"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="C48" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>131</v>
       </c>
       <c r="D48" s="10" t="n">
         <v>3</v>
@@ -2134,21 +2142,24 @@
       <c r="E48" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="F48" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="G48" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H48" s="12"/>
-      <c r="I48" s="15"/>
+      <c r="I48" s="22"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="C49" s="24" t="s">
         <v>134</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>135</v>
       </c>
       <c r="D49" s="10" t="n">
         <v>3</v>
@@ -2156,145 +2167,146 @@
       <c r="E49" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="12" t="s">
-        <v>136</v>
-      </c>
+      <c r="G49" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H49" s="12"/>
       <c r="I49" s="15"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="C50" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="D50" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="I50" s="15"/>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E51" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I50" s="13"/>
-    </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="11"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="15"/>
-    </row>
-    <row r="52" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E52" s="23"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="20"/>
-    </row>
-    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9"/>
-      <c r="B53" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="0" t="n">
+      <c r="I51" s="13"/>
+    </row>
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="11"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" s="23"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="20"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E54" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H53" s="12"/>
-      <c r="I53" s="13"/>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D54" s="10" t="n">
+      <c r="H54" s="12"/>
+      <c r="I54" s="13"/>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E55" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H54" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="I54" s="15"/>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="11"/>
       <c r="H55" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I55" s="15"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
+      <c r="C56" s="9" t="s">
+        <v>146</v>
+      </c>
       <c r="D56" s="10"/>
       <c r="E56" s="11"/>
-      <c r="H56" s="12"/>
+      <c r="H56" s="12" t="s">
+        <v>147</v>
+      </c>
       <c r="I56" s="15"/>
     </row>
-    <row r="57" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E57" s="23"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="20"/>
-    </row>
-    <row r="58" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C58" s="9" t="s">
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="11"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D58" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H58" s="12" t="s">
+      <c r="E58" s="23"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="20"/>
+    </row>
+    <row r="59" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="I58" s="15"/>
-    </row>
-    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="C59" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="D59" s="10" t="n">
         <v>1</v>
@@ -2303,19 +2315,23 @@
         <v>12</v>
       </c>
       <c r="H59" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="I59" s="22"/>
-    </row>
-    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9"/>
       <c r="B60" s="9" t="s">
         <v>154</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D60" s="10"/>
+      <c r="D60" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E60" s="11" t="s">
         <v>12</v>
       </c>
@@ -2324,121 +2340,119 @@
       </c>
       <c r="I60" s="22"/>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9" t="s">
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="C61" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C61" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D61" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="D61" s="10"/>
       <c r="E61" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="25" t="s">
+      <c r="H61" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I61" s="22"/>
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="I61" s="15"/>
-    </row>
-    <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="9" t="s">
+      <c r="B62" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="C62" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="D62" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="25" t="s">
-        <v>164</v>
       </c>
       <c r="I62" s="15"/>
     </row>
     <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B63" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="C63" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C63" s="9" t="s">
-        <v>167</v>
-      </c>
       <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
+      <c r="E63" s="11"/>
       <c r="G63" s="10"/>
       <c r="H63" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="I63" s="15"/>
+    </row>
+    <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="I63" s="15"/>
-    </row>
-    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9" t="s">
+      <c r="B64" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="C64" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="D64" s="10" t="n">
+      <c r="I64" s="15"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D65" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="E65" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G64" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="H64" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="I64" s="15"/>
-    </row>
-    <row r="65" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B65" s="9" t="s">
+      <c r="G65" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="H65" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="D65" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E65" s="11" t="s">
+      <c r="I65" s="15"/>
+    </row>
+    <row r="66" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="H65" s="12" t="s">
+      <c r="B66" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="I65" s="15"/>
-    </row>
-    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>180</v>
       </c>
       <c r="D66" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H66" s="12" t="s">
         <v>181</v>
@@ -2457,15 +2471,15 @@
         <v>1</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="H67" s="12"/>
+        <v>180</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="I67" s="15"/>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="9" t="s">
-        <v>184</v>
-      </c>
+      <c r="A68" s="9"/>
       <c r="B68" s="9" t="s">
         <v>185</v>
       </c>
@@ -2476,15 +2490,12 @@
         <v>1</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="H68" s="12"/>
-      <c r="I68" s="22"/>
-    </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
         <v>187</v>
       </c>
@@ -2500,57 +2511,67 @@
       <c r="E69" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="F69" s="11" t="s">
+        <v>82</v>
+      </c>
       <c r="H69" s="12"/>
-      <c r="I69" s="15"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="16"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="1" t="s">
+      <c r="I69" s="22"/>
+    </row>
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="E71" s="23"/>
-      <c r="H71" s="19"/>
-      <c r="I71" s="20"/>
-    </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="9" t="s">
+      <c r="B70" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="C70" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="D70" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" s="12"/>
+      <c r="I70" s="15"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="16"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E72" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H72" s="12" t="s">
+      <c r="E72" s="23"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="20"/>
+    </row>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="I72" s="15"/>
-    </row>
-    <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9"/>
       <c r="B73" s="9" t="s">
         <v>195</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E73" s="11"/>
-      <c r="H73" s="12"/>
+      <c r="E73" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="I73" s="15"/>
     </row>
     <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9"/>
       <c r="B74" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E74" s="11"/>
       <c r="H74" s="12"/>
@@ -2559,55 +2580,52 @@
     <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9"/>
       <c r="B75" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E75" s="11"/>
       <c r="H75" s="12"/>
       <c r="I75" s="15"/>
     </row>
     <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B76" s="9"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="9" t="s">
+        <v>202</v>
+      </c>
       <c r="C76" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="D76" s="10" t="n">
-        <v>1</v>
+        <v>203</v>
       </c>
       <c r="E76" s="11"/>
       <c r="H76" s="12"/>
       <c r="I76" s="15"/>
     </row>
     <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="9"/>
+      <c r="A77" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="B77" s="9"/>
       <c r="C77" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D77" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="D77" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E77" s="11"/>
-      <c r="H77" s="12" t="s">
-        <v>204</v>
-      </c>
+      <c r="H77" s="12"/>
       <c r="I77" s="15"/>
     </row>
-    <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D78" s="10"/>
-      <c r="E78" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E78" s="11"/>
       <c r="H78" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I78" s="15"/>
     </row>
@@ -2615,14 +2633,14 @@
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D79" s="10"/>
       <c r="E79" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H79" s="12" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="I79" s="15"/>
     </row>
@@ -2630,7 +2648,7 @@
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D80" s="10"/>
       <c r="E80" s="11" t="s">
@@ -2641,31 +2659,31 @@
       </c>
       <c r="I80" s="15"/>
     </row>
-    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9" t="s">
-        <v>56</v>
+        <v>211</v>
       </c>
       <c r="D81" s="10"/>
-      <c r="E81" s="11"/>
+      <c r="E81" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H81" s="12" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="I81" s="15"/>
     </row>
-    <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
-        <v>211</v>
+        <v>56</v>
       </c>
       <c r="D82" s="10"/>
-      <c r="E82" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E82" s="11"/>
       <c r="H82" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I82" s="15"/>
     </row>
@@ -2673,66 +2691,81 @@
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
-        <v>213</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="D83" s="10"/>
       <c r="E83" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I83" s="15"/>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="9"/>
+      <c r="B84" s="9"/>
       <c r="C84" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>217</v>
+      </c>
+      <c r="I84" s="15"/>
+    </row>
+    <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E85" s="11"/>
+      <c r="H85" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="I85" s="15"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C86" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="H86" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="9"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="9"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="11"/>
-      <c r="H90" s="12"/>
-      <c r="I90" s="15"/>
-    </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="26"/>
-      <c r="B91" s="26"/>
-      <c r="C91" s="26"/>
-      <c r="H91" s="12"/>
-      <c r="I91" s="15"/>
-    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="26"/>
-      <c r="B92" s="26"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
       <c r="C92" s="9"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="11"/>
       <c r="H92" s="12"/>
+      <c r="I92" s="15"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="26"/>
       <c r="B93" s="26"/>
+      <c r="C93" s="26"/>
       <c r="H93" s="12"/>
+      <c r="I93" s="15"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="26"/>
       <c r="B94" s="26"/>
-      <c r="C94" s="26"/>
+      <c r="C94" s="9"/>
       <c r="H94" s="12"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="26"/>
       <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
       <c r="H95" s="12"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8513,9 +8546,21 @@
       <c r="C1058" s="26"/>
       <c r="H1058" s="12"/>
     </row>
+    <row r="1059" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1059" s="26"/>
+      <c r="B1059" s="26"/>
+      <c r="C1059" s="26"/>
+      <c r="H1059" s="12"/>
+    </row>
+    <row r="1060" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1060" s="26"/>
+      <c r="B1060" s="26"/>
+      <c r="C1060" s="26"/>
+      <c r="H1060" s="12"/>
+    </row>
   </sheetData>
-  <autoFilter ref="E1:E1058"/>
-  <conditionalFormatting sqref="A90:B1058 A1:B37 A71:B83 A39:B69">
+  <autoFilter ref="E1:E1060"/>
+  <conditionalFormatting sqref="A92:B1060 A1:B38 A72:B85 A40:B70">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
@@ -8549,7 +8594,7 @@
     <hyperlink ref="E32" r:id="rId26" display="link"/>
     <hyperlink ref="E34" r:id="rId27" display="link"/>
     <hyperlink ref="E35" r:id="rId28" display="link"/>
-    <hyperlink ref="E39" r:id="rId29" display="link"/>
+    <hyperlink ref="E36" r:id="rId29" display="link"/>
     <hyperlink ref="E40" r:id="rId30" display="link"/>
     <hyperlink ref="E41" r:id="rId31" display="link"/>
     <hyperlink ref="E42" r:id="rId32" display="link"/>
@@ -8558,30 +8603,31 @@
     <hyperlink ref="E45" r:id="rId35" display="link"/>
     <hyperlink ref="E46" r:id="rId36" display="link"/>
     <hyperlink ref="E47" r:id="rId37" display="link"/>
-    <hyperlink ref="F47" r:id="rId38" display="link"/>
-    <hyperlink ref="E48" r:id="rId39" display="link"/>
+    <hyperlink ref="E48" r:id="rId38" display="link"/>
+    <hyperlink ref="F48" r:id="rId39" display="link"/>
     <hyperlink ref="E49" r:id="rId40" display="link"/>
     <hyperlink ref="E50" r:id="rId41" display="link"/>
-    <hyperlink ref="E53" r:id="rId42" display="link"/>
+    <hyperlink ref="E51" r:id="rId42" display="link"/>
     <hyperlink ref="E54" r:id="rId43" display="link"/>
-    <hyperlink ref="E58" r:id="rId44" display="link"/>
-    <hyperlink ref="H58" r:id="rId45" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E59" r:id="rId46" display="link"/>
+    <hyperlink ref="E55" r:id="rId44" display="link"/>
+    <hyperlink ref="E59" r:id="rId45" display="link"/>
+    <hyperlink ref="H59" r:id="rId46" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
     <hyperlink ref="E60" r:id="rId47" display="link"/>
     <hyperlink ref="E61" r:id="rId48" display="link"/>
-    <hyperlink ref="E64" r:id="rId49" display="link"/>
-    <hyperlink ref="E65" r:id="rId50" display="printed"/>
+    <hyperlink ref="E62" r:id="rId49" display="link"/>
+    <hyperlink ref="E65" r:id="rId50" display="link"/>
     <hyperlink ref="E66" r:id="rId51" display="printed"/>
     <hyperlink ref="E67" r:id="rId52" display="printed"/>
-    <hyperlink ref="E68" r:id="rId53" display="link"/>
-    <hyperlink ref="F68" r:id="rId54" display="6oz link"/>
-    <hyperlink ref="E69" r:id="rId55" display="link"/>
-    <hyperlink ref="E72" r:id="rId56" display="link"/>
-    <hyperlink ref="E78" r:id="rId57" display="link"/>
+    <hyperlink ref="E68" r:id="rId53" display="printed"/>
+    <hyperlink ref="E69" r:id="rId54" display="link"/>
+    <hyperlink ref="F69" r:id="rId55" display="6oz link"/>
+    <hyperlink ref="E70" r:id="rId56" display="link"/>
+    <hyperlink ref="E73" r:id="rId57" display="link"/>
     <hyperlink ref="E79" r:id="rId58" display="link"/>
     <hyperlink ref="E80" r:id="rId59" display="link"/>
-    <hyperlink ref="E82" r:id="rId60" display="link"/>
+    <hyperlink ref="E81" r:id="rId60" display="link"/>
     <hyperlink ref="E83" r:id="rId61" display="link"/>
+    <hyperlink ref="E84" r:id="rId62" display="link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8590,7 +8636,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId62"/>
+  <drawing r:id="rId63"/>
 </worksheet>
 </file>
 
@@ -8605,7 +8651,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>
@@ -8639,10 +8685,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8653,7 +8699,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>2</v>
@@ -8665,36 +8711,36 @@
         <v>14</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="I2" s="13" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="I3" s="13" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8702,7 +8748,7 @@
         <v>64</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>66</v>
@@ -8717,19 +8763,19 @@
         <v>13</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="I4" s="13" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="K4" s="13" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8740,7 +8786,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="D5" s="10" t="n">
         <v>1</v>
@@ -8753,18 +8799,18 @@
         <v>7.36</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>1</v>
@@ -8775,18 +8821,18 @@
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
       <c r="J6" s="10" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D7" s="10" t="n">
         <v>4</v>
@@ -8799,21 +8845,21 @@
         <v>9.99</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D8" s="10" t="n">
         <v>2</v>
@@ -8822,78 +8868,78 @@
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I8" s="13" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="I10" s="15" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D11" s="10" t="n">
         <v>1</v>
@@ -8902,67 +8948,67 @@
         <v>12</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="I11" s="13" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="11" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="12" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="I12" s="13" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="12" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="I13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
@@ -8971,14 +9017,14 @@
         <v>12</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="13" t="n">
         <v>3.82</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8989,7 +9035,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>1</v>
@@ -8998,13 +9044,13 @@
         <v>12</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="I15" s="13" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9015,7 +9061,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>1</v>
@@ -9028,7 +9074,7 @@
         <v>10.91</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9039,7 +9085,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>1</v>
@@ -9049,16 +9095,16 @@
       </c>
       <c r="F17" s="10"/>
       <c r="H17" s="12" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9078,13 +9124,13 @@
         <v>12</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="I18" s="13" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9110,7 +9156,7 @@
         <v>64.08</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9132,7 +9178,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="15"/>
       <c r="J20" s="10" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9156,18 +9202,18 @@
         <v>26.79</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D22" s="10" t="n">
         <v>2</v>
@@ -9178,18 +9224,18 @@
       <c r="H22" s="12"/>
       <c r="I22" s="15"/>
       <c r="J22" s="10" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="D23" s="10" t="n">
         <v>2</v>
@@ -9200,18 +9246,18 @@
       <c r="H23" s="12"/>
       <c r="I23" s="15"/>
       <c r="J23" s="10" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D24" s="10" t="n">
         <v>2</v>
@@ -9222,18 +9268,18 @@
       <c r="H24" s="12"/>
       <c r="I24" s="15"/>
       <c r="J24" s="10" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="D25" s="10" t="n">
         <v>2</v>
@@ -9244,18 +9290,18 @@
       <c r="H25" s="12"/>
       <c r="I25" s="15"/>
       <c r="J25" s="10" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="D26" s="10" t="n">
         <v>2</v>
@@ -9266,18 +9312,18 @@
       <c r="H26" s="12"/>
       <c r="I26" s="15"/>
       <c r="J26" s="10" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>2</v>
@@ -9288,40 +9334,40 @@
       <c r="H27" s="12"/>
       <c r="I27" s="15"/>
       <c r="J27" s="10" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="15"/>
       <c r="J28" s="10" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>2</v>
@@ -9333,55 +9379,55 @@
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="15" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="K29" s="10" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E31" s="28"/>
       <c r="H31" s="12"/>
@@ -9390,10 +9436,10 @@
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E32" s="28"/>
       <c r="H32" s="12"/>
@@ -9402,10 +9448,10 @@
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E33" s="28"/>
       <c r="H33" s="12"/>
@@ -9413,13 +9459,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D34" s="10" t="n">
         <v>2</v>
@@ -9428,25 +9474,25 @@
         <v>12</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="13" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D35" s="10" t="n">
         <v>1</v>
@@ -9462,13 +9508,13 @@
         <v>7.63</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="K35" s="10" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9490,18 +9536,18 @@
       <c r="H36" s="12"/>
       <c r="I36" s="15"/>
       <c r="J36" s="10" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D37" s="10" t="n">
         <v>2</v>
@@ -9510,22 +9556,22 @@
         <v>12</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>1.18</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="D38" s="10" t="n">
         <v>1</v>
@@ -9535,13 +9581,13 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D39" s="10" t="n">
         <v>1</v>
@@ -9554,37 +9600,37 @@
         <v>9.35</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="26"/>
       <c r="B40" s="9" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="I40" s="13" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26"/>
       <c r="B41" s="9" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="D41" s="10" t="n">
         <v>1</v>
@@ -9597,7 +9643,7 @@
         <v>8.99</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9611,7 +9657,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9619,32 +9665,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="10" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="10" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="I46" s="13" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9652,24 +9698,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="30" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="K48" s="30" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
More assembly documentation updates
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1063</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1064</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="306">
   <si>
     <t xml:space="preserve">pic label</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">Relay hat / relay board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use either a “hat” that fits directly over the Pi’s GPIO pins, or you can wire a relay board separately.</t>
   </si>
   <si>
     <t xml:space="preserve">13</t>
@@ -206,6 +209,15 @@
   </si>
   <si>
     <t xml:space="preserve">NOTE: Consider using a power supply that provides more than 2A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC-FAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5v or 12v fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These can be scavenged from old computers</t>
   </si>
   <si>
     <t xml:space="preserve">Extension cord</t>
@@ -1351,15 +1363,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:I1064"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
+      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -1485,7 +1497,7 @@
       </c>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>24</v>
       </c>
@@ -1504,18 +1516,20 @@
       <c r="F7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="I7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="10" t="n">
         <v>1</v>
@@ -1527,19 +1541,19 @@
         <v>13</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>1</v>
@@ -1548,19 +1562,19 @@
         <v>12</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>4</v>
@@ -1569,19 +1583,19 @@
         <v>12</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="10" t="n">
         <v>1</v>
@@ -1594,13 +1608,13 @@
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" s="10" t="n">
         <v>1</v>
@@ -1613,13 +1627,13 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" s="10" t="n">
         <v>1</v>
@@ -1633,10 +1647,10 @@
     <row r="14" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>1</v>
@@ -1645,17 +1659,17 @@
         <v>12</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>1</v>
@@ -1664,32 +1678,32 @@
         <v>12</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I15" s="15"/>
     </row>
-    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
+      <c r="B16" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="C16" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E16" s="11"/>
       <c r="H16" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>1</v>
@@ -1698,20 +1712,24 @@
         <v>12</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
+        <v>60</v>
+      </c>
+      <c r="D18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H18" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I18" s="15"/>
     </row>
@@ -1719,110 +1737,103 @@
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="11"/>
       <c r="H19" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I19" s="15"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="11"/>
-      <c r="H20" s="12"/>
+      <c r="H20" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="I20" s="15"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="14"/>
+      <c r="E21" s="11"/>
       <c r="H21" s="12"/>
       <c r="I21" s="15"/>
     </row>
-    <row r="22" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="9" t="s">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="14"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="10" t="n">
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="10" t="n">
         <v>2</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="22"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="10" t="n">
-        <v>1</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="11"/>
+      <c r="F25" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="H25" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9"/>
       <c r="B26" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D26" s="10" t="n">
         <v>1</v>
@@ -1831,14 +1842,18 @@
         <v>12</v>
       </c>
       <c r="F26" s="11"/>
-      <c r="H26" s="12"/>
+      <c r="H26" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="I26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
+      <c r="B27" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="C27" s="9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>1</v>
@@ -1847,18 +1862,14 @@
         <v>12</v>
       </c>
       <c r="F27" s="11"/>
-      <c r="H27" s="12" t="s">
-        <v>74</v>
-      </c>
+      <c r="H27" s="12"/>
       <c r="I27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9"/>
-      <c r="B28" s="9" t="s">
-        <v>75</v>
-      </c>
+      <c r="B28" s="9"/>
       <c r="C28" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
@@ -1868,47 +1879,49 @@
       </c>
       <c r="F28" s="11"/>
       <c r="H28" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9"/>
       <c r="B29" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D29" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="11"/>
-      <c r="H29" s="12"/>
+      <c r="H29" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I29" s="22"/>
     </row>
-    <row r="30" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9"/>
       <c r="B30" s="9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="10"/>
+        <v>83</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="E30" s="11" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="F30" s="11"/>
-      <c r="H30" s="12" t="s">
-        <v>83</v>
-      </c>
+      <c r="H30" s="12"/>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
         <v>84</v>
@@ -1918,21 +1931,21 @@
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="11" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="F31" s="11"/>
       <c r="H31" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="11" t="s">
@@ -1940,51 +1953,51 @@
       </c>
       <c r="F32" s="11"/>
       <c r="H32" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
+      <c r="E33" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F33" s="11"/>
       <c r="H33" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9"/>
       <c r="B34" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D34" s="10"/>
-      <c r="E34" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="H34" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I34" s="22"/>
     </row>
-    <row r="35" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="11" t="s">
@@ -1992,17 +2005,17 @@
       </c>
       <c r="F35" s="11"/>
       <c r="H35" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I35" s="22"/>
     </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="11" t="s">
@@ -2010,99 +2023,96 @@
       </c>
       <c r="F36" s="11"/>
       <c r="H36" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9"/>
       <c r="B37" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
+      <c r="E37" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F37" s="11"/>
       <c r="H37" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I37" s="22"/>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
+      <c r="B38" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="D38" s="10"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
-      <c r="H38" s="12"/>
+      <c r="H38" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E39" s="23"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="20"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="9" t="s">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="22"/>
+    </row>
+    <row r="40" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="12"/>
-      <c r="I41" s="15"/>
+      <c r="E40" s="23"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="20"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="8" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D42" s="10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="12" t="s">
-        <v>113</v>
-      </c>
+      <c r="H42" s="12"/>
       <c r="I42" s="15"/>
     </row>
-    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
         <v>114</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="9" t="s">
         <v>116</v>
       </c>
       <c r="D43" s="10" t="n">
@@ -2111,18 +2121,20 @@
       <c r="E43" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="12"/>
+      <c r="H43" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="I43" s="15"/>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D44" s="10" t="n">
         <v>3</v>
@@ -2135,13 +2147,13 @@
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D45" s="10" t="n">
         <v>3</v>
@@ -2154,13 +2166,13 @@
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" s="9" t="s">
         <v>125</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>126</v>
       </c>
       <c r="D46" s="10" t="n">
         <v>3</v>
@@ -2173,13 +2185,13 @@
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D47" s="10" t="n">
         <v>3</v>
@@ -2192,13 +2204,13 @@
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C48" s="24" t="s">
         <v>131</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="D48" s="10" t="n">
         <v>3</v>
@@ -2209,15 +2221,15 @@
       <c r="H48" s="12"/>
       <c r="I48" s="15"/>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C49" s="9" t="s">
         <v>134</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>135</v>
       </c>
       <c r="D49" s="10" t="n">
         <v>3</v>
@@ -2225,14 +2237,8 @@
       <c r="E49" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>135</v>
-      </c>
       <c r="H49" s="12"/>
-      <c r="I49" s="22"/>
+      <c r="I49" s="15"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
@@ -2241,7 +2247,7 @@
       <c r="B50" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="9" t="s">
         <v>138</v>
       </c>
       <c r="D50" s="10" t="n">
@@ -2250,11 +2256,14 @@
       <c r="E50" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="F50" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="G50" s="10" t="s">
         <v>139</v>
       </c>
       <c r="H50" s="12"/>
-      <c r="I50" s="15"/>
+      <c r="I50" s="22"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
@@ -2263,7 +2272,7 @@
       <c r="B51" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="24" t="s">
         <v>142</v>
       </c>
       <c r="D51" s="10" t="n">
@@ -2272,9 +2281,10 @@
       <c r="E51" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H51" s="12" t="s">
+      <c r="G51" s="10" t="s">
         <v>143</v>
       </c>
+      <c r="H51" s="12"/>
       <c r="I51" s="15"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,130 +2297,130 @@
       <c r="C52" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="D52" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="11"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="15"/>
-    </row>
-    <row r="54" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="1" t="s">
+      <c r="H52" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="E54" s="23"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="20"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="8" t="s">
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="E55" s="14"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="13"/>
-    </row>
-    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I53" s="13"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="11"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="16"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" s="23"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="20"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9"/>
-      <c r="B56" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>12</v>
-      </c>
+      <c r="B56" s="9"/>
+      <c r="C56" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" s="14"/>
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="s">
-        <v>140</v>
-      </c>
+    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9"/>
       <c r="B57" s="9" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D57" s="10" t="n">
+        <v>154</v>
+      </c>
+      <c r="D57" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="E57" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H57" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="I57" s="15"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="13"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
+      <c r="A58" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="C58" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D58" s="10"/>
-      <c r="E58" s="11"/>
+        <v>146</v>
+      </c>
+      <c r="D58" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H58" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I58" s="15"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
+      <c r="C59" s="9" t="s">
+        <v>155</v>
+      </c>
       <c r="D59" s="10"/>
       <c r="E59" s="11"/>
-      <c r="H59" s="12"/>
+      <c r="H59" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="I59" s="15"/>
     </row>
-    <row r="60" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="16"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E60" s="23"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="20"/>
-    </row>
-    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D61" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H61" s="12" t="s">
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="11"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I61" s="15"/>
+      <c r="E61" s="23"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="20"/>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
@@ -2431,47 +2441,47 @@
       <c r="H62" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="I62" s="22"/>
+      <c r="I62" s="15"/>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="9"/>
+      <c r="A63" s="9" t="s">
+        <v>162</v>
+      </c>
       <c r="B63" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D63" s="10"/>
+        <v>164</v>
+      </c>
+      <c r="D63" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E63" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H63" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I63" s="22"/>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9" t="s">
-        <v>165</v>
-      </c>
+    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="9"/>
       <c r="B64" s="9" t="s">
         <v>166</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D64" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="D64" s="10"/>
       <c r="E64" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H64" s="25" t="s">
+      <c r="H64" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="I64" s="15"/>
-    </row>
-    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I64" s="22"/>
+    </row>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
         <v>169</v>
       </c>
@@ -2481,9 +2491,12 @@
       <c r="C65" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="11"/>
-      <c r="G65" s="10"/>
+      <c r="D65" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H65" s="25" t="s">
         <v>172</v>
       </c>
@@ -2500,14 +2513,14 @@
         <v>175</v>
       </c>
       <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
+      <c r="E66" s="11"/>
       <c r="G66" s="10"/>
       <c r="H66" s="25" t="s">
         <v>176</v>
       </c>
       <c r="I66" s="15"/>
     </row>
-    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
         <v>177</v>
       </c>
@@ -2517,43 +2530,42 @@
       <c r="C67" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D67" s="10" t="n">
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="I67" s="15"/>
+    </row>
+    <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D68" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E67" s="11" t="s">
+      <c r="E68" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G67" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="H67" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="I67" s="15"/>
-    </row>
-    <row r="68" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="C68" s="9" t="s">
+      <c r="G68" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D68" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E68" s="11" t="s">
+      <c r="H68" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="H68" s="12" t="s">
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="I68" s="15"/>
-    </row>
-    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="9"/>
       <c r="B69" s="9" t="s">
         <v>187</v>
       </c>
@@ -2564,61 +2576,58 @@
         <v>1</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="H69" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I69" s="15"/>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9"/>
       <c r="B70" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D70" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="H70" s="12"/>
+        <v>189</v>
+      </c>
+      <c r="H70" s="12" t="s">
+        <v>193</v>
+      </c>
       <c r="I70" s="15"/>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="9" t="s">
-        <v>192</v>
-      </c>
+      <c r="A71" s="9"/>
       <c r="B71" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D71" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>82</v>
+        <v>189</v>
       </c>
       <c r="H71" s="12"/>
-      <c r="I71" s="22"/>
-    </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I71" s="15"/>
+    </row>
+    <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D72" s="10" t="n">
         <v>1</v>
@@ -2626,57 +2635,67 @@
       <c r="E72" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="F72" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="H72" s="12"/>
-      <c r="I72" s="15"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="16"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E74" s="23"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="20"/>
-    </row>
-    <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="9" t="s">
+      <c r="I72" s="22"/>
+    </row>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B73" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C73" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="E75" s="11" t="s">
+      <c r="D73" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H75" s="12" t="s">
+      <c r="H73" s="12"/>
+      <c r="I73" s="15"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="16"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="I75" s="15"/>
-    </row>
-    <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="9"/>
+      <c r="E75" s="23"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="20"/>
+    </row>
+    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="B76" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="E76" s="11"/>
-      <c r="H76" s="12"/>
+        <v>205</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H76" s="12" t="s">
+        <v>206</v>
+      </c>
       <c r="I76" s="15"/>
     </row>
     <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9"/>
       <c r="B77" s="9" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E77" s="11"/>
       <c r="H77" s="12"/>
@@ -2685,55 +2704,52 @@
     <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9"/>
       <c r="B78" s="9" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E78" s="11"/>
       <c r="H78" s="12"/>
       <c r="I78" s="15"/>
     </row>
     <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="B79" s="9"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="9" t="s">
+        <v>211</v>
+      </c>
       <c r="C79" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="D79" s="10" t="n">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="E79" s="11"/>
       <c r="H79" s="12"/>
       <c r="I79" s="15"/>
     </row>
     <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="9"/>
+      <c r="A80" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="B80" s="9"/>
       <c r="C80" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D80" s="10"/>
+        <v>214</v>
+      </c>
+      <c r="D80" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E80" s="11"/>
-      <c r="H80" s="12" t="s">
-        <v>212</v>
-      </c>
+      <c r="H80" s="12"/>
       <c r="I80" s="15"/>
     </row>
-    <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D81" s="10"/>
-      <c r="E81" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E81" s="11"/>
       <c r="H81" s="12" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="I81" s="15"/>
     </row>
@@ -2741,14 +2757,14 @@
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D82" s="10"/>
       <c r="E82" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H82" s="12" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="I82" s="15"/>
     </row>
@@ -2756,42 +2772,42 @@
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D83" s="10"/>
       <c r="E83" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I83" s="15"/>
     </row>
-    <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9" t="s">
-        <v>56</v>
+        <v>220</v>
       </c>
       <c r="D84" s="10"/>
-      <c r="E84" s="11"/>
+      <c r="E84" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H84" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I84" s="15"/>
     </row>
-    <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9" t="s">
-        <v>219</v>
+        <v>60</v>
       </c>
       <c r="D85" s="10"/>
-      <c r="E85" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E85" s="11"/>
       <c r="H85" s="12" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I85" s="15"/>
     </row>
@@ -2799,25 +2815,28 @@
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9" t="s">
-        <v>221</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="D86" s="10"/>
       <c r="E86" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H86" s="12" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="I86" s="15"/>
     </row>
-    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="E87" s="11"/>
+        <v>225</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H87" s="12" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="I87" s="15"/>
     </row>
@@ -2825,71 +2844,77 @@
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E88" s="11"/>
       <c r="H88" s="12" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I88" s="15"/>
     </row>
     <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
       <c r="C89" s="9" t="s">
-        <v>227</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="E89" s="11"/>
       <c r="H89" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>230</v>
+      </c>
+      <c r="I89" s="15"/>
+    </row>
+    <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="D90" s="0" t="n">
+        <v>231</v>
+      </c>
+      <c r="H90" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D91" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E90" s="11" t="s">
+      <c r="E91" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H90" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H91" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="9"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="11"/>
-      <c r="H95" s="12"/>
-      <c r="I95" s="15"/>
-    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="26"/>
-      <c r="B96" s="26"/>
-      <c r="C96" s="26"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="11"/>
       <c r="H96" s="12"/>
       <c r="I96" s="15"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="26"/>
       <c r="B97" s="26"/>
-      <c r="C97" s="9"/>
+      <c r="C97" s="26"/>
       <c r="H97" s="12"/>
+      <c r="I97" s="15"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="26"/>
       <c r="B98" s="26"/>
+      <c r="C98" s="9"/>
       <c r="H98" s="12"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="26"/>
       <c r="B99" s="26"/>
-      <c r="C99" s="26"/>
       <c r="H99" s="12"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8676,10 +8701,15 @@
       <c r="C1063" s="26"/>
       <c r="H1063" s="12"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1064" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1064" s="26"/>
+      <c r="B1064" s="26"/>
+      <c r="C1064" s="26"/>
+      <c r="H1064" s="12"/>
+    </row>
   </sheetData>
-  <autoFilter ref="E1:E1063"/>
-  <conditionalFormatting sqref="A95:B1063 A1:B39 A74:B88 A41:B72">
+  <autoFilter ref="E1:E1064"/>
+  <conditionalFormatting sqref="A96:B1064 A1:B40 A75:B89 A42:B73">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
@@ -8699,55 +8729,55 @@
     <hyperlink ref="E13" r:id="rId12" display="link"/>
     <hyperlink ref="E14" r:id="rId13" display="link"/>
     <hyperlink ref="E15" r:id="rId14" display="link"/>
-    <hyperlink ref="E16" r:id="rId15" display="link"/>
-    <hyperlink ref="E17" r:id="rId16" display="link"/>
-    <hyperlink ref="E24" r:id="rId17" display="link"/>
-    <hyperlink ref="F24" r:id="rId18" display="link2"/>
-    <hyperlink ref="E25" r:id="rId19" display="link"/>
-    <hyperlink ref="E26" r:id="rId20" display="link"/>
-    <hyperlink ref="E27" r:id="rId21" display="link"/>
-    <hyperlink ref="E28" r:id="rId22" display="link"/>
-    <hyperlink ref="E29" r:id="rId23" display="link"/>
-    <hyperlink ref="E30" r:id="rId24" display="6oz link"/>
-    <hyperlink ref="E31" r:id="rId25" display="link"/>
-    <hyperlink ref="E32" r:id="rId26" display="link"/>
-    <hyperlink ref="E34" r:id="rId27" display="link"/>
-    <hyperlink ref="E35" r:id="rId28" display="link"/>
-    <hyperlink ref="E36" r:id="rId29" display="link"/>
-    <hyperlink ref="E41" r:id="rId30" display="link"/>
-    <hyperlink ref="E42" r:id="rId31" display="link"/>
-    <hyperlink ref="E43" r:id="rId32" display="link"/>
-    <hyperlink ref="E44" r:id="rId33" display="link"/>
-    <hyperlink ref="E45" r:id="rId34" display="link"/>
-    <hyperlink ref="E46" r:id="rId35" display="link"/>
-    <hyperlink ref="E47" r:id="rId36" display="link"/>
-    <hyperlink ref="E48" r:id="rId37" display="link"/>
-    <hyperlink ref="E49" r:id="rId38" display="link"/>
-    <hyperlink ref="F49" r:id="rId39" display="link"/>
-    <hyperlink ref="E50" r:id="rId40" display="link"/>
-    <hyperlink ref="E51" r:id="rId41" display="link"/>
-    <hyperlink ref="E52" r:id="rId42" display="link"/>
-    <hyperlink ref="E56" r:id="rId43" display="link"/>
-    <hyperlink ref="E57" r:id="rId44" display="link"/>
-    <hyperlink ref="E61" r:id="rId45" display="link"/>
-    <hyperlink ref="H61" r:id="rId46" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E62" r:id="rId47" display="link"/>
-    <hyperlink ref="E63" r:id="rId48" display="link"/>
-    <hyperlink ref="E64" r:id="rId49" display="link"/>
-    <hyperlink ref="E67" r:id="rId50" display="link"/>
-    <hyperlink ref="E68" r:id="rId51" display="printed"/>
-    <hyperlink ref="E69" r:id="rId52" display="printed"/>
-    <hyperlink ref="E70" r:id="rId53" display="printed"/>
-    <hyperlink ref="E71" r:id="rId54" display="link"/>
-    <hyperlink ref="F71" r:id="rId55" display="6oz link"/>
-    <hyperlink ref="E72" r:id="rId56" display="link"/>
-    <hyperlink ref="E75" r:id="rId57" display="link"/>
-    <hyperlink ref="E81" r:id="rId58" display="link"/>
-    <hyperlink ref="E82" r:id="rId59" display="link"/>
-    <hyperlink ref="E83" r:id="rId60" display="link"/>
-    <hyperlink ref="E85" r:id="rId61" display="link"/>
-    <hyperlink ref="E86" r:id="rId62" display="link"/>
-    <hyperlink ref="E90" r:id="rId63" display="link"/>
+    <hyperlink ref="E17" r:id="rId15" display="link"/>
+    <hyperlink ref="E18" r:id="rId16" display="link"/>
+    <hyperlink ref="E25" r:id="rId17" display="link"/>
+    <hyperlink ref="F25" r:id="rId18" display="link2"/>
+    <hyperlink ref="E26" r:id="rId19" display="link"/>
+    <hyperlink ref="E27" r:id="rId20" display="link"/>
+    <hyperlink ref="E28" r:id="rId21" display="link"/>
+    <hyperlink ref="E29" r:id="rId22" display="link"/>
+    <hyperlink ref="E30" r:id="rId23" display="link"/>
+    <hyperlink ref="E31" r:id="rId24" display="6oz link"/>
+    <hyperlink ref="E32" r:id="rId25" display="link"/>
+    <hyperlink ref="E33" r:id="rId26" display="link"/>
+    <hyperlink ref="E35" r:id="rId27" display="link"/>
+    <hyperlink ref="E36" r:id="rId28" display="link"/>
+    <hyperlink ref="E37" r:id="rId29" display="link"/>
+    <hyperlink ref="E42" r:id="rId30" display="link"/>
+    <hyperlink ref="E43" r:id="rId31" display="link"/>
+    <hyperlink ref="E44" r:id="rId32" display="link"/>
+    <hyperlink ref="E45" r:id="rId33" display="link"/>
+    <hyperlink ref="E46" r:id="rId34" display="link"/>
+    <hyperlink ref="E47" r:id="rId35" display="link"/>
+    <hyperlink ref="E48" r:id="rId36" display="link"/>
+    <hyperlink ref="E49" r:id="rId37" display="link"/>
+    <hyperlink ref="E50" r:id="rId38" display="link"/>
+    <hyperlink ref="F50" r:id="rId39" display="link"/>
+    <hyperlink ref="E51" r:id="rId40" display="link"/>
+    <hyperlink ref="E52" r:id="rId41" display="link"/>
+    <hyperlink ref="E53" r:id="rId42" display="link"/>
+    <hyperlink ref="E57" r:id="rId43" display="link"/>
+    <hyperlink ref="E58" r:id="rId44" display="link"/>
+    <hyperlink ref="E62" r:id="rId45" display="link"/>
+    <hyperlink ref="H62" r:id="rId46" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
+    <hyperlink ref="E63" r:id="rId47" display="link"/>
+    <hyperlink ref="E64" r:id="rId48" display="link"/>
+    <hyperlink ref="E65" r:id="rId49" display="link"/>
+    <hyperlink ref="E68" r:id="rId50" display="link"/>
+    <hyperlink ref="E69" r:id="rId51" display="printed"/>
+    <hyperlink ref="E70" r:id="rId52" display="printed"/>
+    <hyperlink ref="E71" r:id="rId53" display="printed"/>
+    <hyperlink ref="E72" r:id="rId54" display="link"/>
+    <hyperlink ref="F72" r:id="rId55" display="6oz link"/>
+    <hyperlink ref="E73" r:id="rId56" display="link"/>
+    <hyperlink ref="E76" r:id="rId57" display="link"/>
+    <hyperlink ref="E82" r:id="rId58" display="link"/>
+    <hyperlink ref="E83" r:id="rId59" display="link"/>
+    <hyperlink ref="E84" r:id="rId60" display="link"/>
+    <hyperlink ref="E86" r:id="rId61" display="link"/>
+    <hyperlink ref="E87" r:id="rId62" display="link"/>
+    <hyperlink ref="E91" r:id="rId63" display="link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8771,7 +8801,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>
@@ -8805,10 +8835,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8819,7 +8849,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>2</v>
@@ -8831,47 +8861,47 @@
         <v>14</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I2" s="13" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="I3" s="13" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D4" s="10" t="n">
         <v>2</v>
@@ -8883,19 +8913,19 @@
         <v>13</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I4" s="13" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="K4" s="13" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8906,7 +8936,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D5" s="10" t="n">
         <v>1</v>
@@ -8919,18 +8949,18 @@
         <v>7.36</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>1</v>
@@ -8941,18 +8971,18 @@
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
       <c r="J6" s="10" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D7" s="10" t="n">
         <v>4</v>
@@ -8965,21 +8995,21 @@
         <v>9.99</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D8" s="10" t="n">
         <v>2</v>
@@ -8988,78 +9018,78 @@
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I8" s="13" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="I10" s="15" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D11" s="10" t="n">
         <v>1</v>
@@ -9068,67 +9098,67 @@
         <v>12</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="I11" s="13" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="11" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="12" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="I12" s="13" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="12" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="I13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
@@ -9137,14 +9167,14 @@
         <v>12</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="13" t="n">
         <v>3.82</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9155,7 +9185,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>1</v>
@@ -9164,13 +9194,13 @@
         <v>12</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="I15" s="13" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9181,7 +9211,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>1</v>
@@ -9194,18 +9224,18 @@
         <v>10.91</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>1</v>
@@ -9215,27 +9245,27 @@
       </c>
       <c r="F17" s="10"/>
       <c r="H17" s="12" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>1</v>
@@ -9244,24 +9274,24 @@
         <v>12</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="I18" s="13" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>4</v>
@@ -9270,24 +9300,24 @@
         <v>12</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I19" s="13" t="n">
         <v>64.08</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="D20" s="10" t="n">
         <v>1</v>
@@ -9298,18 +9328,18 @@
       <c r="H20" s="12"/>
       <c r="I20" s="15"/>
       <c r="J20" s="10" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D21" s="10" t="n">
         <v>1</v>
@@ -9322,18 +9352,18 @@
         <v>26.79</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D22" s="10" t="n">
         <v>2</v>
@@ -9344,18 +9374,18 @@
       <c r="H22" s="12"/>
       <c r="I22" s="15"/>
       <c r="J22" s="10" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D23" s="10" t="n">
         <v>2</v>
@@ -9366,18 +9396,18 @@
       <c r="H23" s="12"/>
       <c r="I23" s="15"/>
       <c r="J23" s="10" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D24" s="10" t="n">
         <v>2</v>
@@ -9388,18 +9418,18 @@
       <c r="H24" s="12"/>
       <c r="I24" s="15"/>
       <c r="J24" s="10" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D25" s="10" t="n">
         <v>2</v>
@@ -9410,18 +9440,18 @@
       <c r="H25" s="12"/>
       <c r="I25" s="15"/>
       <c r="J25" s="10" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D26" s="10" t="n">
         <v>2</v>
@@ -9432,18 +9462,18 @@
       <c r="H26" s="12"/>
       <c r="I26" s="15"/>
       <c r="J26" s="10" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>2</v>
@@ -9454,40 +9484,40 @@
       <c r="H27" s="12"/>
       <c r="I27" s="15"/>
       <c r="J27" s="10" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="15"/>
       <c r="J28" s="10" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>2</v>
@@ -9499,55 +9529,55 @@
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="15" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="K29" s="10" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E31" s="28"/>
       <c r="H31" s="12"/>
@@ -9556,10 +9586,10 @@
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E32" s="28"/>
       <c r="H32" s="12"/>
@@ -9568,10 +9598,10 @@
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="E33" s="28"/>
       <c r="H33" s="12"/>
@@ -9579,13 +9609,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D34" s="10" t="n">
         <v>2</v>
@@ -9594,25 +9624,25 @@
         <v>12</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="13" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D35" s="10" t="n">
         <v>1</v>
@@ -9621,31 +9651,31 @@
         <v>12</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="15" t="n">
         <v>7.63</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="K35" s="10" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D36" s="10" t="n">
         <v>1</v>
@@ -9656,18 +9686,18 @@
       <c r="H36" s="12"/>
       <c r="I36" s="15"/>
       <c r="J36" s="10" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D37" s="10" t="n">
         <v>2</v>
@@ -9676,22 +9706,22 @@
         <v>12</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>1.18</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D38" s="10" t="n">
         <v>1</v>
@@ -9701,13 +9731,13 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D39" s="10" t="n">
         <v>1</v>
@@ -9720,37 +9750,37 @@
         <v>9.35</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="26"/>
       <c r="B40" s="9" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="I40" s="13" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26"/>
       <c r="B41" s="9" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D41" s="10" t="n">
         <v>1</v>
@@ -9763,7 +9793,7 @@
         <v>8.99</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9777,7 +9807,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9785,32 +9815,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="10" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="10" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="I46" s="13" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9818,24 +9848,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="30" t="s">
+        <v>305</v>
+      </c>
+      <c r="J48" s="30" t="s">
         <v>301</v>
       </c>
-      <c r="J48" s="30" t="s">
-        <v>297</v>
-      </c>
       <c r="K48" s="30" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated parts list, handle thermometer read errors.
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -95,7 +95,7 @@
     <t xml:space="preserve">Touch screen</t>
   </si>
   <si>
-    <t xml:space="preserve">Linked screen is to a raspberry pi 4. Be sure to select a touchscreen that fits your Raspberry Pi or Libre Computer</t>
+    <t xml:space="preserve">Linked screen is to a raspberry pi 4. Be sure to select a touchscreen that fits your Raspberry Pi or Libre Computer. You will also need to download drivers that match your screen. The linked screen uses goodtft’s LCDshow.</t>
   </si>
   <si>
     <t xml:space="preserve">12</t>
@@ -1368,10 +1368,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="I5" s="15"/>
     </row>
-    <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
@@ -8718,66 +8718,67 @@
     <hyperlink ref="E4" r:id="rId1" display="link"/>
     <hyperlink ref="E5" r:id="rId2" display="link"/>
     <hyperlink ref="E6" r:id="rId3" display="link"/>
-    <hyperlink ref="E7" r:id="rId4" display="link"/>
-    <hyperlink ref="F7" r:id="rId5" display="link2"/>
-    <hyperlink ref="E8" r:id="rId6" display="link"/>
-    <hyperlink ref="F8" r:id="rId7" display="link2"/>
-    <hyperlink ref="E9" r:id="rId8" display="link"/>
-    <hyperlink ref="E10" r:id="rId9" display="link"/>
-    <hyperlink ref="E11" r:id="rId10" display="link"/>
-    <hyperlink ref="E12" r:id="rId11" display="link"/>
-    <hyperlink ref="E13" r:id="rId12" display="link"/>
-    <hyperlink ref="E14" r:id="rId13" display="link"/>
-    <hyperlink ref="E15" r:id="rId14" display="link"/>
-    <hyperlink ref="E17" r:id="rId15" display="link"/>
-    <hyperlink ref="E18" r:id="rId16" display="link"/>
-    <hyperlink ref="E25" r:id="rId17" display="link"/>
-    <hyperlink ref="F25" r:id="rId18" display="link2"/>
-    <hyperlink ref="E26" r:id="rId19" display="link"/>
-    <hyperlink ref="E27" r:id="rId20" display="link"/>
-    <hyperlink ref="E28" r:id="rId21" display="link"/>
-    <hyperlink ref="E29" r:id="rId22" display="link"/>
-    <hyperlink ref="E30" r:id="rId23" display="link"/>
-    <hyperlink ref="E31" r:id="rId24" display="6oz link"/>
-    <hyperlink ref="E32" r:id="rId25" display="link"/>
-    <hyperlink ref="E33" r:id="rId26" display="link"/>
-    <hyperlink ref="E35" r:id="rId27" display="link"/>
-    <hyperlink ref="E36" r:id="rId28" display="link"/>
-    <hyperlink ref="E37" r:id="rId29" display="link"/>
-    <hyperlink ref="E42" r:id="rId30" display="link"/>
-    <hyperlink ref="E43" r:id="rId31" display="link"/>
-    <hyperlink ref="E44" r:id="rId32" display="link"/>
-    <hyperlink ref="E45" r:id="rId33" display="link"/>
-    <hyperlink ref="E46" r:id="rId34" display="link"/>
-    <hyperlink ref="E47" r:id="rId35" display="link"/>
-    <hyperlink ref="E48" r:id="rId36" display="link"/>
-    <hyperlink ref="E49" r:id="rId37" display="link"/>
-    <hyperlink ref="E50" r:id="rId38" display="link"/>
-    <hyperlink ref="F50" r:id="rId39" display="link"/>
-    <hyperlink ref="E51" r:id="rId40" display="link"/>
-    <hyperlink ref="E52" r:id="rId41" display="link"/>
-    <hyperlink ref="E53" r:id="rId42" display="link"/>
-    <hyperlink ref="E57" r:id="rId43" display="link"/>
-    <hyperlink ref="E58" r:id="rId44" display="link"/>
-    <hyperlink ref="E62" r:id="rId45" display="link"/>
-    <hyperlink ref="H62" r:id="rId46" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E63" r:id="rId47" display="link"/>
-    <hyperlink ref="E64" r:id="rId48" display="link"/>
-    <hyperlink ref="E65" r:id="rId49" display="link"/>
-    <hyperlink ref="E68" r:id="rId50" display="link"/>
-    <hyperlink ref="E69" r:id="rId51" display="printed"/>
-    <hyperlink ref="E70" r:id="rId52" display="printed"/>
-    <hyperlink ref="E71" r:id="rId53" display="printed"/>
-    <hyperlink ref="E72" r:id="rId54" display="link"/>
-    <hyperlink ref="F72" r:id="rId55" display="6oz link"/>
-    <hyperlink ref="E73" r:id="rId56" display="link"/>
-    <hyperlink ref="E76" r:id="rId57" display="link"/>
-    <hyperlink ref="E82" r:id="rId58" display="link"/>
-    <hyperlink ref="E83" r:id="rId59" display="link"/>
-    <hyperlink ref="E84" r:id="rId60" display="link"/>
-    <hyperlink ref="E86" r:id="rId61" display="link"/>
-    <hyperlink ref="E87" r:id="rId62" display="link"/>
-    <hyperlink ref="E91" r:id="rId63" display="link"/>
+    <hyperlink ref="H6" r:id="rId4" display="goodtft’s LCDshow"/>
+    <hyperlink ref="E7" r:id="rId5" display="link"/>
+    <hyperlink ref="F7" r:id="rId6" display="link2"/>
+    <hyperlink ref="E8" r:id="rId7" display="link"/>
+    <hyperlink ref="F8" r:id="rId8" display="link2"/>
+    <hyperlink ref="E9" r:id="rId9" display="link"/>
+    <hyperlink ref="E10" r:id="rId10" display="link"/>
+    <hyperlink ref="E11" r:id="rId11" display="link"/>
+    <hyperlink ref="E12" r:id="rId12" display="link"/>
+    <hyperlink ref="E13" r:id="rId13" display="link"/>
+    <hyperlink ref="E14" r:id="rId14" display="link"/>
+    <hyperlink ref="E15" r:id="rId15" display="link"/>
+    <hyperlink ref="E17" r:id="rId16" display="link"/>
+    <hyperlink ref="E18" r:id="rId17" display="link"/>
+    <hyperlink ref="E25" r:id="rId18" display="link"/>
+    <hyperlink ref="F25" r:id="rId19" display="link2"/>
+    <hyperlink ref="E26" r:id="rId20" display="link"/>
+    <hyperlink ref="E27" r:id="rId21" display="link"/>
+    <hyperlink ref="E28" r:id="rId22" display="link"/>
+    <hyperlink ref="E29" r:id="rId23" display="link"/>
+    <hyperlink ref="E30" r:id="rId24" display="link"/>
+    <hyperlink ref="E31" r:id="rId25" display="6oz link"/>
+    <hyperlink ref="E32" r:id="rId26" display="link"/>
+    <hyperlink ref="E33" r:id="rId27" display="link"/>
+    <hyperlink ref="E35" r:id="rId28" display="link"/>
+    <hyperlink ref="E36" r:id="rId29" display="link"/>
+    <hyperlink ref="E37" r:id="rId30" display="link"/>
+    <hyperlink ref="E42" r:id="rId31" display="link"/>
+    <hyperlink ref="E43" r:id="rId32" display="link"/>
+    <hyperlink ref="E44" r:id="rId33" display="link"/>
+    <hyperlink ref="E45" r:id="rId34" display="link"/>
+    <hyperlink ref="E46" r:id="rId35" display="link"/>
+    <hyperlink ref="E47" r:id="rId36" display="link"/>
+    <hyperlink ref="E48" r:id="rId37" display="link"/>
+    <hyperlink ref="E49" r:id="rId38" display="link"/>
+    <hyperlink ref="E50" r:id="rId39" display="link"/>
+    <hyperlink ref="F50" r:id="rId40" display="link"/>
+    <hyperlink ref="E51" r:id="rId41" display="link"/>
+    <hyperlink ref="E52" r:id="rId42" display="link"/>
+    <hyperlink ref="E53" r:id="rId43" display="link"/>
+    <hyperlink ref="E57" r:id="rId44" display="link"/>
+    <hyperlink ref="E58" r:id="rId45" display="link"/>
+    <hyperlink ref="E62" r:id="rId46" display="link"/>
+    <hyperlink ref="H62" r:id="rId47" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
+    <hyperlink ref="E63" r:id="rId48" display="link"/>
+    <hyperlink ref="E64" r:id="rId49" display="link"/>
+    <hyperlink ref="E65" r:id="rId50" display="link"/>
+    <hyperlink ref="E68" r:id="rId51" display="link"/>
+    <hyperlink ref="E69" r:id="rId52" display="printed"/>
+    <hyperlink ref="E70" r:id="rId53" display="printed"/>
+    <hyperlink ref="E71" r:id="rId54" display="printed"/>
+    <hyperlink ref="E72" r:id="rId55" display="link"/>
+    <hyperlink ref="F72" r:id="rId56" display="6oz link"/>
+    <hyperlink ref="E73" r:id="rId57" display="link"/>
+    <hyperlink ref="E76" r:id="rId58" display="link"/>
+    <hyperlink ref="E82" r:id="rId59" display="link"/>
+    <hyperlink ref="E83" r:id="rId60" display="link"/>
+    <hyperlink ref="E84" r:id="rId61" display="link"/>
+    <hyperlink ref="E86" r:id="rId62" display="link"/>
+    <hyperlink ref="E87" r:id="rId63" display="link"/>
+    <hyperlink ref="E91" r:id="rId64" display="link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8786,7 +8787,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId64"/>
+  <drawing r:id="rId65"/>
 </worksheet>
 </file>
 
@@ -8801,7 +8802,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>

</xml_diff>

<commit_message>
Update parts list with copper tubing
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1064</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1066</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="312">
   <si>
     <t xml:space="preserve">pic label</t>
   </si>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">Circulating pump</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTE Operational limits to pumps in terms of capacity and temperature have not been determined. Larger or self-priming pumps may be desired for optimal operation, especially at high temperatures</t>
+    <t xml:space="preserve">NOTE Operational limits to pumps in terms of capacity and temperature have not been determined. Larger or self-priming pumps may be desired for optimal operation, especially at high temperatures.</t>
   </si>
   <si>
     <t xml:space="preserve">TC-HOU</t>
@@ -296,6 +296,24 @@
   </si>
   <si>
     <t xml:space="preserve">Submersible heater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-CTB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copper tubing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copper tubing should fit snugly within the silicone tubing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-STB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicone tubing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicone tubing should fit snugly around the copper tubing</t>
   </si>
   <si>
     <t xml:space="preserve">TC-JAR</t>
@@ -1363,15 +1381,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I1064"/>
+  <dimension ref="A1:I1066"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -1814,14 +1832,12 @@
         <v>70</v>
       </c>
       <c r="D25" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="F25" s="11"/>
       <c r="H25" s="12" t="s">
         <v>71</v>
       </c>
@@ -1921,7 +1937,7 @@
       <c r="H30" s="12"/>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
         <v>84</v>
@@ -1929,45 +1945,49 @@
       <c r="C31" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E31" s="11" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="F31" s="11"/>
       <c r="H31" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E32" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F32" s="11"/>
       <c r="H32" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="11" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="F33" s="11"/>
       <c r="H33" s="12" t="s">
@@ -1975,7 +1995,7 @@
       </c>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9"/>
       <c r="B34" s="9" t="s">
         <v>94</v>
@@ -1984,7 +2004,9 @@
         <v>95</v>
       </c>
       <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
+      <c r="E34" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F34" s="11"/>
       <c r="H34" s="12" t="s">
         <v>96</v>
@@ -2018,9 +2040,7 @@
         <v>101</v>
       </c>
       <c r="D36" s="10"/>
-      <c r="E36" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="H36" s="12" t="s">
         <v>102</v>
@@ -2045,7 +2065,7 @@
       </c>
       <c r="I37" s="22"/>
     </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9"/>
       <c r="B38" s="9" t="s">
         <v>106</v>
@@ -2054,90 +2074,86 @@
         <v>107</v>
       </c>
       <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
+      <c r="E38" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F38" s="11"/>
       <c r="H38" s="12" t="s">
         <v>108</v>
       </c>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
+      <c r="B39" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
+      <c r="E39" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F39" s="11"/>
-      <c r="H39" s="12"/>
+      <c r="H39" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="I39" s="22"/>
     </row>
-    <row r="40" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" s="23"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="20"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" s="9" t="s">
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C40" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D42" s="10" t="n">
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="H40" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I40" s="22"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="22"/>
+    </row>
+    <row r="42" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" s="23"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="20"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="10" t="n">
         <v>4</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" s="12"/>
-      <c r="I42" s="15"/>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I43" s="15"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" s="10" t="n">
-        <v>3</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>12</v>
@@ -2145,15 +2161,15 @@
       <c r="H44" s="12"/>
       <c r="I44" s="15"/>
     </row>
-    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="C45" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="C45" s="24" t="s">
-        <v>123</v>
       </c>
       <c r="D45" s="10" t="n">
         <v>3</v>
@@ -2161,7 +2177,9 @@
       <c r="E45" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="12"/>
+      <c r="H45" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="I45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2190,7 +2208,7 @@
       <c r="B47" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="24" t="s">
         <v>129</v>
       </c>
       <c r="D47" s="10" t="n">
@@ -2209,7 +2227,7 @@
       <c r="B48" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="24" t="s">
         <v>132</v>
       </c>
       <c r="D48" s="10" t="n">
@@ -2228,7 +2246,7 @@
       <c r="B49" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="9" t="s">
         <v>135</v>
       </c>
       <c r="D49" s="10" t="n">
@@ -2240,7 +2258,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="15"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
         <v>136</v>
       </c>
@@ -2256,24 +2274,18 @@
       <c r="E50" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="10" t="s">
+      <c r="H50" s="12"/>
+      <c r="I50" s="15"/>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="H50" s="12"/>
-      <c r="I50" s="22"/>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9" t="s">
+      <c r="B51" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="C51" s="24" t="s">
         <v>141</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>142</v>
       </c>
       <c r="D51" s="10" t="n">
         <v>3</v>
@@ -2281,21 +2293,18 @@
       <c r="E51" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G51" s="10" t="s">
-        <v>143</v>
-      </c>
       <c r="H51" s="12"/>
       <c r="I51" s="15"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>146</v>
       </c>
       <c r="D52" s="10" t="n">
         <v>3</v>
@@ -2303,193 +2312,202 @@
       <c r="E52" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H52" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I52" s="15"/>
+      <c r="F52" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H52" s="12"/>
+      <c r="I52" s="22"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="D53" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="H53" s="12"/>
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="B54" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="13"/>
-    </row>
-    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="11"/>
-      <c r="H54" s="12"/>
+      <c r="H54" s="12" t="s">
+        <v>153</v>
+      </c>
       <c r="I54" s="15"/>
     </row>
-    <row r="55" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E55" s="23"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="20"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I55" s="13"/>
+    </row>
+    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="24"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="11"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E57" s="23"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="20"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E58" s="14"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" s="12"/>
+      <c r="I59" s="13"/>
+    </row>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E56" s="14"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="13"/>
-    </row>
-    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9" t="s">
+      <c r="D60" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="C57" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D57" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H57" s="12"/>
-      <c r="I57" s="13"/>
-    </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D58" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H58" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I58" s="15"/>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="11"/>
-      <c r="H59" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="I59" s="15"/>
-    </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="11"/>
-      <c r="H60" s="12"/>
       <c r="I60" s="15"/>
     </row>
-    <row r="61" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="16"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E61" s="23"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="20"/>
-    </row>
-    <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D62" s="10" t="n">
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D61" s="10"/>
+      <c r="E61" s="11"/>
+      <c r="H61" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="11"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="15"/>
+    </row>
+    <row r="63" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E63" s="23"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="20"/>
+    </row>
+    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D64" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E62" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H62" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="I62" s="15"/>
-    </row>
-    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D63" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H63" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="I63" s="22"/>
-    </row>
-    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D64" s="10"/>
       <c r="E64" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H64" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="I64" s="15"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="I64" s="22"/>
-    </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="9" t="s">
+      <c r="B65" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="C65" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="D65" s="10" t="n">
         <v>1</v>
@@ -2497,132 +2515,132 @@
       <c r="E65" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="25" t="s">
+      <c r="H65" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="I65" s="22"/>
+    </row>
+    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="9"/>
+      <c r="B66" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="I65" s="15"/>
-    </row>
-    <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="D66" s="10"/>
+      <c r="E66" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="I66" s="22"/>
+    </row>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D66" s="10"/>
-      <c r="E66" s="11"/>
-      <c r="G66" s="10"/>
-      <c r="H66" s="25" t="s">
+      <c r="B67" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="I66" s="15"/>
-    </row>
-    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="s">
+      <c r="C67" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="D67" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="I67" s="15"/>
+    </row>
+    <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="G67" s="10"/>
-      <c r="H67" s="25" t="s">
+      <c r="B68" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="I67" s="15"/>
-    </row>
-    <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="9" t="s">
+      <c r="C68" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="D68" s="10"/>
+      <c r="E68" s="11"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D68" s="10" t="n">
+      <c r="B69" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="I69" s="15"/>
+    </row>
+    <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D70" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E68" s="11" t="s">
+      <c r="E70" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G68" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="H68" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="I68" s="15"/>
-    </row>
-    <row r="69" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D69" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E69" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="H69" s="12" t="s">
+      <c r="G70" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="I69" s="15"/>
-    </row>
-    <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9" t="s">
+      <c r="H70" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="I70" s="15"/>
+    </row>
+    <row r="71" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="D70" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="H70" s="12" t="s">
+      <c r="B71" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="I70" s="15"/>
-    </row>
-    <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9" t="s">
+      <c r="C71" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="D71" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="H71" s="12"/>
+        <v>195</v>
+      </c>
+      <c r="H71" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="I71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="9" t="s">
-        <v>196</v>
-      </c>
+      <c r="A72" s="9"/>
       <c r="B72" s="9" t="s">
         <v>197</v>
       </c>
@@ -2633,18 +2651,15 @@
         <v>1</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H72" s="12"/>
-      <c r="I72" s="22"/>
-    </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H72" s="12" t="s">
         <v>199</v>
       </c>
+      <c r="I72" s="15"/>
+    </row>
+    <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="9"/>
       <c r="B73" s="9" t="s">
         <v>200</v>
       </c>
@@ -2655,86 +2670,100 @@
         <v>1</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>12</v>
+        <v>195</v>
       </c>
       <c r="H73" s="12"/>
       <c r="I73" s="15"/>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="16"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="1" t="s">
+    <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E75" s="23"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="20"/>
-    </row>
-    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="9" t="s">
+      <c r="B74" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="C74" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="D74" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H74" s="12"/>
+      <c r="I74" s="22"/>
+    </row>
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="E76" s="11" t="s">
+      <c r="B75" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D75" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H76" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="I76" s="15"/>
-    </row>
-    <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C77" s="9" t="s">
+      <c r="H75" s="12"/>
+      <c r="I75" s="15"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="16"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E77" s="11"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="15"/>
-    </row>
-    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9"/>
+      <c r="E77" s="23"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="20"/>
+    </row>
+    <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="9" t="s">
+        <v>209</v>
+      </c>
       <c r="B78" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E78" s="11"/>
-      <c r="H78" s="12"/>
+        <v>211</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78" s="12" t="s">
+        <v>212</v>
+      </c>
       <c r="I78" s="15"/>
     </row>
     <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9"/>
       <c r="B79" s="9" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E79" s="11"/>
       <c r="H79" s="12"/>
       <c r="I79" s="15"/>
     </row>
     <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="B80" s="9"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="9" t="s">
+        <v>215</v>
+      </c>
       <c r="C80" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="D80" s="10" t="n">
-        <v>1</v>
+        <v>216</v>
       </c>
       <c r="E80" s="11"/>
       <c r="H80" s="12"/>
@@ -2742,44 +2771,41 @@
     </row>
     <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9"/>
-      <c r="B81" s="9"/>
+      <c r="B81" s="9" t="s">
+        <v>217</v>
+      </c>
       <c r="C81" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D81" s="10"/>
+        <v>218</v>
+      </c>
       <c r="E81" s="11"/>
-      <c r="H81" s="12" t="s">
-        <v>216</v>
-      </c>
+      <c r="H81" s="12"/>
       <c r="I81" s="15"/>
     </row>
-    <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="9"/>
+    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="9" t="s">
+        <v>219</v>
+      </c>
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="D82" s="10"/>
-      <c r="E82" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H82" s="12" t="s">
-        <v>218</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="D82" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" s="11"/>
+      <c r="H82" s="12"/>
       <c r="I82" s="15"/>
     </row>
-    <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D83" s="10"/>
-      <c r="E83" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E83" s="11"/>
       <c r="H83" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="I83" s="15"/>
     </row>
@@ -2787,27 +2813,29 @@
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="I84" s="15"/>
     </row>
-    <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="D85" s="10"/>
-      <c r="E85" s="11"/>
+      <c r="E85" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H85" s="12" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="I85" s="15"/>
     </row>
@@ -2815,118 +2843,134 @@
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D86" s="10"/>
       <c r="E86" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H86" s="12" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="I86" s="15"/>
     </row>
-    <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>12</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D87" s="10"/>
+      <c r="E87" s="11"/>
       <c r="H87" s="12" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I87" s="15"/>
     </row>
-    <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="E88" s="11"/>
+        <v>229</v>
+      </c>
+      <c r="D88" s="10"/>
+      <c r="E88" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H88" s="12" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="I88" s="15"/>
     </row>
-    <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="E89" s="11"/>
+        <v>231</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H89" s="12" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I89" s="15"/>
     </row>
     <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
       <c r="C90" s="9" t="s">
-        <v>231</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="E90" s="11"/>
       <c r="H90" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+      <c r="I90" s="15"/>
+    </row>
+    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
       <c r="C91" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D91" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="E91" s="11"/>
+      <c r="H91" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="I91" s="15"/>
+    </row>
+    <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="H92" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D93" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E91" s="11" t="s">
+      <c r="E93" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H91" s="12" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H93" s="12" t="s">
+        <v>240</v>
+      </c>
+    </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="9"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="11"/>
-      <c r="H96" s="12"/>
-      <c r="I96" s="15"/>
-    </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="26"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="26"/>
-      <c r="H97" s="12"/>
-      <c r="I97" s="15"/>
-    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="26"/>
-      <c r="B98" s="26"/>
+      <c r="A98" s="9"/>
+      <c r="B98" s="9"/>
       <c r="C98" s="9"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="11"/>
       <c r="H98" s="12"/>
+      <c r="I98" s="15"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="26"/>
       <c r="B99" s="26"/>
+      <c r="C99" s="26"/>
       <c r="H99" s="12"/>
+      <c r="I99" s="15"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="26"/>
       <c r="B100" s="26"/>
-      <c r="C100" s="26"/>
+      <c r="C100" s="9"/>
       <c r="H100" s="12"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="26"/>
       <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
       <c r="H101" s="12"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8707,9 +8751,21 @@
       <c r="C1064" s="26"/>
       <c r="H1064" s="12"/>
     </row>
+    <row r="1065" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1065" s="26"/>
+      <c r="B1065" s="26"/>
+      <c r="C1065" s="26"/>
+      <c r="H1065" s="12"/>
+    </row>
+    <row r="1066" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1066" s="26"/>
+      <c r="B1066" s="26"/>
+      <c r="C1066" s="26"/>
+      <c r="H1066" s="12"/>
+    </row>
   </sheetData>
-  <autoFilter ref="E1:E1064"/>
-  <conditionalFormatting sqref="A96:B1064 A1:B40 A75:B89 A42:B73">
+  <autoFilter ref="E1:E1066"/>
+  <conditionalFormatting sqref="A98:B1066 A1:B42 A77:B91 A44:B75">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
@@ -8718,7 +8774,7 @@
     <hyperlink ref="E4" r:id="rId1" display="link"/>
     <hyperlink ref="E5" r:id="rId2" display="link"/>
     <hyperlink ref="E6" r:id="rId3" display="link"/>
-    <hyperlink ref="H6" r:id="rId4" display="goodtft’s LCDshow"/>
+    <hyperlink ref="H6" r:id="rId4" display="Linked screen is to a raspberry pi 4. Be sure to select a touchscreen that fits your Raspberry Pi or Libre Computer. You will also need to download drivers that match your screen. The linked screen uses goodtft’s LCDshow."/>
     <hyperlink ref="E7" r:id="rId5" display="link"/>
     <hyperlink ref="F7" r:id="rId6" display="link2"/>
     <hyperlink ref="E8" r:id="rId7" display="link"/>
@@ -8733,52 +8789,53 @@
     <hyperlink ref="E17" r:id="rId16" display="link"/>
     <hyperlink ref="E18" r:id="rId17" display="link"/>
     <hyperlink ref="E25" r:id="rId18" display="link"/>
-    <hyperlink ref="F25" r:id="rId19" display="link2"/>
-    <hyperlink ref="E26" r:id="rId20" display="link"/>
-    <hyperlink ref="E27" r:id="rId21" display="link"/>
-    <hyperlink ref="E28" r:id="rId22" display="link"/>
-    <hyperlink ref="E29" r:id="rId23" display="link"/>
-    <hyperlink ref="E30" r:id="rId24" display="link"/>
-    <hyperlink ref="E31" r:id="rId25" display="6oz link"/>
-    <hyperlink ref="E32" r:id="rId26" display="link"/>
-    <hyperlink ref="E33" r:id="rId27" display="link"/>
+    <hyperlink ref="E26" r:id="rId19" display="link"/>
+    <hyperlink ref="E27" r:id="rId20" display="link"/>
+    <hyperlink ref="E28" r:id="rId21" display="link"/>
+    <hyperlink ref="E29" r:id="rId22" display="link"/>
+    <hyperlink ref="E30" r:id="rId23" display="link"/>
+    <hyperlink ref="E31" r:id="rId24" display="link"/>
+    <hyperlink ref="E32" r:id="rId25" display="link"/>
+    <hyperlink ref="E33" r:id="rId26" display="6oz link"/>
+    <hyperlink ref="E34" r:id="rId27" display="link"/>
     <hyperlink ref="E35" r:id="rId28" display="link"/>
-    <hyperlink ref="E36" r:id="rId29" display="link"/>
-    <hyperlink ref="E37" r:id="rId30" display="link"/>
-    <hyperlink ref="E42" r:id="rId31" display="link"/>
-    <hyperlink ref="E43" r:id="rId32" display="link"/>
-    <hyperlink ref="E44" r:id="rId33" display="link"/>
-    <hyperlink ref="E45" r:id="rId34" display="link"/>
-    <hyperlink ref="E46" r:id="rId35" display="link"/>
-    <hyperlink ref="E47" r:id="rId36" display="link"/>
-    <hyperlink ref="E48" r:id="rId37" display="link"/>
-    <hyperlink ref="E49" r:id="rId38" display="link"/>
-    <hyperlink ref="E50" r:id="rId39" display="link"/>
-    <hyperlink ref="F50" r:id="rId40" display="link"/>
-    <hyperlink ref="E51" r:id="rId41" display="link"/>
-    <hyperlink ref="E52" r:id="rId42" display="link"/>
-    <hyperlink ref="E53" r:id="rId43" display="link"/>
-    <hyperlink ref="E57" r:id="rId44" display="link"/>
-    <hyperlink ref="E58" r:id="rId45" display="link"/>
-    <hyperlink ref="E62" r:id="rId46" display="link"/>
-    <hyperlink ref="H62" r:id="rId47" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E63" r:id="rId48" display="link"/>
-    <hyperlink ref="E64" r:id="rId49" display="link"/>
-    <hyperlink ref="E65" r:id="rId50" display="link"/>
-    <hyperlink ref="E68" r:id="rId51" display="link"/>
-    <hyperlink ref="E69" r:id="rId52" display="printed"/>
-    <hyperlink ref="E70" r:id="rId53" display="printed"/>
-    <hyperlink ref="E71" r:id="rId54" display="printed"/>
-    <hyperlink ref="E72" r:id="rId55" display="link"/>
-    <hyperlink ref="F72" r:id="rId56" display="6oz link"/>
-    <hyperlink ref="E73" r:id="rId57" display="link"/>
-    <hyperlink ref="E76" r:id="rId58" display="link"/>
-    <hyperlink ref="E82" r:id="rId59" display="link"/>
-    <hyperlink ref="E83" r:id="rId60" display="link"/>
-    <hyperlink ref="E84" r:id="rId61" display="link"/>
+    <hyperlink ref="E37" r:id="rId29" display="link"/>
+    <hyperlink ref="E38" r:id="rId30" display="link"/>
+    <hyperlink ref="E39" r:id="rId31" display="link"/>
+    <hyperlink ref="E44" r:id="rId32" display="link"/>
+    <hyperlink ref="E45" r:id="rId33" display="link"/>
+    <hyperlink ref="E46" r:id="rId34" display="link"/>
+    <hyperlink ref="E47" r:id="rId35" display="link"/>
+    <hyperlink ref="E48" r:id="rId36" display="link"/>
+    <hyperlink ref="E49" r:id="rId37" display="link"/>
+    <hyperlink ref="E50" r:id="rId38" display="link"/>
+    <hyperlink ref="E51" r:id="rId39" display="link"/>
+    <hyperlink ref="E52" r:id="rId40" display="link"/>
+    <hyperlink ref="F52" r:id="rId41" display="link"/>
+    <hyperlink ref="E53" r:id="rId42" display="link"/>
+    <hyperlink ref="E54" r:id="rId43" display="link"/>
+    <hyperlink ref="E55" r:id="rId44" display="link"/>
+    <hyperlink ref="E59" r:id="rId45" display="link"/>
+    <hyperlink ref="E60" r:id="rId46" display="link"/>
+    <hyperlink ref="E64" r:id="rId47" display="link"/>
+    <hyperlink ref="H64" r:id="rId48" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
+    <hyperlink ref="E65" r:id="rId49" display="link"/>
+    <hyperlink ref="E66" r:id="rId50" display="link"/>
+    <hyperlink ref="E67" r:id="rId51" display="link"/>
+    <hyperlink ref="E70" r:id="rId52" display="link"/>
+    <hyperlink ref="E71" r:id="rId53" display="printed"/>
+    <hyperlink ref="E72" r:id="rId54" display="printed"/>
+    <hyperlink ref="E73" r:id="rId55" display="printed"/>
+    <hyperlink ref="E74" r:id="rId56" display="link"/>
+    <hyperlink ref="F74" r:id="rId57" display="6oz link"/>
+    <hyperlink ref="E75" r:id="rId58" display="link"/>
+    <hyperlink ref="E78" r:id="rId59" display="link"/>
+    <hyperlink ref="E84" r:id="rId60" display="link"/>
+    <hyperlink ref="E85" r:id="rId61" display="link"/>
     <hyperlink ref="E86" r:id="rId62" display="link"/>
-    <hyperlink ref="E87" r:id="rId63" display="link"/>
-    <hyperlink ref="E91" r:id="rId64" display="link"/>
+    <hyperlink ref="E88" r:id="rId63" display="link"/>
+    <hyperlink ref="E89" r:id="rId64" display="link"/>
+    <hyperlink ref="E93" r:id="rId65" display="link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8787,7 +8844,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId65"/>
+  <drawing r:id="rId66"/>
 </worksheet>
 </file>
 
@@ -8802,7 +8859,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>
@@ -8836,10 +8893,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8850,7 +8907,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>2</v>
@@ -8862,36 +8919,36 @@
         <v>14</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="I2" s="13" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="I3" s="13" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8899,10 +8956,10 @@
         <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="D4" s="10" t="n">
         <v>2</v>
@@ -8914,19 +8971,19 @@
         <v>13</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="I4" s="13" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="K4" s="13" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8937,7 +8994,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D5" s="10" t="n">
         <v>1</v>
@@ -8950,18 +9007,18 @@
         <v>7.36</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>1</v>
@@ -8972,18 +9029,18 @@
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
       <c r="J6" s="10" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D7" s="10" t="n">
         <v>4</v>
@@ -8996,21 +9053,21 @@
         <v>9.99</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D8" s="10" t="n">
         <v>2</v>
@@ -9019,78 +9076,78 @@
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="I8" s="13" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="I10" s="15" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D11" s="10" t="n">
         <v>1</v>
@@ -9099,67 +9156,67 @@
         <v>12</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="I11" s="13" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="11" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="12" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="I12" s="13" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="12" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="I13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
@@ -9168,14 +9225,14 @@
         <v>12</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="13" t="n">
         <v>3.82</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9186,7 +9243,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>1</v>
@@ -9195,13 +9252,13 @@
         <v>12</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="I15" s="13" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9212,7 +9269,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>1</v>
@@ -9225,7 +9282,7 @@
         <v>10.91</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9236,7 +9293,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>1</v>
@@ -9246,16 +9303,16 @@
       </c>
       <c r="F17" s="10"/>
       <c r="H17" s="12" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9266,7 +9323,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>1</v>
@@ -9275,13 +9332,13 @@
         <v>12</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="I18" s="13" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9292,7 +9349,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>4</v>
@@ -9307,7 +9364,7 @@
         <v>64.08</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9318,7 +9375,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D20" s="10" t="n">
         <v>1</v>
@@ -9329,7 +9386,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="15"/>
       <c r="J20" s="10" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9340,7 +9397,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D21" s="10" t="n">
         <v>1</v>
@@ -9353,18 +9410,18 @@
         <v>26.79</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D22" s="10" t="n">
         <v>2</v>
@@ -9375,18 +9432,18 @@
       <c r="H22" s="12"/>
       <c r="I22" s="15"/>
       <c r="J22" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="D23" s="10" t="n">
         <v>2</v>
@@ -9397,18 +9454,18 @@
       <c r="H23" s="12"/>
       <c r="I23" s="15"/>
       <c r="J23" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="D24" s="10" t="n">
         <v>2</v>
@@ -9419,18 +9476,18 @@
       <c r="H24" s="12"/>
       <c r="I24" s="15"/>
       <c r="J24" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="D25" s="10" t="n">
         <v>2</v>
@@ -9441,18 +9498,18 @@
       <c r="H25" s="12"/>
       <c r="I25" s="15"/>
       <c r="J25" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="D26" s="10" t="n">
         <v>2</v>
@@ -9463,18 +9520,18 @@
       <c r="H26" s="12"/>
       <c r="I26" s="15"/>
       <c r="J26" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>2</v>
@@ -9485,40 +9542,40 @@
       <c r="H27" s="12"/>
       <c r="I27" s="15"/>
       <c r="J27" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="15"/>
       <c r="J28" s="10" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>2</v>
@@ -9530,55 +9587,55 @@
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="15" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="K29" s="10" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="E31" s="28"/>
       <c r="H31" s="12"/>
@@ -9587,10 +9644,10 @@
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="E32" s="28"/>
       <c r="H32" s="12"/>
@@ -9599,10 +9656,10 @@
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E33" s="28"/>
       <c r="H33" s="12"/>
@@ -9610,13 +9667,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D34" s="10" t="n">
         <v>2</v>
@@ -9625,25 +9682,25 @@
         <v>12</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="13" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D35" s="10" t="n">
         <v>1</v>
@@ -9652,20 +9709,20 @@
         <v>12</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="15" t="n">
         <v>7.63</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="K35" s="10" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9687,18 +9744,18 @@
       <c r="H36" s="12"/>
       <c r="I36" s="15"/>
       <c r="J36" s="10" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="D37" s="10" t="n">
         <v>2</v>
@@ -9707,22 +9764,22 @@
         <v>12</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>1.18</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="D38" s="10" t="n">
         <v>1</v>
@@ -9732,13 +9789,13 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D39" s="10" t="n">
         <v>1</v>
@@ -9751,37 +9808,37 @@
         <v>9.35</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="26"/>
       <c r="B40" s="9" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="I40" s="13" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26"/>
       <c r="B41" s="9" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="D41" s="10" t="n">
         <v>1</v>
@@ -9794,7 +9851,7 @@
         <v>8.99</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9808,7 +9865,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9816,32 +9873,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="10" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="10" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="I46" s="13" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9849,24 +9906,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="30" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="K48" s="30" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update parts list: Remove old tubing, add notes
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1066</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1065</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="312">
   <si>
     <t xml:space="preserve">pic label</t>
   </si>
@@ -119,7 +119,8 @@
     <t xml:space="preserve">Raspberry Pi</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary link is to a 4 - 3b+'s seem hard to come by. We also have experimental support for Le Potato by Libre Computer</t>
+    <t xml:space="preserve">Primary link is to a Raspberry Pi. 4’s and 3b+'s seem hard to come by. 
+We also have experimental support for Le Potato by Libre Computer (link2).</t>
   </si>
   <si>
     <t xml:space="preserve">14</t>
@@ -298,24 +299,45 @@
     <t xml:space="preserve">Submersible heater</t>
   </si>
   <si>
+    <t xml:space="preserve">1 or 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC-CTB</t>
   </si>
   <si>
-    <t xml:space="preserve">Copper tubing</t>
+    <t xml:space="preserve">Copper tubing 1/4" OD x 3/16" ID</t>
   </si>
   <si>
     <t xml:space="preserve">Copper tubing should fit snugly within the silicone tubing</t>
   </si>
   <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC-STB</t>
   </si>
   <si>
-    <t xml:space="preserve">Silicone tubing</t>
+    <t xml:space="preserve">Silicone tubing 5mm ID x 7mm OD</t>
   </si>
   <si>
     <t xml:space="preserve">Silicone tubing should fit snugly around the copper tubing</t>
   </si>
   <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX-TEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barbed tee fittings for 6mm tubing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2429K55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase tubing compatible with your circulation pump and the copper heat exchanger!</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC-JAR</t>
   </si>
   <si>
@@ -391,10 +413,10 @@
     <t xml:space="preserve">Any “coozie” drink insulator or other insulator (like a knit hat) that will fit over the jar</t>
   </si>
   <si>
-    <t xml:space="preserve">REAGENT PUMP UNIT – Linear Syringe Pumps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE: Consider using peristaltic pumps instead. They work with the same stepper motor interface and require very little assembly.</t>
+    <t xml:space="preserve">REAGENT PUMP UNIT – Linear Syringe Pumps (DEPRECATED)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: We HIGHLY recommend using peristaltic pumps instead. They work with the same stepper motor interface and require very little assembly and fiddling.</t>
   </si>
   <si>
     <t xml:space="preserve">06</t>
@@ -571,16 +593,254 @@
     <t xml:space="preserve">NOTE: the motor mount is still under development and this coupling is not optimal</t>
   </si>
   <si>
-    <t xml:space="preserve">09</t>
+    <t xml:space="preserve">09C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX-RED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reducing fitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">might be needed – Purchase tubing compatible with your circulation pumps!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX-LID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reactor manifold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">printed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: the manifold can be a tight squeeze to pass through the mouth of the large mason jar, especially if your printer over-extrudes even slightly. Post-processing (i.e.: sand paper) may be necessary.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX-MMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mixing motor mount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: the motor mount is under development and does not exactly fit the linked motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX-RUC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reactor collar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX-COR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/6 oz mason jar for core chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX-OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1qt wide mouth mason jar for outer jacket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISCELLANEOUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-M310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3x10mm screw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon assortment contains all needed sizes and wrench 
+TODO: Which ones to use where?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-M320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3x20mm screw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-M340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3x40mm screw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-M3N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 nut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex wrench for syringe pump, M3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18g wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For miscellaneous connections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barrel plug connectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional, but good for modularity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barrel plug wires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12v button and lights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional, but nice for viewing the reaction chamber. Any 12v lights can be used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See the entry in the CONTROL UNIT for details – useful for assembly of the housing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Split loom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is optional but is very helpful for cable management!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thin plywood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used to build the housing for the Reactor Unit and as support for the pumps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corner supports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link 3 corner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link 2 corner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reinforcements for rear corners of the housing. We used upcycled plastic shipping corners because it allows the unit to disassemble and pack flat for shipping. Any bracket or method to stably join 3 faces of cube (4 times in the back) will work. The front corners are also joined but velcro straps alone seem to be sufficient there.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packing tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used to make a transparent door for the Reactor Unit housing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paint and stickers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have fun with it! Make the Microlab yours!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional, but good for storage and shipping. The linked one was the cheapest profile we could find at ~$25 ea. The control unit and assembled reaction chamber module can fit side by side in one case while the reactor housing and pumps pack flatish next to the temperature control parts. A broader, less deep profile would be more convenient, but those seemed to be more expensive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price Aug/Sep 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wire nuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lever connectors are better, orange wire nuts (video) will also work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McMasterCarr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or 1/8 inch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX-PMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">circulating pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mini pump (first link) may not withstand being sumberged in 100C water. The 5A pump in link 2 is almost certainly overkill, but should withstand high heat and is self-priming. Power supply connector here. Power supply here. We may want smaller pumps that can run at fewer amps (screw terminals seem to max out at 12v 5A, which is only half of what two of the larger pumps require.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lightobject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thermistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aliexpress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX-TMPD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB dongle for thermistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same link as thermistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">syringe slides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">right item?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mixing motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mixing paddle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mixing paddle needs to be coated. Stainless steel may react.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not available</t>
   </si>
   <si>
     <t xml:space="preserve">RX-TB5</t>
   </si>
   <si>
-    <t xml:space="preserve">Tubing 5-6mm x 8mm (1/4")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pump outlet – Purchase tubing compatible with your circulation pumps!</t>
+    <t xml:space="preserve">tubing 5-6mm x 8mm (1/4")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pump outlet</t>
   </si>
   <si>
     <t xml:space="preserve">09B</t>
@@ -589,349 +849,91 @@
     <t xml:space="preserve">RX-TB8</t>
   </si>
   <si>
-    <t xml:space="preserve">Tubing 8mm x 12mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pump inlet – Purchase tubing compatible with your circulation pumps!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX-RED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reducing fitting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">might be needed – Purchase tubing compatible with your circulation pumps!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX-TEE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barbed tee fittings for 6mm tubing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2429K55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase tubing compatible with your circulation pumps!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX-LID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reactor manifold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">printed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE: the manifold can be a tight squeeze to pass through the mouth of the large mason jar, especially if your printer over-extrudes even slightly. Post-processing (i.e.: sand paper) may be necessary.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX-MMM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mixing motor mount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE: the motor mount is under development and does not exactly fit the linked motor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX-RUC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reactor collar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX-COR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4/6 oz mason jar for core chamber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX-OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1qt wide mouth mason jar for outer jacket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISCELLANEOUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP-M310</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3x10mm screw</t>
+    <t xml:space="preserve">tubing 8mm x 12mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pump inlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">might be needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barbed tee fittings for 6mm tubing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McMaster Carr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">touch screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">screen is to a raspberry pi 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relay hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raspberry pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary link is to a 4 - 3b+'s seem hard to come by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~$12.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro SD card, 32GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motor drivers for CNC hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arduino CNC hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same link as motor drivers for CNC hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arduino UNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plunger holder tab (Linear Actuator V0 7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print instuctions not a thing to buy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">body holder (Linear Actuator V0 5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plunger holder base (Linear Actuator V0 7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motor end (Linear Actuator V0 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carriage (Linear Actuator V0 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idler end (Linear Actuator V0 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reactor manifold assembly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no print instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stepper motors</t>
   </si>
   <si>
     <t xml:space="preserve">Amazon assortment contains all needed sizes and wrench</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP-M320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3x20mm screw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP-M340</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3x40mm screw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP-M3N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3 nut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hex wrench for syringe pump, M3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18g wire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For miscellaneous connections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barrel plug connectors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional, but good for modularity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barrel plug wires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12v button and lights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional, but nice for viewing the reaction chamber. Any 12v lights can be used.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See the entry in the CONTROL UNIT for details – useful for assembly of the housing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Split loom </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is optional but is very helpful for cable management!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thin plywood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used to build the housing for the Reactor Unit and as support for the pumps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corner supports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reinforcements for rear corners of the housing. We used upcycled shipping corners.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packing tape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used to make a transparent door for the Reactor Unit housing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paint and stickers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have fun with it! Make the Microlab yours!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hard case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional, but good for storage and shipping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price Aug/Sep 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wire nuts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lever connectors are better, orange wire nuts (video) will also work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">McMasterCarr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">or 1/8 inch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amazon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX-PMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">circulating pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mini pump (first link) may not withstand being sumberged in 100C water. The 5A pump in link 2 is almost certainly overkill, but should withstand high heat and is self-priming. Power supply connector here. Power supply here. We may want smaller pumps that can run at fewer amps (screw terminals seem to max out at 12v 5A, which is only half of what two of the larger pumps require.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lightobject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thermistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aliexpress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX-TMPD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB dongle for thermistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">same link as thermistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">syringe slides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">right item?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mixing motor</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mixing paddle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mixing paddle needs to be coated. Stainless steel may react.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not available</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tubing 5-6mm x 8mm (1/4")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pump outlet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tubing 8mm x 12mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pump inlet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">might be needed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barbed tee fittings for 6mm tubing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">McMaster Carr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">touch screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">screen is to a raspberry pi 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relay hat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raspberry pi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary link is to a 4 - 3b+'s seem hard to come by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~$12.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro SD card, 32GB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32GB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">motor drivers for CNC hat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arduino CNC hat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">same link as motor drivers for CNC hat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arduino UNO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plunger holder tab (Linear Actuator V0 7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">print instuctions not a thing to buy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">body holder (Linear Actuator V0 5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plunger holder base (Linear Actuator V0 7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">motor end (Linear Actuator V0 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carriage (Linear Actuator V0 4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idler end (Linear Actuator V0 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reactor manifold assembly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no print instructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stepper motors</t>
   </si>
   <si>
     <t xml:space="preserve">not available </t>
@@ -1223,16 +1225,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1381,15 +1383,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I1066"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
+      <selection pane="bottomLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -1927,8 +1929,8 @@
       <c r="C30" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="10" t="n">
-        <v>2</v>
+      <c r="D30" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>12</v>
@@ -1940,10 +1942,10 @@
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D31" s="10" t="n">
         <v>1</v>
@@ -1953,17 +1955,19 @@
       </c>
       <c r="F31" s="11"/>
       <c r="H31" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9"/>
+      <c r="A32" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="B32" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D32" s="10" t="n">
         <v>1</v>
@@ -1973,53 +1977,59 @@
       </c>
       <c r="F32" s="11"/>
       <c r="H32" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9"/>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="B33" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="D33" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="E33" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F33" s="11"/>
-      <c r="H33" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="I33" s="22"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="I33" s="15"/>
+    </row>
+    <row r="34" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9"/>
       <c r="B34" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="11" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F34" s="11"/>
       <c r="H34" s="12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="11" t="s">
@@ -2027,51 +2037,51 @@
       </c>
       <c r="F35" s="11"/>
       <c r="H35" s="12" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I35" s="22"/>
     </row>
-    <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
+      <c r="E36" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F36" s="11"/>
       <c r="H36" s="12" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9"/>
       <c r="B37" s="9" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D37" s="10"/>
-      <c r="E37" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="H37" s="12" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I37" s="22"/>
     </row>
-    <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9"/>
       <c r="B38" s="9" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="11" t="s">
@@ -2079,17 +2089,17 @@
       </c>
       <c r="F38" s="11"/>
       <c r="H38" s="12" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9"/>
       <c r="B39" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="11" t="s">
@@ -2097,100 +2107,97 @@
       </c>
       <c r="F39" s="11"/>
       <c r="H39" s="12" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9"/>
       <c r="B40" s="9" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D40" s="10"/>
-      <c r="E40" s="11"/>
+      <c r="E40" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F40" s="11"/>
       <c r="H40" s="12" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I40" s="22"/>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
+      <c r="B41" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>120</v>
+      </c>
       <c r="D41" s="10"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
-      <c r="H41" s="12"/>
+      <c r="H41" s="12" t="s">
+        <v>121</v>
+      </c>
       <c r="I41" s="22"/>
     </row>
-    <row r="42" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E42" s="23"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="20"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" s="12"/>
-      <c r="I44" s="15"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="22"/>
+    </row>
+    <row r="43" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E43" s="24"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="20"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="8" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D45" s="10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="12" t="s">
-        <v>123</v>
-      </c>
+      <c r="H45" s="12"/>
       <c r="I45" s="15"/>
     </row>
-    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>126</v>
+        <v>128</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D46" s="10" t="n">
         <v>3</v>
@@ -2198,18 +2205,20 @@
       <c r="E46" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="12"/>
+      <c r="H46" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="I46" s="15"/>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>133</v>
       </c>
       <c r="D47" s="10" t="n">
         <v>3</v>
@@ -2222,13 +2231,13 @@
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>132</v>
+        <v>135</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>136</v>
       </c>
       <c r="D48" s="10" t="n">
         <v>3</v>
@@ -2241,13 +2250,13 @@
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>135</v>
+        <v>138</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>139</v>
       </c>
       <c r="D49" s="10" t="n">
         <v>3</v>
@@ -2260,13 +2269,13 @@
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D50" s="10" t="n">
         <v>3</v>
@@ -2279,13 +2288,13 @@
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>141</v>
+        <v>144</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="D51" s="10" t="n">
         <v>3</v>
@@ -2296,15 +2305,15 @@
       <c r="H51" s="12"/>
       <c r="I51" s="15"/>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>144</v>
+        <v>147</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>148</v>
       </c>
       <c r="D52" s="10" t="n">
         <v>3</v>
@@ -2312,24 +2321,18 @@
       <c r="E52" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>145</v>
-      </c>
       <c r="H52" s="12"/>
-      <c r="I52" s="22"/>
+      <c r="I52" s="15"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>148</v>
+        <v>150</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="D53" s="10" t="n">
         <v>3</v>
@@ -2337,21 +2340,24 @@
       <c r="E53" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="F53" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="G53" s="10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H53" s="12"/>
-      <c r="I53" s="15"/>
+      <c r="I53" s="22"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="D54" s="10" t="n">
         <v>3</v>
@@ -2359,155 +2365,156 @@
       <c r="E54" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H54" s="12" t="s">
-        <v>153</v>
-      </c>
+      <c r="G54" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="H54" s="12"/>
       <c r="I54" s="15"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E55" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D55" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I55" s="13"/>
-    </row>
-    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="11"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="15"/>
-    </row>
-    <row r="57" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E57" s="23"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="20"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E58" s="14"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="13"/>
-    </row>
-    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H55" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="11"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E58" s="24"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="20"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9"/>
-      <c r="B59" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D59" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>12</v>
-      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E59" s="14"/>
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9" t="s">
-        <v>150</v>
-      </c>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="9"/>
       <c r="B60" s="9" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D60" s="10" t="n">
+        <v>167</v>
+      </c>
+      <c r="D60" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E60" s="11" t="s">
+      <c r="E60" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H60" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="I60" s="15"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="13"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9"/>
+      <c r="A61" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>158</v>
+      </c>
       <c r="C61" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D61" s="10"/>
-      <c r="E61" s="11"/>
+        <v>159</v>
+      </c>
+      <c r="D61" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H61" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I61" s="15"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
+      <c r="C62" s="9" t="s">
+        <v>168</v>
+      </c>
       <c r="D62" s="10"/>
       <c r="E62" s="11"/>
-      <c r="H62" s="12"/>
+      <c r="H62" s="12" t="s">
+        <v>169</v>
+      </c>
       <c r="I62" s="15"/>
     </row>
-    <row r="63" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="16"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E63" s="23"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="20"/>
-    </row>
-    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D64" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H64" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="I64" s="15"/>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="11"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="15"/>
+    </row>
+    <row r="64" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E64" s="24"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="20"/>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D65" s="10" t="n">
         <v>1</v>
@@ -2516,174 +2523,155 @@
         <v>12</v>
       </c>
       <c r="H65" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="I65" s="22"/>
+        <v>174</v>
+      </c>
+      <c r="I65" s="15"/>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9"/>
+      <c r="A66" s="9" t="s">
+        <v>175</v>
+      </c>
       <c r="B66" s="9" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="D66" s="10"/>
+        <v>177</v>
+      </c>
+      <c r="D66" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E66" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H66" s="12" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="I66" s="22"/>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="s">
-        <v>175</v>
-      </c>
+    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="9"/>
       <c r="B67" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D67" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="D67" s="10"/>
       <c r="E67" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H67" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="I67" s="15"/>
+      <c r="H67" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I67" s="22"/>
     </row>
     <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D68" s="10"/>
-      <c r="E68" s="11"/>
+      <c r="E68" s="10"/>
       <c r="G68" s="10"/>
-      <c r="H68" s="25" t="s">
-        <v>182</v>
+      <c r="H68" s="23" t="s">
+        <v>185</v>
       </c>
       <c r="I68" s="15"/>
     </row>
-    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="G69" s="10"/>
-      <c r="H69" s="25" t="s">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="I69" s="15"/>
-    </row>
-    <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="9" t="s">
+      <c r="B70" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="C70" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="D70" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="D70" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="10" t="s">
+      <c r="H70" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="H70" s="25" t="s">
+      <c r="I70" s="15"/>
+    </row>
+    <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="I70" s="15"/>
-    </row>
-    <row r="71" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="9" t="s">
+      <c r="C71" s="9" t="s">
         <v>192</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>194</v>
       </c>
       <c r="D71" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H71" s="12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9"/>
       <c r="B72" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D72" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="H72" s="12" t="s">
-        <v>199</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="H72" s="12"/>
       <c r="I72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9"/>
+      <c r="A73" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="B73" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D73" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>195</v>
+        <v>12</v>
+      </c>
+      <c r="F73" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="H73" s="12"/>
-      <c r="I73" s="15"/>
-    </row>
-    <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I73" s="22"/>
+    </row>
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D74" s="10" t="n">
         <v>1</v>
@@ -2691,67 +2679,57 @@
       <c r="E74" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F74" s="11" t="s">
-        <v>92</v>
-      </c>
       <c r="H74" s="12"/>
-      <c r="I74" s="22"/>
-    </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="9" t="s">
+      <c r="I74" s="15"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="16"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E76" s="24"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="20"/>
+    </row>
+    <row r="77" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="E77" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H77" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="I77" s="15"/>
+    </row>
+    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="9"/>
+      <c r="B78" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D75" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H75" s="12"/>
-      <c r="I75" s="15"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="16"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="1" t="s">
+      <c r="C78" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E77" s="23"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="20"/>
-    </row>
-    <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H78" s="12" t="s">
-        <v>212</v>
-      </c>
+      <c r="E78" s="11"/>
+      <c r="H78" s="12"/>
       <c r="I78" s="15"/>
     </row>
     <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9"/>
       <c r="B79" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E79" s="11"/>
       <c r="H79" s="12"/>
@@ -2760,52 +2738,55 @@
     <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9"/>
       <c r="B80" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E80" s="11"/>
       <c r="H80" s="12"/>
       <c r="I80" s="15"/>
     </row>
     <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="9"/>
-      <c r="B81" s="9" t="s">
-        <v>217</v>
-      </c>
+      <c r="A81" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B81" s="9"/>
       <c r="C81" s="9" t="s">
-        <v>218</v>
+        <v>214</v>
+      </c>
+      <c r="D81" s="10" t="n">
+        <v>1</v>
       </c>
       <c r="E81" s="11"/>
       <c r="H81" s="12"/>
       <c r="I81" s="15"/>
     </row>
     <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="9" t="s">
-        <v>219</v>
-      </c>
+      <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="D82" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="D82" s="10"/>
       <c r="E82" s="11"/>
-      <c r="H82" s="12"/>
+      <c r="H82" s="12" t="s">
+        <v>216</v>
+      </c>
       <c r="I82" s="15"/>
     </row>
-    <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D83" s="10"/>
-      <c r="E83" s="11"/>
+      <c r="E83" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H83" s="12" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I83" s="15"/>
     </row>
@@ -2813,14 +2794,14 @@
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="I84" s="15"/>
     </row>
@@ -2828,42 +2809,42 @@
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D85" s="10"/>
       <c r="E85" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I85" s="15"/>
     </row>
-    <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9" t="s">
-        <v>226</v>
+        <v>60</v>
       </c>
       <c r="D86" s="10"/>
-      <c r="E86" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E86" s="11"/>
       <c r="H86" s="12" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="I86" s="15"/>
     </row>
-    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9" t="s">
-        <v>60</v>
+        <v>223</v>
       </c>
       <c r="D87" s="10"/>
-      <c r="E87" s="11"/>
+      <c r="E87" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H87" s="12" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I87" s="15"/>
     </row>
@@ -2871,28 +2852,30 @@
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="D88" s="10"/>
+        <v>225</v>
+      </c>
       <c r="E88" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H88" s="12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="I88" s="15"/>
     </row>
-    <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>12</v>
+        <v>228</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>229</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I89" s="15"/>
     </row>
@@ -2900,77 +2883,71 @@
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E90" s="11"/>
       <c r="H90" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="I90" s="15"/>
+    </row>
+    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="H91" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="I90" s="15"/>
-    </row>
-    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9" t="s">
+    </row>
+    <row r="92" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="E91" s="11"/>
-      <c r="H91" s="12" t="s">
+      <c r="D92" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="I91" s="15"/>
-    </row>
-    <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="H92" s="12" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="D93" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E93" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H93" s="12" t="s">
-        <v>240</v>
-      </c>
-    </row>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="11"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="15"/>
+    </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="9"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="11"/>
+      <c r="A98" s="26"/>
+      <c r="B98" s="26"/>
+      <c r="C98" s="26"/>
       <c r="H98" s="12"/>
       <c r="I98" s="15"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="26"/>
       <c r="B99" s="26"/>
-      <c r="C99" s="26"/>
+      <c r="C99" s="9"/>
       <c r="H99" s="12"/>
-      <c r="I99" s="15"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="26"/>
       <c r="B100" s="26"/>
-      <c r="C100" s="9"/>
       <c r="H100" s="12"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="26"/>
       <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
       <c r="H101" s="12"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8757,15 +8734,10 @@
       <c r="C1065" s="26"/>
       <c r="H1065" s="12"/>
     </row>
-    <row r="1066" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1066" s="26"/>
-      <c r="B1066" s="26"/>
-      <c r="C1066" s="26"/>
-      <c r="H1066" s="12"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="E1:E1066"/>
-  <conditionalFormatting sqref="A98:B1066 A1:B42 A77:B91 A44:B75">
+  <autoFilter ref="E1:E1065"/>
+  <conditionalFormatting sqref="A97:B1065 A76:B90 A70:B74 A45:B68 A1:B43">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
@@ -8796,13 +8768,13 @@
     <hyperlink ref="E30" r:id="rId23" display="link"/>
     <hyperlink ref="E31" r:id="rId24" display="link"/>
     <hyperlink ref="E32" r:id="rId25" display="link"/>
-    <hyperlink ref="E33" r:id="rId26" display="6oz link"/>
-    <hyperlink ref="E34" r:id="rId27" display="link"/>
+    <hyperlink ref="E33" r:id="rId26" display="link"/>
+    <hyperlink ref="E34" r:id="rId27" display="6oz link"/>
     <hyperlink ref="E35" r:id="rId28" display="link"/>
-    <hyperlink ref="E37" r:id="rId29" display="link"/>
+    <hyperlink ref="E36" r:id="rId29" display="link"/>
     <hyperlink ref="E38" r:id="rId30" display="link"/>
     <hyperlink ref="E39" r:id="rId31" display="link"/>
-    <hyperlink ref="E44" r:id="rId32" display="link"/>
+    <hyperlink ref="E40" r:id="rId32" display="link"/>
     <hyperlink ref="E45" r:id="rId33" display="link"/>
     <hyperlink ref="E46" r:id="rId34" display="link"/>
     <hyperlink ref="E47" r:id="rId35" display="link"/>
@@ -8811,31 +8783,32 @@
     <hyperlink ref="E50" r:id="rId38" display="link"/>
     <hyperlink ref="E51" r:id="rId39" display="link"/>
     <hyperlink ref="E52" r:id="rId40" display="link"/>
-    <hyperlink ref="F52" r:id="rId41" display="link"/>
-    <hyperlink ref="E53" r:id="rId42" display="link"/>
+    <hyperlink ref="E53" r:id="rId41" display="link"/>
+    <hyperlink ref="F53" r:id="rId42" display="link"/>
     <hyperlink ref="E54" r:id="rId43" display="link"/>
     <hyperlink ref="E55" r:id="rId44" display="link"/>
-    <hyperlink ref="E59" r:id="rId45" display="link"/>
+    <hyperlink ref="E56" r:id="rId45" display="link"/>
     <hyperlink ref="E60" r:id="rId46" display="link"/>
-    <hyperlink ref="E64" r:id="rId47" display="link"/>
-    <hyperlink ref="H64" r:id="rId48" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E65" r:id="rId49" display="link"/>
+    <hyperlink ref="E61" r:id="rId47" display="link"/>
+    <hyperlink ref="E65" r:id="rId48" display="link"/>
+    <hyperlink ref="H65" r:id="rId49" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
     <hyperlink ref="E66" r:id="rId50" display="link"/>
     <hyperlink ref="E67" r:id="rId51" display="link"/>
-    <hyperlink ref="E70" r:id="rId52" display="link"/>
+    <hyperlink ref="E70" r:id="rId52" display="printed"/>
     <hyperlink ref="E71" r:id="rId53" display="printed"/>
     <hyperlink ref="E72" r:id="rId54" display="printed"/>
-    <hyperlink ref="E73" r:id="rId55" display="printed"/>
-    <hyperlink ref="E74" r:id="rId56" display="link"/>
-    <hyperlink ref="F74" r:id="rId57" display="6oz link"/>
-    <hyperlink ref="E75" r:id="rId58" display="link"/>
-    <hyperlink ref="E78" r:id="rId59" display="link"/>
+    <hyperlink ref="E73" r:id="rId55" display="link"/>
+    <hyperlink ref="F73" r:id="rId56" display="6oz link"/>
+    <hyperlink ref="E74" r:id="rId57" display="link"/>
+    <hyperlink ref="E77" r:id="rId58" display="link"/>
+    <hyperlink ref="E83" r:id="rId59" display="link"/>
     <hyperlink ref="E84" r:id="rId60" display="link"/>
     <hyperlink ref="E85" r:id="rId61" display="link"/>
-    <hyperlink ref="E86" r:id="rId62" display="link"/>
+    <hyperlink ref="E87" r:id="rId62" display="link"/>
     <hyperlink ref="E88" r:id="rId63" display="link"/>
-    <hyperlink ref="E89" r:id="rId64" display="link"/>
-    <hyperlink ref="E93" r:id="rId65" display="link"/>
+    <hyperlink ref="E89" r:id="rId64" display="link 3 corner"/>
+    <hyperlink ref="F89" r:id="rId65" display="link 2 corner"/>
+    <hyperlink ref="E92" r:id="rId66" display="link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8844,7 +8817,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId66"/>
+  <drawing r:id="rId67"/>
 </worksheet>
 </file>
 
@@ -8859,7 +8832,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>
@@ -8893,10 +8866,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8907,7 +8880,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>2</v>
@@ -8919,36 +8892,36 @@
         <v>14</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="I2" s="13" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I3" s="13" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8956,10 +8929,10 @@
         <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D4" s="10" t="n">
         <v>2</v>
@@ -8971,19 +8944,19 @@
         <v>13</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="I4" s="13" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="K4" s="13" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8994,7 +8967,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D5" s="10" t="n">
         <v>1</v>
@@ -9007,18 +8980,18 @@
         <v>7.36</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>1</v>
@@ -9029,18 +9002,18 @@
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
       <c r="J6" s="10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D7" s="10" t="n">
         <v>4</v>
@@ -9053,21 +9026,21 @@
         <v>9.99</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D8" s="10" t="n">
         <v>2</v>
@@ -9076,78 +9049,78 @@
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="I8" s="13" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I10" s="15" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>175</v>
+        <v>88</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>176</v>
+        <v>262</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D11" s="10" t="n">
         <v>1</v>
@@ -9156,67 +9129,67 @@
         <v>12</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="I11" s="13" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>179</v>
+        <v>265</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>180</v>
+        <v>266</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I12" s="13" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>185</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>187</v>
+        <v>92</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>188</v>
+        <v>93</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
@@ -9225,14 +9198,14 @@
         <v>12</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>190</v>
+        <v>95</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="13" t="n">
         <v>3.82</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9243,7 +9216,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>1</v>
@@ -9252,13 +9225,13 @@
         <v>12</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I15" s="13" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9269,7 +9242,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>1</v>
@@ -9282,7 +9255,7 @@
         <v>10.91</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9293,7 +9266,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>1</v>
@@ -9303,16 +9276,16 @@
       </c>
       <c r="F17" s="10"/>
       <c r="H17" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>278</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9323,7 +9296,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>1</v>
@@ -9332,13 +9305,13 @@
         <v>12</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I18" s="13" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9349,7 +9322,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>4</v>
@@ -9364,7 +9337,7 @@
         <v>64.08</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9375,7 +9348,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D20" s="10" t="n">
         <v>1</v>
@@ -9386,7 +9359,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="15"/>
       <c r="J20" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9397,7 +9370,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D21" s="10" t="n">
         <v>1</v>
@@ -9410,18 +9383,18 @@
         <v>26.79</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>286</v>
+        <v>132</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>285</v>
       </c>
       <c r="D22" s="10" t="n">
         <v>2</v>
@@ -9432,18 +9405,18 @@
       <c r="H22" s="12"/>
       <c r="I22" s="15"/>
       <c r="J22" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>288</v>
+        <v>135</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>287</v>
       </c>
       <c r="D23" s="10" t="n">
         <v>2</v>
@@ -9454,18 +9427,18 @@
       <c r="H23" s="12"/>
       <c r="I23" s="15"/>
       <c r="J23" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>289</v>
+        <v>138</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>288</v>
       </c>
       <c r="D24" s="10" t="n">
         <v>2</v>
@@ -9476,18 +9449,18 @@
       <c r="H24" s="12"/>
       <c r="I24" s="15"/>
       <c r="J24" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D25" s="10" t="n">
         <v>2</v>
@@ -9498,18 +9471,18 @@
       <c r="H25" s="12"/>
       <c r="I25" s="15"/>
       <c r="J25" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D26" s="10" t="n">
         <v>2</v>
@@ -9520,18 +9493,18 @@
       <c r="H26" s="12"/>
       <c r="I26" s="15"/>
       <c r="J26" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>292</v>
+        <v>147</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>291</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>2</v>
@@ -9542,40 +9515,40 @@
       <c r="H27" s="12"/>
       <c r="I27" s="15"/>
       <c r="J27" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="15"/>
       <c r="J28" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>2</v>
@@ -9587,43 +9560,43 @@
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="15" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="K29" s="10" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>212</v>
+        <v>295</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>296</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K30" s="10" t="s">
         <v>297</v>
@@ -9632,10 +9605,10 @@
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E31" s="28"/>
       <c r="H31" s="12"/>
@@ -9644,10 +9617,10 @@
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E32" s="28"/>
       <c r="H32" s="12"/>
@@ -9656,10 +9629,10 @@
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E33" s="28"/>
       <c r="H33" s="12"/>
@@ -9667,13 +9640,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>148</v>
+        <v>154</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="D34" s="10" t="n">
         <v>2</v>
@@ -9682,25 +9655,25 @@
         <v>12</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="13" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D35" s="10" t="n">
         <v>1</v>
@@ -9709,20 +9682,20 @@
         <v>12</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="15" t="n">
         <v>7.63</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K35" s="10" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9744,15 +9717,15 @@
       <c r="H36" s="12"/>
       <c r="I36" s="15"/>
       <c r="J36" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>298</v>
@@ -9764,7 +9737,7 @@
         <v>12</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>1.18</v>
@@ -9775,7 +9748,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
@@ -9789,13 +9762,13 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D39" s="10" t="n">
         <v>1</v>
@@ -9808,7 +9781,7 @@
         <v>9.35</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9829,7 +9802,7 @@
         <v>16.99</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9851,7 +9824,7 @@
         <v>8.99</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9876,7 +9849,7 @@
         <v>307</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9898,7 +9871,7 @@
         <v>307</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9923,7 +9896,7 @@
         <v>307</v>
       </c>
       <c r="K48" s="30" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
A few more BOM tweaks
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="313">
   <si>
     <t xml:space="preserve">pic label</t>
   </si>
@@ -335,7 +335,7 @@
     <t xml:space="preserve">2429K55</t>
   </si>
   <si>
-    <t xml:space="preserve">Purchase tubing compatible with your circulation pump and the copper heat exchanger!</t>
+    <t xml:space="preserve">Purchase tubing compatible with your circulation pump and the copper tubing!</t>
   </si>
   <si>
     <t xml:space="preserve">TC-JAR</t>
@@ -347,7 +347,10 @@
     <t xml:space="preserve">6oz link</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTE: We are investigating the simplest and most reliable configuration. A larger jar allows the pumps to be submerged, but submerging the pumps may lead them to over-heat at high temperatures.</t>
+    <t xml:space="preserve">16oz link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: We are investigating the simplest and most reliable configuration. 16Oz wide mouth jar may be optimal.</t>
   </si>
   <si>
     <t xml:space="preserve">TC-RLY</t>
@@ -1386,12 +1389,12 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="G25" activeCellId="1" sqref="H33 G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -2017,19 +2020,21 @@
       <c r="E34" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F34" s="11"/>
+      <c r="F34" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="H34" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="11" t="s">
@@ -2037,17 +2042,17 @@
       </c>
       <c r="F35" s="11"/>
       <c r="H35" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="11" t="s">
@@ -2055,33 +2060,33 @@
       </c>
       <c r="F36" s="11"/>
       <c r="H36" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9"/>
       <c r="B37" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="H37" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9"/>
       <c r="B38" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="11" t="s">
@@ -2089,17 +2094,17 @@
       </c>
       <c r="F38" s="11"/>
       <c r="H38" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9"/>
       <c r="B39" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="11" t="s">
@@ -2107,17 +2112,17 @@
       </c>
       <c r="F39" s="11"/>
       <c r="H39" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9"/>
       <c r="B40" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="11" t="s">
@@ -2125,23 +2130,23 @@
       </c>
       <c r="F40" s="11"/>
       <c r="H40" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I40" s="22"/>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9"/>
       <c r="B41" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="H41" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I41" s="22"/>
     </row>
@@ -2159,7 +2164,7 @@
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E43" s="24"/>
       <c r="H43" s="19"/>
@@ -2167,18 +2172,18 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D45" s="10" t="n">
         <v>4</v>
@@ -2191,13 +2196,13 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D46" s="10" t="n">
         <v>3</v>
@@ -2206,19 +2211,19 @@
         <v>12</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I46" s="15"/>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D47" s="10" t="n">
         <v>3</v>
@@ -2231,13 +2236,13 @@
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D48" s="10" t="n">
         <v>3</v>
@@ -2250,13 +2255,13 @@
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D49" s="10" t="n">
         <v>3</v>
@@ -2269,13 +2274,13 @@
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D50" s="10" t="n">
         <v>3</v>
@@ -2288,13 +2293,13 @@
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D51" s="10" t="n">
         <v>3</v>
@@ -2307,13 +2312,13 @@
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D52" s="10" t="n">
         <v>3</v>
@@ -2326,13 +2331,13 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D53" s="10" t="n">
         <v>3</v>
@@ -2344,20 +2349,20 @@
         <v>12</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H53" s="12"/>
       <c r="I53" s="22"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D54" s="10" t="n">
         <v>3</v>
@@ -2366,20 +2371,20 @@
         <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H54" s="12"/>
       <c r="I54" s="15"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D55" s="10" t="n">
         <v>3</v>
@@ -2388,19 +2393,19 @@
         <v>12</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I55" s="15"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E56" s="14" t="s">
         <v>12</v>
@@ -2420,7 +2425,7 @@
       <c r="A58" s="16"/>
       <c r="B58" s="16"/>
       <c r="C58" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E58" s="24"/>
       <c r="H58" s="19"/>
@@ -2430,7 +2435,7 @@
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E59" s="14"/>
       <c r="H59" s="12"/>
@@ -2439,10 +2444,10 @@
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9"/>
       <c r="B60" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>3</v>
@@ -2455,13 +2460,13 @@
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D61" s="10" t="n">
         <v>3</v>
@@ -2470,7 +2475,7 @@
         <v>12</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I61" s="15"/>
     </row>
@@ -2478,12 +2483,12 @@
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="11"/>
       <c r="H62" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I62" s="15"/>
     </row>
@@ -2500,7 +2505,7 @@
       <c r="A64" s="16"/>
       <c r="B64" s="16"/>
       <c r="C64" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E64" s="24"/>
       <c r="H64" s="19"/>
@@ -2508,13 +2513,13 @@
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D65" s="10" t="n">
         <v>1</v>
@@ -2523,19 +2528,19 @@
         <v>12</v>
       </c>
       <c r="H65" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I65" s="15"/>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D66" s="10" t="n">
         <v>1</v>
@@ -2544,112 +2549,112 @@
         <v>12</v>
       </c>
       <c r="H66" s="12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I66" s="22"/>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9"/>
       <c r="B67" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D67" s="10"/>
       <c r="E67" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H67" s="12" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I67" s="22"/>
     </row>
     <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="10"/>
       <c r="G68" s="10"/>
       <c r="H68" s="23" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I68" s="15"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="70" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D70" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H70" s="12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I70" s="15"/>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9"/>
       <c r="B71" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D71" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H71" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9"/>
       <c r="B72" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D72" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H72" s="12"/>
       <c r="I72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D73" s="10" t="n">
         <v>1</v>
@@ -2665,13 +2670,13 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D74" s="10" t="n">
         <v>1</v>
@@ -2687,7 +2692,7 @@
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E76" s="24"/>
       <c r="H76" s="19"/>
@@ -2695,29 +2700,29 @@
     </row>
     <row r="77" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H77" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I77" s="15"/>
     </row>
     <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9"/>
       <c r="B78" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E78" s="11"/>
       <c r="H78" s="12"/>
@@ -2726,10 +2731,10 @@
     <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9"/>
       <c r="B79" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E79" s="11"/>
       <c r="H79" s="12"/>
@@ -2738,10 +2743,10 @@
     <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9"/>
       <c r="B80" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E80" s="11"/>
       <c r="H80" s="12"/>
@@ -2749,11 +2754,11 @@
     </row>
     <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D81" s="10" t="n">
         <v>1</v>
@@ -2766,12 +2771,12 @@
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D82" s="10"/>
       <c r="E82" s="11"/>
       <c r="H82" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I82" s="15"/>
     </row>
@@ -2779,14 +2784,14 @@
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D83" s="10"/>
       <c r="E83" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I83" s="15"/>
     </row>
@@ -2794,14 +2799,14 @@
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I84" s="15"/>
     </row>
@@ -2809,14 +2814,14 @@
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D85" s="10"/>
       <c r="E85" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I85" s="15"/>
     </row>
@@ -2829,7 +2834,7 @@
       <c r="D86" s="10"/>
       <c r="E86" s="11"/>
       <c r="H86" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I86" s="15"/>
     </row>
@@ -2837,14 +2842,14 @@
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D87" s="10"/>
       <c r="E87" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I87" s="15"/>
     </row>
@@ -2852,13 +2857,13 @@
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E88" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H88" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I88" s="15"/>
     </row>
@@ -2866,16 +2871,16 @@
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I89" s="15"/>
     </row>
@@ -2883,25 +2888,25 @@
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E90" s="11"/>
       <c r="H90" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I90" s="15"/>
     </row>
     <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H91" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>2</v>
@@ -2910,7 +2915,7 @@
         <v>12</v>
       </c>
       <c r="H92" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -8770,45 +8775,46 @@
     <hyperlink ref="E32" r:id="rId25" display="link"/>
     <hyperlink ref="E33" r:id="rId26" display="link"/>
     <hyperlink ref="E34" r:id="rId27" display="6oz link"/>
-    <hyperlink ref="E35" r:id="rId28" display="link"/>
-    <hyperlink ref="E36" r:id="rId29" display="link"/>
-    <hyperlink ref="E38" r:id="rId30" display="link"/>
-    <hyperlink ref="E39" r:id="rId31" display="link"/>
-    <hyperlink ref="E40" r:id="rId32" display="link"/>
-    <hyperlink ref="E45" r:id="rId33" display="link"/>
-    <hyperlink ref="E46" r:id="rId34" display="link"/>
-    <hyperlink ref="E47" r:id="rId35" display="link"/>
-    <hyperlink ref="E48" r:id="rId36" display="link"/>
-    <hyperlink ref="E49" r:id="rId37" display="link"/>
-    <hyperlink ref="E50" r:id="rId38" display="link"/>
-    <hyperlink ref="E51" r:id="rId39" display="link"/>
-    <hyperlink ref="E52" r:id="rId40" display="link"/>
-    <hyperlink ref="E53" r:id="rId41" display="link"/>
-    <hyperlink ref="F53" r:id="rId42" display="link"/>
-    <hyperlink ref="E54" r:id="rId43" display="link"/>
-    <hyperlink ref="E55" r:id="rId44" display="link"/>
-    <hyperlink ref="E56" r:id="rId45" display="link"/>
-    <hyperlink ref="E60" r:id="rId46" display="link"/>
-    <hyperlink ref="E61" r:id="rId47" display="link"/>
-    <hyperlink ref="E65" r:id="rId48" display="link"/>
-    <hyperlink ref="H65" r:id="rId49" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E66" r:id="rId50" display="link"/>
-    <hyperlink ref="E67" r:id="rId51" display="link"/>
-    <hyperlink ref="E70" r:id="rId52" display="printed"/>
-    <hyperlink ref="E71" r:id="rId53" display="printed"/>
-    <hyperlink ref="E72" r:id="rId54" display="printed"/>
-    <hyperlink ref="E73" r:id="rId55" display="link"/>
-    <hyperlink ref="F73" r:id="rId56" display="6oz link"/>
-    <hyperlink ref="E74" r:id="rId57" display="link"/>
-    <hyperlink ref="E77" r:id="rId58" display="link"/>
-    <hyperlink ref="E83" r:id="rId59" display="link"/>
-    <hyperlink ref="E84" r:id="rId60" display="link"/>
-    <hyperlink ref="E85" r:id="rId61" display="link"/>
-    <hyperlink ref="E87" r:id="rId62" display="link"/>
-    <hyperlink ref="E88" r:id="rId63" display="link"/>
-    <hyperlink ref="E89" r:id="rId64" display="link 3 corner"/>
-    <hyperlink ref="F89" r:id="rId65" display="link 2 corner"/>
-    <hyperlink ref="E92" r:id="rId66" display="link"/>
+    <hyperlink ref="F34" r:id="rId28" display="16oz link"/>
+    <hyperlink ref="E35" r:id="rId29" display="link"/>
+    <hyperlink ref="E36" r:id="rId30" display="link"/>
+    <hyperlink ref="E38" r:id="rId31" display="link"/>
+    <hyperlink ref="E39" r:id="rId32" display="link"/>
+    <hyperlink ref="E40" r:id="rId33" display="link"/>
+    <hyperlink ref="E45" r:id="rId34" display="link"/>
+    <hyperlink ref="E46" r:id="rId35" display="link"/>
+    <hyperlink ref="E47" r:id="rId36" display="link"/>
+    <hyperlink ref="E48" r:id="rId37" display="link"/>
+    <hyperlink ref="E49" r:id="rId38" display="link"/>
+    <hyperlink ref="E50" r:id="rId39" display="link"/>
+    <hyperlink ref="E51" r:id="rId40" display="link"/>
+    <hyperlink ref="E52" r:id="rId41" display="link"/>
+    <hyperlink ref="E53" r:id="rId42" display="link"/>
+    <hyperlink ref="F53" r:id="rId43" display="link"/>
+    <hyperlink ref="E54" r:id="rId44" display="link"/>
+    <hyperlink ref="E55" r:id="rId45" display="link"/>
+    <hyperlink ref="E56" r:id="rId46" display="link"/>
+    <hyperlink ref="E60" r:id="rId47" display="link"/>
+    <hyperlink ref="E61" r:id="rId48" display="link"/>
+    <hyperlink ref="E65" r:id="rId49" display="link"/>
+    <hyperlink ref="H65" r:id="rId50" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
+    <hyperlink ref="E66" r:id="rId51" display="link"/>
+    <hyperlink ref="E67" r:id="rId52" display="link"/>
+    <hyperlink ref="E70" r:id="rId53" display="printed"/>
+    <hyperlink ref="E71" r:id="rId54" display="printed"/>
+    <hyperlink ref="E72" r:id="rId55" display="printed"/>
+    <hyperlink ref="E73" r:id="rId56" display="link"/>
+    <hyperlink ref="F73" r:id="rId57" display="6oz link"/>
+    <hyperlink ref="E74" r:id="rId58" display="link"/>
+    <hyperlink ref="E77" r:id="rId59" display="link"/>
+    <hyperlink ref="E83" r:id="rId60" display="link"/>
+    <hyperlink ref="E84" r:id="rId61" display="link"/>
+    <hyperlink ref="E85" r:id="rId62" display="link"/>
+    <hyperlink ref="E87" r:id="rId63" display="link"/>
+    <hyperlink ref="E88" r:id="rId64" display="link"/>
+    <hyperlink ref="E89" r:id="rId65" display="link 3 corner"/>
+    <hyperlink ref="F89" r:id="rId66" display="link 2 corner"/>
+    <hyperlink ref="E92" r:id="rId67" display="link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8817,7 +8823,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId67"/>
+  <drawing r:id="rId68"/>
 </worksheet>
 </file>
 
@@ -8829,10 +8835,10 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="H33 G25 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>
@@ -8866,10 +8872,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8880,7 +8886,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>2</v>
@@ -8892,36 +8898,36 @@
         <v>14</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I2" s="13" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I3" s="13" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8929,10 +8935,10 @@
         <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D4" s="10" t="n">
         <v>2</v>
@@ -8944,19 +8950,19 @@
         <v>13</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I4" s="13" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="K4" s="13" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8967,7 +8973,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D5" s="10" t="n">
         <v>1</v>
@@ -8980,18 +8986,18 @@
         <v>7.36</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>1</v>
@@ -9002,18 +9008,18 @@
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
       <c r="J6" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D7" s="10" t="n">
         <v>4</v>
@@ -9026,21 +9032,21 @@
         <v>9.99</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D8" s="10" t="n">
         <v>2</v>
@@ -9049,67 +9055,67 @@
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I8" s="13" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I10" s="15" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9117,10 +9123,10 @@
         <v>88</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D11" s="10" t="n">
         <v>1</v>
@@ -9129,55 +9135,55 @@
         <v>12</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I11" s="13" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="11" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I12" s="13" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I13" s="15"/>
     </row>
@@ -9189,7 +9195,7 @@
         <v>93</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
@@ -9205,7 +9211,7 @@
         <v>3.82</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9216,7 +9222,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>1</v>
@@ -9225,13 +9231,13 @@
         <v>12</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="I15" s="13" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9242,7 +9248,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>1</v>
@@ -9255,7 +9261,7 @@
         <v>10.91</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9266,7 +9272,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>1</v>
@@ -9276,16 +9282,16 @@
       </c>
       <c r="F17" s="10"/>
       <c r="H17" s="12" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9296,7 +9302,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>1</v>
@@ -9305,13 +9311,13 @@
         <v>12</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I18" s="13" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9322,7 +9328,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>4</v>
@@ -9337,7 +9343,7 @@
         <v>64.08</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9348,7 +9354,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D20" s="10" t="n">
         <v>1</v>
@@ -9359,7 +9365,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="15"/>
       <c r="J20" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9370,7 +9376,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D21" s="10" t="n">
         <v>1</v>
@@ -9383,18 +9389,18 @@
         <v>26.79</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D22" s="10" t="n">
         <v>2</v>
@@ -9405,18 +9411,18 @@
       <c r="H22" s="12"/>
       <c r="I22" s="15"/>
       <c r="J22" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D23" s="10" t="n">
         <v>2</v>
@@ -9427,18 +9433,18 @@
       <c r="H23" s="12"/>
       <c r="I23" s="15"/>
       <c r="J23" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D24" s="10" t="n">
         <v>2</v>
@@ -9449,18 +9455,18 @@
       <c r="H24" s="12"/>
       <c r="I24" s="15"/>
       <c r="J24" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D25" s="10" t="n">
         <v>2</v>
@@ -9471,18 +9477,18 @@
       <c r="H25" s="12"/>
       <c r="I25" s="15"/>
       <c r="J25" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D26" s="10" t="n">
         <v>2</v>
@@ -9493,18 +9499,18 @@
       <c r="H26" s="12"/>
       <c r="I26" s="15"/>
       <c r="J26" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>2</v>
@@ -9515,40 +9521,40 @@
       <c r="H27" s="12"/>
       <c r="I27" s="15"/>
       <c r="J27" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="15"/>
       <c r="J28" s="10" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>2</v>
@@ -9560,55 +9566,55 @@
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="15" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K29" s="10" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E31" s="28"/>
       <c r="H31" s="12"/>
@@ -9617,10 +9623,10 @@
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E32" s="28"/>
       <c r="H32" s="12"/>
@@ -9629,10 +9635,10 @@
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E33" s="28"/>
       <c r="H33" s="12"/>
@@ -9640,13 +9646,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D34" s="10" t="n">
         <v>2</v>
@@ -9655,25 +9661,25 @@
         <v>12</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="13" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D35" s="10" t="n">
         <v>1</v>
@@ -9689,13 +9695,13 @@
         <v>7.63</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K35" s="10" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9717,18 +9723,18 @@
       <c r="H36" s="12"/>
       <c r="I36" s="15"/>
       <c r="J36" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D37" s="10" t="n">
         <v>2</v>
@@ -9737,22 +9743,22 @@
         <v>12</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>1.18</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D38" s="10" t="n">
         <v>1</v>
@@ -9762,13 +9768,13 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D39" s="10" t="n">
         <v>1</v>
@@ -9781,37 +9787,37 @@
         <v>9.35</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="26"/>
       <c r="B40" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I40" s="13" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26"/>
       <c r="B41" s="9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D41" s="10" t="n">
         <v>1</v>
@@ -9824,7 +9830,7 @@
         <v>8.99</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9838,7 +9844,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9846,32 +9852,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="10" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I46" s="13" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9879,24 +9885,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="30" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K48" s="30" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated parts list and docs
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="313">
   <si>
     <t xml:space="preserve">pic label</t>
   </si>
@@ -260,7 +260,11 @@
     <t xml:space="preserve">Circulating pump</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTE Operational limits to pumps in terms of capacity and temperature have not been determined. Larger or self-priming pumps may be desired for optimal operation, especially at high temperatures.</t>
+    <t xml:space="preserve">1 or 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To run both heating and cooling in the same recipe without hardware reconfiguration between recipe steps, 2 pumps are required.
+NOTE: Operational limits to pumps in terms of capacity and temperature have not been determined. Larger pumps may be desired for optimal operation, especially at high temperatures. Self-priming pumps are HIGHLY recommended.</t>
   </si>
   <si>
     <t xml:space="preserve">TC-HOU</t>
@@ -299,16 +303,13 @@
     <t xml:space="preserve">Submersible heater</t>
   </si>
   <si>
-    <t xml:space="preserve">1 or 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC-CTB</t>
   </si>
   <si>
     <t xml:space="preserve">Copper tubing 1/4" OD x 3/16" ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Copper tubing should fit snugly within the silicone tubing</t>
+    <t xml:space="preserve">Copper tubing should fit snugly within the silicone tubing. This should be enough to make 2 heat exchanger coils.</t>
   </si>
   <si>
     <t xml:space="preserve">09</t>
@@ -317,25 +318,7 @@
     <t xml:space="preserve">TC-STB</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Silicone tubing 7mm OD x </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">5mm ID</t>
-    </r>
+    <t xml:space="preserve">Silicone tubing 7mm OD x 5mm ID</t>
   </si>
   <si>
     <t xml:space="preserve">Silicone tubing should fit snugly around the copper tubing</t>
@@ -359,7 +342,7 @@
     <t xml:space="preserve">TC-JAR</t>
   </si>
   <si>
-    <t xml:space="preserve">6oz canning jar or large Ball jar</t>
+    <t xml:space="preserve">16oz canning jar and/or large Ball jar</t>
   </si>
   <si>
     <t xml:space="preserve">6oz link</t>
@@ -777,7 +760,7 @@
     <t xml:space="preserve">Hard case</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional, but good for storage and shipping. The linked one was the cheapest profile we could find at ~$25 ea. The control unit and assembled reaction chamber module can fit side by side in one case while the reactor housing and pumps pack flatish next to the temperature control parts. A broader, less deep profile would be more convenient, but those seemed to be more expensive.</t>
+    <t xml:space="preserve">Optional, but good for storage and shipping. The linked one was the cheapest profile we could find at 2x ~$25 ea. The control unit and assembled reaction chamber module can fit side by side in one case while the reactor housing and pumps pack flat-ish next to the temperature control parts. A broader, less deep profile would be more convenient, but those seem to be more expensive. It’s snug – a separate cooling jar and coil will NOT fit.</t>
   </si>
   <si>
     <t xml:space="preserve">Price Aug/Sep 2022</t>
@@ -1014,7 +997,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="\$#,##0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1083,12 +1066,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1256,7 +1233,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1413,12 +1390,12 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="H93" activeCellId="0" sqref="H93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.90234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -1850,7 +1827,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
         <v>68</v>
       </c>
@@ -1860,25 +1837,25 @@
       <c r="C25" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="10" t="n">
-        <v>1</v>
+      <c r="D25" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F25" s="11"/>
       <c r="H25" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9"/>
       <c r="B26" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D26" s="10" t="n">
         <v>1</v>
@@ -1888,17 +1865,17 @@
       </c>
       <c r="F26" s="11"/>
       <c r="H26" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9"/>
       <c r="B27" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>1</v>
@@ -1914,7 +1891,7 @@
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
@@ -1924,17 +1901,17 @@
       </c>
       <c r="F28" s="11"/>
       <c r="H28" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9"/>
       <c r="B29" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>1</v>
@@ -1944,20 +1921,20 @@
       </c>
       <c r="F29" s="11"/>
       <c r="H29" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9"/>
       <c r="B30" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>12</v>
@@ -1966,7 +1943,7 @@
       <c r="H30" s="12"/>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
         <v>85</v>
@@ -8863,7 +8840,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.90234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>

</xml_diff>

<commit_message>
Add "on brand" paint colors to the parts list
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -754,7 +754,14 @@
     <t xml:space="preserve">Paint and stickers</t>
   </si>
   <si>
-    <t xml:space="preserve">Have fun with it! Make the Microlab yours!</t>
+    <t xml:space="preserve">Have fun with it! Make the Microlab yours! 
+OR MAKE IT OURS and use the colors from our “brand guidelines” (lmao):
+https://www.homedepot.com/p/MONTANA-11-oz-GOLD-Spray-Paint-Banana-Joe-034498/304354434
+https://www.homedepot.com/p/MONTANA-11-oz-GOLD-Spray-Paint-Pink-Pink-034546/304354610
+https://www.homedepot.com/p/MONTANA-11-oz-GOLD-Spray-Paint-Malachite-034600/304354558
+https://www.homedepot.com/p/MONTANA-11-oz-GOLD-Spray-Paint-Lavender-034556/304354620
+https://www.homedepot.com/p/MONTANA-11-oz-GOLD-Spray-Paint-Capri-034527/304354508
+https://www.homedepot.com/p/MONTANA-11-oz-GOLD-Spray-Paint-Blue-Magic-034574/304354574</t>
   </si>
   <si>
     <t xml:space="preserve">Hard case</t>
@@ -1392,10 +1399,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H93" activeCellId="0" sqref="H93"/>
+      <selection pane="bottomLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -2897,7 +2904,7 @@
       </c>
       <c r="I90" s="15"/>
     </row>
-    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="9" t="s">
         <v>234</v>
       </c>
@@ -8840,7 +8847,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>

</xml_diff>

<commit_message>
Add entry for breadboard jumpers
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1065</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$E$1066</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="321">
   <si>
     <t xml:space="preserve">pic label</t>
   </si>
@@ -221,22 +221,46 @@
     <t xml:space="preserve">These can be scavenged from old computers</t>
   </si>
   <si>
+    <t xml:space="preserve">MC-JMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breadboard Jumpers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small wires to connect exposed pins on the Pi and Arduino to lever and screw terminals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC-ECD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Extension cord</t>
   </si>
   <si>
     <t xml:space="preserve">This provides power for the 5v and 12v circuits in the LAB CONTROL UNIT. The heaters that run on mains power are powered separately.</t>
   </si>
   <si>
+    <t xml:space="preserve">MC-VCR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Velcro / hook-and-loop straps</t>
   </si>
   <si>
     <t xml:space="preserve">Optional, but useful for assembly and affixing components to the case</t>
   </si>
   <si>
+    <t xml:space="preserve">MC-SMC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stepper Motor Cables</t>
   </si>
   <si>
     <t xml:space="preserve">Most stepper motors will come with these</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC-HOU</t>
   </si>
   <si>
     <t xml:space="preserve">Corrugated plastic </t>
@@ -1394,15 +1418,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:I1066"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
+      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -1730,28 +1754,32 @@
       </c>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
+      <c r="B17" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="C17" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="10" t="n">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C18" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>1</v>
@@ -1760,129 +1788,132 @@
         <v>12</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I18" s="15"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
+      <c r="B19" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="C19" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H19" s="12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="I19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
+      <c r="B20" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="C20" s="9" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="11"/>
       <c r="H20" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I20" s="15"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="D21" s="10"/>
       <c r="E21" s="11"/>
-      <c r="H21" s="12"/>
+      <c r="H21" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="I21" s="15"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="14"/>
+      <c r="E22" s="11"/>
       <c r="H22" s="12"/>
       <c r="I22" s="15"/>
     </row>
-    <row r="23" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="20"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="13"/>
-    </row>
-    <row r="25" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>12</v>
-      </c>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="14"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="20"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="11"/>
-      <c r="H25" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I25" s="22"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="B26" s="9" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="10" t="n">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="11"/>
       <c r="H26" s="12" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9"/>
       <c r="B27" s="9" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>1</v>
@@ -1891,14 +1922,18 @@
         <v>12</v>
       </c>
       <c r="F27" s="11"/>
-      <c r="H27" s="12"/>
+      <c r="H27" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="I27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
+      <c r="B28" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="C28" s="9" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
@@ -1907,18 +1942,14 @@
         <v>12</v>
       </c>
       <c r="F28" s="11"/>
-      <c r="H28" s="12" t="s">
-        <v>79</v>
-      </c>
+      <c r="H28" s="12"/>
       <c r="I28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9"/>
-      <c r="B29" s="9" t="s">
-        <v>80</v>
-      </c>
+      <c r="B29" s="9"/>
       <c r="C29" s="9" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>1</v>
@@ -1928,57 +1959,55 @@
       </c>
       <c r="F29" s="11"/>
       <c r="H29" s="12" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9"/>
       <c r="B30" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>71</v>
+        <v>89</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>1</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="11"/>
-      <c r="H30" s="12"/>
+      <c r="H30" s="12" t="s">
+        <v>90</v>
+      </c>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="10" t="n">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F31" s="11"/>
-      <c r="H31" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="H31" s="12"/>
       <c r="I31" s="22"/>
     </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
-        <v>88</v>
-      </c>
+    <row r="32" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D32" s="10" t="n">
         <v>1</v>
@@ -1988,79 +2017,83 @@
       </c>
       <c r="F32" s="11"/>
       <c r="H32" s="12" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="I32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D33" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="10" t="s">
-        <v>95</v>
-      </c>
+      <c r="F33" s="11"/>
       <c r="H33" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="I33" s="15"/>
-    </row>
-    <row r="34" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="I33" s="22"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="B34" s="9" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" s="10"/>
+        <v>102</v>
+      </c>
+      <c r="D34" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="E34" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>100</v>
+        <v>12</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>103</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="I34" s="22"/>
-    </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>104</v>
+      </c>
+      <c r="I34" s="15"/>
+    </row>
+    <row r="35" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="11"/>
+        <v>107</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="H35" s="12" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="I35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="11" t="s">
@@ -2068,51 +2101,51 @@
       </c>
       <c r="F36" s="11"/>
       <c r="H36" s="12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9"/>
       <c r="B37" s="9" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
+      <c r="E37" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F37" s="11"/>
       <c r="H37" s="12" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="I37" s="22"/>
     </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9"/>
       <c r="B38" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D38" s="10"/>
-      <c r="E38" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="H38" s="12" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9"/>
       <c r="B39" s="9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="11" t="s">
@@ -2120,17 +2153,17 @@
       </c>
       <c r="F39" s="11"/>
       <c r="H39" s="12" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="I39" s="22"/>
     </row>
-    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9"/>
       <c r="B40" s="9" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="11" t="s">
@@ -2138,100 +2171,97 @@
       </c>
       <c r="F40" s="11"/>
       <c r="H40" s="12" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="I40" s="22"/>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9"/>
       <c r="B41" s="9" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
+      <c r="E41" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F41" s="11"/>
       <c r="H41" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="I41" s="22"/>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
+      <c r="B42" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="D42" s="10"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
-      <c r="H42" s="12"/>
+      <c r="H42" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="I42" s="22"/>
     </row>
-    <row r="43" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E43" s="23"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="20"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D45" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" s="12"/>
-      <c r="I45" s="15"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="22"/>
+    </row>
+    <row r="44" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E44" s="23"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="20"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="8" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D46" s="10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="12" t="s">
-        <v>131</v>
-      </c>
+      <c r="H46" s="12"/>
       <c r="I46" s="15"/>
     </row>
-    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>134</v>
+        <v>137</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="D47" s="10" t="n">
         <v>3</v>
@@ -2239,18 +2269,20 @@
       <c r="E47" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="12"/>
+      <c r="H47" s="12" t="s">
+        <v>139</v>
+      </c>
       <c r="I47" s="15"/>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D48" s="10" t="n">
         <v>3</v>
@@ -2263,13 +2295,13 @@
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D49" s="10" t="n">
         <v>3</v>
@@ -2282,13 +2314,13 @@
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>143</v>
+        <v>147</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>148</v>
       </c>
       <c r="D50" s="10" t="n">
         <v>3</v>
@@ -2301,13 +2333,13 @@
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D51" s="10" t="n">
         <v>3</v>
@@ -2320,13 +2352,13 @@
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>149</v>
+        <v>153</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="D52" s="10" t="n">
         <v>3</v>
@@ -2337,15 +2369,15 @@
       <c r="H52" s="12"/>
       <c r="I52" s="15"/>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>152</v>
+        <v>156</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>157</v>
       </c>
       <c r="D53" s="10" t="n">
         <v>3</v>
@@ -2353,24 +2385,18 @@
       <c r="E53" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>153</v>
-      </c>
       <c r="H53" s="12"/>
-      <c r="I53" s="22"/>
+      <c r="I53" s="15"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="D54" s="10" t="n">
         <v>3</v>
@@ -2378,21 +2404,24 @@
       <c r="E54" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="F54" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="G54" s="10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H54" s="12"/>
-      <c r="I54" s="15"/>
+      <c r="I54" s="22"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>160</v>
+        <v>163</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>164</v>
       </c>
       <c r="D55" s="10" t="n">
         <v>3</v>
@@ -2400,155 +2429,156 @@
       <c r="E55" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H55" s="12" t="s">
-        <v>161</v>
-      </c>
+      <c r="G55" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H55" s="12"/>
       <c r="I55" s="15"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E56" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D56" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I56" s="13"/>
-    </row>
-    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="11"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="15"/>
-    </row>
-    <row r="58" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E58" s="23"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="20"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E59" s="14"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="13"/>
-    </row>
-    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H56" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="11"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E59" s="23"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="20"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9"/>
-      <c r="B60" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D60" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>12</v>
-      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="14"/>
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9" t="s">
-        <v>158</v>
-      </c>
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9"/>
       <c r="B61" s="9" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D61" s="10" t="n">
+        <v>176</v>
+      </c>
+      <c r="D61" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E61" s="11" t="s">
+      <c r="E61" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="I61" s="15"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="13"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9"/>
+      <c r="A62" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>167</v>
+      </c>
       <c r="C62" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D62" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="12" t="s">
         <v>169</v>
-      </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11"/>
-      <c r="H62" s="12" t="s">
-        <v>170</v>
       </c>
       <c r="I62" s="15"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
+      <c r="C63" s="9" t="s">
+        <v>177</v>
+      </c>
       <c r="D63" s="10"/>
       <c r="E63" s="11"/>
-      <c r="H63" s="12"/>
+      <c r="H63" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I63" s="15"/>
     </row>
-    <row r="64" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="16"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E64" s="23"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="20"/>
-    </row>
-    <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D65" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H65" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="I65" s="15"/>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="11"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="15"/>
+    </row>
+    <row r="65" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E65" s="23"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="20"/>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D66" s="10" t="n">
         <v>1</v>
@@ -2557,134 +2587,133 @@
         <v>12</v>
       </c>
       <c r="H66" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="I66" s="22"/>
+        <v>183</v>
+      </c>
+      <c r="I66" s="15"/>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9"/>
+      <c r="A67" s="9" t="s">
+        <v>184</v>
+      </c>
       <c r="B67" s="9" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D67" s="10"/>
+        <v>186</v>
+      </c>
+      <c r="D67" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E67" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H67" s="12" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="I67" s="22"/>
     </row>
-    <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="9" t="s">
-        <v>183</v>
-      </c>
+    <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="9"/>
       <c r="B68" s="9" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="G68" s="10"/>
-      <c r="H68" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="I68" s="15"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="D70" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E70" s="11" t="s">
+      <c r="E68" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="H70" s="12" t="s">
+      <c r="I68" s="22"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="I70" s="15"/>
-    </row>
-    <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="9"/>
+      <c r="B69" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="I69" s="15"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="B71" s="9" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D71" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="H71" s="12" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="I71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9"/>
       <c r="B72" s="9" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D72" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="H72" s="12"/>
+        <v>198</v>
+      </c>
+      <c r="H72" s="12" t="s">
+        <v>202</v>
+      </c>
       <c r="I72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9" t="s">
-        <v>197</v>
-      </c>
+      <c r="A73" s="9"/>
       <c r="B73" s="9" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D73" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F73" s="11" t="s">
-        <v>99</v>
+        <v>198</v>
       </c>
       <c r="H73" s="12"/>
-      <c r="I73" s="22"/>
-    </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I73" s="15"/>
+    </row>
+    <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D74" s="10" t="n">
         <v>1</v>
@@ -2692,57 +2721,67 @@
       <c r="E74" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="F74" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="H74" s="12"/>
-      <c r="I74" s="15"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="16"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E76" s="23"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="20"/>
-    </row>
-    <row r="77" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E77" s="11" t="s">
+      <c r="I74" s="22"/>
+    </row>
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D75" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H77" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="I77" s="15"/>
-    </row>
-    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="15"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="16"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E77" s="23"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="20"/>
+    </row>
+    <row r="78" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="9" t="s">
+        <v>212</v>
+      </c>
       <c r="B78" s="9" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="E78" s="11"/>
-      <c r="H78" s="12"/>
+        <v>214</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78" s="12" t="s">
+        <v>215</v>
+      </c>
       <c r="I78" s="15"/>
     </row>
     <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9"/>
       <c r="B79" s="9" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E79" s="11"/>
       <c r="H79" s="12"/>
@@ -2751,55 +2790,52 @@
     <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9"/>
       <c r="B80" s="9" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="E80" s="11"/>
       <c r="H80" s="12"/>
       <c r="I80" s="15"/>
     </row>
     <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="B81" s="9"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="9" t="s">
+        <v>220</v>
+      </c>
       <c r="C81" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D81" s="10" t="n">
-        <v>1</v>
+        <v>221</v>
       </c>
       <c r="E81" s="11"/>
       <c r="H81" s="12"/>
       <c r="I81" s="15"/>
     </row>
     <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="9"/>
+      <c r="A82" s="9" t="s">
+        <v>222</v>
+      </c>
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D82" s="10"/>
+        <v>223</v>
+      </c>
+      <c r="D82" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E82" s="11"/>
-      <c r="H82" s="12" t="s">
-        <v>217</v>
-      </c>
+      <c r="H82" s="12"/>
       <c r="I82" s="15"/>
     </row>
-    <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D83" s="10"/>
-      <c r="E83" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E83" s="11"/>
       <c r="H83" s="12" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="I83" s="15"/>
     </row>
@@ -2807,14 +2843,14 @@
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="I84" s="15"/>
     </row>
@@ -2822,42 +2858,42 @@
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="D85" s="10"/>
       <c r="E85" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="I85" s="15"/>
     </row>
-    <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9" t="s">
-        <v>60</v>
+        <v>229</v>
       </c>
       <c r="D86" s="10"/>
-      <c r="E86" s="11"/>
+      <c r="E86" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="H86" s="12" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="I86" s="15"/>
     </row>
-    <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9" t="s">
-        <v>224</v>
+        <v>66</v>
       </c>
       <c r="D87" s="10"/>
-      <c r="E87" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E87" s="11"/>
       <c r="H87" s="12" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="I87" s="15"/>
     </row>
@@ -2865,102 +2901,111 @@
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9" t="s">
-        <v>226</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="D88" s="10"/>
       <c r="E88" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H88" s="12" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="I88" s="15"/>
     </row>
-    <row r="89" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F89" s="11" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="I89" s="15"/>
     </row>
-    <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="E90" s="11"/>
+        <v>236</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="F90" s="11" t="s">
+        <v>238</v>
+      </c>
       <c r="H90" s="12" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="I90" s="15"/>
     </row>
-    <row r="91" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
       <c r="C91" s="9" t="s">
-        <v>234</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="E91" s="11"/>
       <c r="H91" s="12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>241</v>
+      </c>
+      <c r="I91" s="15"/>
+    </row>
+    <row r="92" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D92" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="H92" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D93" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="E93" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H92" s="12" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H93" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="9"/>
-      <c r="B97" s="9"/>
-      <c r="C97" s="9"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="11"/>
-      <c r="H97" s="12"/>
-      <c r="I97" s="15"/>
-    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="26"/>
-      <c r="B98" s="26"/>
-      <c r="C98" s="26"/>
+      <c r="A98" s="9"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="11"/>
       <c r="H98" s="12"/>
       <c r="I98" s="15"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="26"/>
       <c r="B99" s="26"/>
-      <c r="C99" s="9"/>
+      <c r="C99" s="26"/>
       <c r="H99" s="12"/>
+      <c r="I99" s="15"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="26"/>
       <c r="B100" s="26"/>
+      <c r="C100" s="9"/>
       <c r="H100" s="12"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="26"/>
       <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
       <c r="H101" s="12"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8747,10 +8792,15 @@
       <c r="C1065" s="26"/>
       <c r="H1065" s="12"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1066" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1066" s="26"/>
+      <c r="B1066" s="26"/>
+      <c r="C1066" s="26"/>
+      <c r="H1066" s="12"/>
+    </row>
   </sheetData>
-  <autoFilter ref="E1:E1065"/>
-  <conditionalFormatting sqref="A97:B1065 A76:B90 A70:B74 A45:B68 A1:B43">
+  <autoFilter ref="E1:E1066"/>
+  <conditionalFormatting sqref="A98:B1066 A77:B91 A71:B75 A46:B69 A1:B44">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
@@ -8774,7 +8824,7 @@
     <hyperlink ref="E15" r:id="rId16" display="link"/>
     <hyperlink ref="E17" r:id="rId17" display="link"/>
     <hyperlink ref="E18" r:id="rId18" display="link"/>
-    <hyperlink ref="E25" r:id="rId19" display="link"/>
+    <hyperlink ref="E19" r:id="rId19" display="link"/>
     <hyperlink ref="E26" r:id="rId20" display="link"/>
     <hyperlink ref="E27" r:id="rId21" display="link"/>
     <hyperlink ref="E28" r:id="rId22" display="link"/>
@@ -8783,14 +8833,14 @@
     <hyperlink ref="E31" r:id="rId25" display="link"/>
     <hyperlink ref="E32" r:id="rId26" display="link"/>
     <hyperlink ref="E33" r:id="rId27" display="link"/>
-    <hyperlink ref="E34" r:id="rId28" display="6oz link"/>
-    <hyperlink ref="F34" r:id="rId29" display="16oz link"/>
-    <hyperlink ref="E35" r:id="rId30" display="link"/>
+    <hyperlink ref="E34" r:id="rId28" display="link"/>
+    <hyperlink ref="E35" r:id="rId29" display="6oz link"/>
+    <hyperlink ref="F35" r:id="rId30" display="16oz link"/>
     <hyperlink ref="E36" r:id="rId31" display="link"/>
-    <hyperlink ref="E38" r:id="rId32" display="link"/>
+    <hyperlink ref="E37" r:id="rId32" display="link"/>
     <hyperlink ref="E39" r:id="rId33" display="link"/>
     <hyperlink ref="E40" r:id="rId34" display="link"/>
-    <hyperlink ref="E45" r:id="rId35" display="link"/>
+    <hyperlink ref="E41" r:id="rId35" display="link"/>
     <hyperlink ref="E46" r:id="rId36" display="link"/>
     <hyperlink ref="E47" r:id="rId37" display="link"/>
     <hyperlink ref="E48" r:id="rId38" display="link"/>
@@ -8799,31 +8849,32 @@
     <hyperlink ref="E51" r:id="rId41" display="link"/>
     <hyperlink ref="E52" r:id="rId42" display="link"/>
     <hyperlink ref="E53" r:id="rId43" display="link"/>
-    <hyperlink ref="F53" r:id="rId44" display="link"/>
-    <hyperlink ref="E54" r:id="rId45" display="link"/>
+    <hyperlink ref="E54" r:id="rId44" display="link"/>
+    <hyperlink ref="F54" r:id="rId45" display="link"/>
     <hyperlink ref="E55" r:id="rId46" display="link"/>
     <hyperlink ref="E56" r:id="rId47" display="link"/>
-    <hyperlink ref="E60" r:id="rId48" display="link"/>
+    <hyperlink ref="E57" r:id="rId48" display="link"/>
     <hyperlink ref="E61" r:id="rId49" display="link"/>
-    <hyperlink ref="E65" r:id="rId50" display="link"/>
-    <hyperlink ref="H65" r:id="rId51" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E66" r:id="rId52" display="link"/>
+    <hyperlink ref="E62" r:id="rId50" display="link"/>
+    <hyperlink ref="E66" r:id="rId51" display="link"/>
+    <hyperlink ref="H66" r:id="rId52" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
     <hyperlink ref="E67" r:id="rId53" display="link"/>
-    <hyperlink ref="E70" r:id="rId54" display="printed"/>
+    <hyperlink ref="E68" r:id="rId54" display="link"/>
     <hyperlink ref="E71" r:id="rId55" display="printed"/>
     <hyperlink ref="E72" r:id="rId56" display="printed"/>
-    <hyperlink ref="E73" r:id="rId57" display="link"/>
-    <hyperlink ref="F73" r:id="rId58" display="6oz link"/>
-    <hyperlink ref="E74" r:id="rId59" display="link"/>
-    <hyperlink ref="E77" r:id="rId60" display="link"/>
-    <hyperlink ref="E83" r:id="rId61" display="link"/>
+    <hyperlink ref="E73" r:id="rId57" display="printed"/>
+    <hyperlink ref="E74" r:id="rId58" display="link"/>
+    <hyperlink ref="F74" r:id="rId59" display="6oz link"/>
+    <hyperlink ref="E75" r:id="rId60" display="link"/>
+    <hyperlink ref="E78" r:id="rId61" display="link"/>
     <hyperlink ref="E84" r:id="rId62" display="link"/>
     <hyperlink ref="E85" r:id="rId63" display="link"/>
-    <hyperlink ref="E87" r:id="rId64" display="link"/>
+    <hyperlink ref="E86" r:id="rId64" display="link"/>
     <hyperlink ref="E88" r:id="rId65" display="link"/>
-    <hyperlink ref="E89" r:id="rId66" display="link 3 corner"/>
-    <hyperlink ref="F89" r:id="rId67" display="link 2 corner"/>
-    <hyperlink ref="E92" r:id="rId68" display="link"/>
+    <hyperlink ref="E89" r:id="rId66" display="link"/>
+    <hyperlink ref="E90" r:id="rId67" display="link 3 corner"/>
+    <hyperlink ref="F90" r:id="rId68" display="link 2 corner"/>
+    <hyperlink ref="E93" r:id="rId69" display="link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8832,7 +8883,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId69"/>
+  <drawing r:id="rId70"/>
 </worksheet>
 </file>
 
@@ -8847,7 +8898,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>
@@ -8881,10 +8932,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8895,7 +8946,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>2</v>
@@ -8907,47 +8958,47 @@
         <v>14</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="I2" s="13" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="I3" s="13" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="D4" s="10" t="n">
         <v>2</v>
@@ -8959,19 +9010,19 @@
         <v>13</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="I4" s="13" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="K4" s="13" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8982,7 +9033,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="D5" s="10" t="n">
         <v>1</v>
@@ -8995,18 +9046,18 @@
         <v>7.36</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>1</v>
@@ -9017,18 +9068,18 @@
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
       <c r="J6" s="10" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D7" s="10" t="n">
         <v>4</v>
@@ -9041,21 +9092,21 @@
         <v>9.99</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D8" s="10" t="n">
         <v>2</v>
@@ -9064,78 +9115,78 @@
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="I8" s="13" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="I10" s="15" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D11" s="10" t="n">
         <v>1</v>
@@ -9144,67 +9195,67 @@
         <v>12</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="I11" s="13" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="11" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="12" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="I12" s="13" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="12" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="I13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
@@ -9213,14 +9264,14 @@
         <v>12</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="13" t="n">
         <v>3.82</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9231,7 +9282,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>1</v>
@@ -9240,13 +9291,13 @@
         <v>12</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="I15" s="13" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9257,7 +9308,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>1</v>
@@ -9270,7 +9321,7 @@
         <v>10.91</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9281,7 +9332,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>1</v>
@@ -9291,16 +9342,16 @@
       </c>
       <c r="F17" s="10"/>
       <c r="H17" s="12" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9311,7 +9362,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>1</v>
@@ -9320,13 +9371,13 @@
         <v>12</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="I18" s="13" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9337,7 +9388,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>4</v>
@@ -9352,7 +9403,7 @@
         <v>64.08</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9363,7 +9414,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D20" s="10" t="n">
         <v>1</v>
@@ -9374,7 +9425,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="15"/>
       <c r="J20" s="10" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9385,7 +9436,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="D21" s="10" t="n">
         <v>1</v>
@@ -9398,18 +9449,18 @@
         <v>26.79</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="D22" s="10" t="n">
         <v>2</v>
@@ -9420,18 +9471,18 @@
       <c r="H22" s="12"/>
       <c r="I22" s="15"/>
       <c r="J22" s="10" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="D23" s="10" t="n">
         <v>2</v>
@@ -9442,18 +9493,18 @@
       <c r="H23" s="12"/>
       <c r="I23" s="15"/>
       <c r="J23" s="10" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="D24" s="10" t="n">
         <v>2</v>
@@ -9464,18 +9515,18 @@
       <c r="H24" s="12"/>
       <c r="I24" s="15"/>
       <c r="J24" s="10" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="D25" s="10" t="n">
         <v>2</v>
@@ -9486,18 +9537,18 @@
       <c r="H25" s="12"/>
       <c r="I25" s="15"/>
       <c r="J25" s="10" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="D26" s="10" t="n">
         <v>2</v>
@@ -9508,18 +9559,18 @@
       <c r="H26" s="12"/>
       <c r="I26" s="15"/>
       <c r="J26" s="10" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>2</v>
@@ -9530,40 +9581,40 @@
       <c r="H27" s="12"/>
       <c r="I27" s="15"/>
       <c r="J27" s="10" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="15"/>
       <c r="J28" s="10" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>2</v>
@@ -9575,55 +9626,55 @@
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="15" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="K29" s="10" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E31" s="28"/>
       <c r="H31" s="12"/>
@@ -9632,10 +9683,10 @@
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="E32" s="28"/>
       <c r="H32" s="12"/>
@@ -9644,10 +9695,10 @@
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="E33" s="28"/>
       <c r="H33" s="12"/>
@@ -9655,13 +9706,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D34" s="10" t="n">
         <v>2</v>
@@ -9670,25 +9721,25 @@
         <v>12</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="13" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="D35" s="10" t="n">
         <v>1</v>
@@ -9697,20 +9748,20 @@
         <v>12</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="15" t="n">
         <v>7.63</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="K35" s="10" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9732,18 +9783,18 @@
       <c r="H36" s="12"/>
       <c r="I36" s="15"/>
       <c r="J36" s="10" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="D37" s="10" t="n">
         <v>2</v>
@@ -9752,22 +9803,22 @@
         <v>12</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>1.18</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="D38" s="10" t="n">
         <v>1</v>
@@ -9777,13 +9828,13 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D39" s="10" t="n">
         <v>1</v>
@@ -9796,37 +9847,37 @@
         <v>9.35</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="26"/>
       <c r="B40" s="9" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="I40" s="13" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26"/>
       <c r="B41" s="9" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="D41" s="10" t="n">
         <v>1</v>
@@ -9839,7 +9890,7 @@
         <v>8.99</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9853,7 +9904,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9861,32 +9912,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="10" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="10" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="I46" s="13" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9894,24 +9945,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="K47" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="K47" s="10" t="s">
-        <v>300</v>
-      </c>
       <c r="L47" s="10" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="30" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="K48" s="30" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Parts list parts updates
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="350">
   <si>
     <t xml:space="preserve">pic label</t>
   </si>
@@ -864,6 +864,12 @@
   </si>
   <si>
     <t xml:space="preserve">Optional, but good for storage and shipping. The linked one was the cheapest profile we could find at 2x ~$25 ea. The control unit and assembled reaction chamber module can fit side by side in one case while the reactor housing and pumps pack flat-ish next to the temperature control parts. A broader, less deep profile would be more convenient, but those seem to be more expensive. It’s snug – a separate cooling jar and coil will NOT fit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra peristaltic tubing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tubing is likely to need to be replaced and to feed from larger containers than syringes, longer pieces may be desired.</t>
   </si>
   <si>
     <t xml:space="preserve">Price Aug/Sep 2022</t>
@@ -1610,13 +1616,13 @@
   </sheetPr>
   <dimension ref="A1:I1068"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E91" activeCellId="0" sqref="E91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F94" activeCellId="0" sqref="F94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
@@ -3230,7 +3236,17 @@
         <v>269</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C96" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H96" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -9133,6 +9149,7 @@
     <hyperlink ref="E92" r:id="rId72" display="Printed 3 corner"/>
     <hyperlink ref="F92" r:id="rId73" display="Printed 2 corner"/>
     <hyperlink ref="E95" r:id="rId74" display="Amazon link"/>
+    <hyperlink ref="E96" r:id="rId75" display="Amazon link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -9141,7 +9158,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId75"/>
+  <drawing r:id="rId76"/>
 </worksheet>
 </file>
 
@@ -9156,7 +9173,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>
@@ -9190,10 +9207,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9204,7 +9221,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>2</v>
@@ -9216,13 +9233,13 @@
         <v>17</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="I2" s="13" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9239,13 +9256,13 @@
         <v>150</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="I3" s="13" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9253,10 +9270,10 @@
         <v>92</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D4" s="10" t="n">
         <v>2</v>
@@ -9265,22 +9282,22 @@
         <v>150</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="I4" s="13" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="K4" s="13" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9291,7 +9308,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D5" s="10" t="n">
         <v>1</v>
@@ -9304,18 +9321,18 @@
         <v>7.36</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>1</v>
@@ -9326,7 +9343,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
       <c r="J6" s="10" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9337,7 +9354,7 @@
         <v>148</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D7" s="10" t="n">
         <v>4</v>
@@ -9350,10 +9367,10 @@
         <v>9.99</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9379,7 +9396,7 @@
         <v>8.99</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9390,13 +9407,13 @@
         <v>199</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="15"/>
@@ -9409,31 +9426,31 @@
         <v>203</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="I10" s="15" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9441,10 +9458,10 @@
         <v>112</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D11" s="10" t="n">
         <v>1</v>
@@ -9453,38 +9470,38 @@
         <v>150</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="I11" s="13" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="19" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="12" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="I12" s="13" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9501,7 +9518,7 @@
       <c r="E13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="12" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I13" s="15"/>
     </row>
@@ -9513,7 +9530,7 @@
         <v>117</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
@@ -9529,7 +9546,7 @@
         <v>3.82</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9540,7 +9557,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>1</v>
@@ -9549,13 +9566,13 @@
         <v>150</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="I15" s="13" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9566,7 +9583,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>1</v>
@@ -9579,7 +9596,7 @@
         <v>10.91</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9590,7 +9607,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>1</v>
@@ -9600,16 +9617,16 @@
       </c>
       <c r="F17" s="10"/>
       <c r="H17" s="12" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9620,7 +9637,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>1</v>
@@ -9629,13 +9646,13 @@
         <v>150</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="I18" s="13" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9646,7 +9663,7 @@
         <v>45</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>4</v>
@@ -9655,13 +9672,13 @@
         <v>150</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="I19" s="13" t="n">
         <v>64.08</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9672,7 +9689,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D20" s="10" t="n">
         <v>1</v>
@@ -9683,7 +9700,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="15"/>
       <c r="J20" s="10" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9694,7 +9711,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D21" s="10" t="n">
         <v>1</v>
@@ -9707,7 +9724,7 @@
         <v>26.79</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9718,7 +9735,7 @@
         <v>156</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D22" s="10" t="n">
         <v>2</v>
@@ -9729,7 +9746,7 @@
       <c r="H22" s="12"/>
       <c r="I22" s="15"/>
       <c r="J22" s="10" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9740,7 +9757,7 @@
         <v>159</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D23" s="10" t="n">
         <v>2</v>
@@ -9751,7 +9768,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="15"/>
       <c r="J23" s="10" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9762,7 +9779,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D24" s="10" t="n">
         <v>2</v>
@@ -9773,7 +9790,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="15"/>
       <c r="J24" s="10" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9784,7 +9801,7 @@
         <v>165</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D25" s="10" t="n">
         <v>2</v>
@@ -9795,7 +9812,7 @@
       <c r="H25" s="12"/>
       <c r="I25" s="15"/>
       <c r="J25" s="10" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9806,7 +9823,7 @@
         <v>168</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D26" s="10" t="n">
         <v>2</v>
@@ -9817,7 +9834,7 @@
       <c r="H26" s="12"/>
       <c r="I26" s="15"/>
       <c r="J26" s="10" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9828,7 +9845,7 @@
         <v>171</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>2</v>
@@ -9839,7 +9856,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="15"/>
       <c r="J27" s="10" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9850,7 +9867,7 @@
         <v>214</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D28" s="10" t="n">
         <v>1</v>
@@ -9861,7 +9878,7 @@
       <c r="H28" s="12"/>
       <c r="I28" s="15"/>
       <c r="J28" s="10" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9872,7 +9889,7 @@
         <v>174</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>2</v>
@@ -9891,13 +9908,13 @@
         <v>13.7</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="K29" s="10" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9914,16 +9931,16 @@
         <v>150</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9986,7 +10003,7 @@
         <v>11.98</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10006,20 +10023,20 @@
         <v>150</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="15" t="n">
         <v>7.63</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K35" s="10" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10041,7 +10058,7 @@
       <c r="H36" s="12"/>
       <c r="I36" s="15"/>
       <c r="J36" s="10" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10052,7 +10069,7 @@
         <v>182</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D37" s="10" t="n">
         <v>2</v>
@@ -10067,7 +10084,7 @@
         <v>1.18</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10076,7 +10093,7 @@
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D38" s="10" t="n">
         <v>1</v>
@@ -10105,37 +10122,37 @@
         <v>9.35</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="35"/>
       <c r="B40" s="9" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>150</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="I40" s="13" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="35"/>
       <c r="B41" s="9" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D41" s="10" t="n">
         <v>1</v>
@@ -10148,7 +10165,7 @@
         <v>8.99</v>
       </c>
       <c r="J41" s="39" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10162,7 +10179,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10170,32 +10187,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="10" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="10" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="I46" s="13" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10203,24 +10220,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="39" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="J48" s="39" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="K48" s="39" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Docs: mention 90-degree bend micro USB cables
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="323">
   <si>
     <t xml:space="preserve">ID code</t>
   </si>
@@ -216,7 +216,7 @@
     <t xml:space="preserve">Pi power cable (ex: micro USB)</t>
   </si>
   <si>
-    <t xml:space="preserve">Your Pi may come with a cable or a power supply. You will need a cable that fits your Pi, typically Micro USB (although newer board usually use USB C)</t>
+    <t xml:space="preserve">Your Pi may come with a cable or a power supply. You will need a cable that fits your Pi, typically Micro USB (although newer board usually use USB C). A cable with a 90 degree bend on the micro end will fit better in the printed cases.</t>
   </si>
   <si>
     <t xml:space="preserve">MC-FAN</t>
@@ -1494,9 +1494,9 @@
   <dimension ref="A1:AMJ1038"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+      <selection pane="bottomLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.0546875" defaultRowHeight="18.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1839,7 +1839,7 @@
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
     </row>
-    <row r="19" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
         <v>60</v>
       </c>
@@ -1848,6 +1848,9 @@
       </c>
       <c r="C19" s="14" t="n">
         <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="E19" s="2"/>
       <c r="G19" s="14" t="s">
@@ -7416,7 +7419,7 @@
   <autoFilter ref="D1:D1038"/>
   <conditionalFormatting sqref="A70:A1038 A60:A64 A1:A58">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>LEN(TRIM(#REF!))&gt;0</formula>
+      <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -7439,39 +7442,40 @@
     <hyperlink ref="D16" r:id="rId17" display="Amazon link"/>
     <hyperlink ref="D17" r:id="rId18" display="Ali Express Link"/>
     <hyperlink ref="D18" r:id="rId19" display="Ali Express Link"/>
-    <hyperlink ref="D20" r:id="rId20" display="Amazon Link"/>
-    <hyperlink ref="D21" r:id="rId21" display="Amazon link"/>
-    <hyperlink ref="D22" r:id="rId22" display="Amazon link"/>
-    <hyperlink ref="D24" r:id="rId23" display="Amazon link"/>
-    <hyperlink ref="D25" r:id="rId24" display="Github Link"/>
-    <hyperlink ref="D28" r:id="rId25" display="Ali Express link"/>
-    <hyperlink ref="D29" r:id="rId26" display="Amazon link"/>
-    <hyperlink ref="D32" r:id="rId27" display="Amazon link"/>
-    <hyperlink ref="D33" r:id="rId28" display="Amazon link"/>
-    <hyperlink ref="D34" r:id="rId29" display="Amazon link"/>
-    <hyperlink ref="D35" r:id="rId30" display="Amazon link"/>
-    <hyperlink ref="D36" r:id="rId31" display="McMaster link"/>
-    <hyperlink ref="D37" r:id="rId32" display="Amazon link"/>
-    <hyperlink ref="D38" r:id="rId33" display="Amazon Link"/>
-    <hyperlink ref="D40" r:id="rId34" display="Amazon link"/>
-    <hyperlink ref="D43" r:id="rId35" display="Amazon link"/>
-    <hyperlink ref="D44" r:id="rId36" display="Amazon link"/>
-    <hyperlink ref="D45" r:id="rId37" display="Github Link"/>
-    <hyperlink ref="D49" r:id="rId38" display="Amazon link"/>
-    <hyperlink ref="G49" r:id="rId39" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="D50" r:id="rId40" display="Amazon link"/>
-    <hyperlink ref="D51" r:id="rId41" display="Amazon link"/>
-    <hyperlink ref="D52" r:id="rId42" display="Amazon link"/>
-    <hyperlink ref="D53" r:id="rId43" display="Github link"/>
-    <hyperlink ref="D54" r:id="rId44" display="Github link"/>
-    <hyperlink ref="D55" r:id="rId45" display="Github link"/>
-    <hyperlink ref="D56" r:id="rId46" display="Amazon 4oz link"/>
-    <hyperlink ref="E56" r:id="rId47" display="Amazon 6oz link"/>
-    <hyperlink ref="D57" r:id="rId48" display="Amazon link"/>
-    <hyperlink ref="D58" r:id="rId49" display="Github link"/>
-    <hyperlink ref="D61" r:id="rId50" display="Amazon assordment link"/>
-    <hyperlink ref="D64" r:id="rId51" display="Amazon link"/>
-    <hyperlink ref="D66" r:id="rId52" display="Amazon link"/>
+    <hyperlink ref="D19" r:id="rId20" display="Amazon Link"/>
+    <hyperlink ref="D20" r:id="rId21" display="Amazon Link"/>
+    <hyperlink ref="D21" r:id="rId22" display="Amazon link"/>
+    <hyperlink ref="D22" r:id="rId23" display="Amazon link"/>
+    <hyperlink ref="D24" r:id="rId24" display="Amazon link"/>
+    <hyperlink ref="D25" r:id="rId25" display="Github Link"/>
+    <hyperlink ref="D28" r:id="rId26" display="Ali Express link"/>
+    <hyperlink ref="D29" r:id="rId27" display="Amazon link"/>
+    <hyperlink ref="D32" r:id="rId28" display="Amazon link"/>
+    <hyperlink ref="D33" r:id="rId29" display="Amazon link"/>
+    <hyperlink ref="D34" r:id="rId30" display="Amazon link for raw copper tubing"/>
+    <hyperlink ref="D35" r:id="rId31" display="Amazon link"/>
+    <hyperlink ref="D36" r:id="rId32" display="McMaster link"/>
+    <hyperlink ref="D37" r:id="rId33" display="Amazon link"/>
+    <hyperlink ref="D38" r:id="rId34" display="Amazon Link"/>
+    <hyperlink ref="D40" r:id="rId35" display="Amazon link"/>
+    <hyperlink ref="D43" r:id="rId36" display="Amazon link"/>
+    <hyperlink ref="D44" r:id="rId37" display="Amazon link"/>
+    <hyperlink ref="D45" r:id="rId38" display="Github Link"/>
+    <hyperlink ref="D49" r:id="rId39" display="Amazon link"/>
+    <hyperlink ref="G49" r:id="rId40" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
+    <hyperlink ref="D50" r:id="rId41" display="Amazon link"/>
+    <hyperlink ref="D51" r:id="rId42" display="Amazon link"/>
+    <hyperlink ref="D52" r:id="rId43" display="Amazon link"/>
+    <hyperlink ref="D53" r:id="rId44" display="Github link"/>
+    <hyperlink ref="D54" r:id="rId45" display="Github link"/>
+    <hyperlink ref="D55" r:id="rId46" display="Github link"/>
+    <hyperlink ref="D56" r:id="rId47" display="Amazon 4oz link"/>
+    <hyperlink ref="E56" r:id="rId48" display="Amazon 6oz link"/>
+    <hyperlink ref="D57" r:id="rId49" display="Amazon link"/>
+    <hyperlink ref="D58" r:id="rId50" display="Github link"/>
+    <hyperlink ref="D61" r:id="rId51" display="Amazon assordment link"/>
+    <hyperlink ref="D64" r:id="rId52" display="Amazon link"/>
+    <hyperlink ref="D66" r:id="rId53" display="Amazon link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7480,7 +7484,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId53"/>
+  <drawing r:id="rId54"/>
 </worksheet>
 </file>
 
@@ -7495,7 +7499,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.09375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.62"/>

</xml_diff>

<commit_message>
tweak assembly and parts docs
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="445">
   <si>
     <t xml:space="preserve">MicroLab Parts List</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t xml:space="preserve">Control Case (Printed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MicroLab link</t>
   </si>
   <si>
     <t xml:space="preserve">Github Link</t>
@@ -516,6 +513,9 @@
     <t xml:space="preserve">Cooling Unit Lid (Printed)</t>
   </si>
   <si>
+    <t xml:space="preserve">MicroLab link</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lid for the  jar </t>
   </si>
   <si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reactor manifold core (Printed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: For particularly high temperatures (above 70C) or particularly strong solvents, you may want materials that are not common for consumer printers. Ordering from a vendor like Craftcloud in a material such as ULTEM 1010 or PPSU costs around $75 for this part (in summer 2024).</t>
   </si>
   <si>
     <t xml:space="preserve">RU-LID</t>
@@ -2336,11 +2339,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G91" activeCellId="0" sqref="G91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F105" activeCellId="0" sqref="F105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.03125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -2733,7 +2736,7 @@
       </c>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -2749,83 +2752,75 @@
       <c r="E23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="0"/>
+      <c r="G23" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="H23" s="24"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="0"/>
+      <c r="G24" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="0"/>
+      <c r="G25" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="H25" s="24"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="0"/>
+      <c r="G26" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="H26" s="24"/>
     </row>
@@ -2834,20 +2829,20 @@
         <v>11</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H27" s="24"/>
     </row>
@@ -2856,16 +2851,16 @@
         <v>11</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D28" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="33" t="s">
         <v>68</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>69</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="6"/>
@@ -2876,16 +2871,16 @@
         <v>11</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="24"/>
@@ -2895,22 +2890,22 @@
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H30" s="24"/>
     </row>
@@ -2919,19 +2914,19 @@
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F31" s="30" t="s">
         <v>14</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H31" s="24"/>
     </row>
@@ -2940,13 +2935,13 @@
         <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E32" s="31" t="s">
         <v>14</v>
@@ -2960,13 +2955,13 @@
         <v>11</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" s="31" t="s">
         <v>14</v>
@@ -2980,13 +2975,13 @@
         <v>11</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E34" s="31" t="s">
         <v>14</v>
@@ -3000,13 +2995,13 @@
         <v>11</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E35" s="31" t="s">
         <v>14</v>
@@ -3028,7 +3023,7 @@
     </row>
     <row r="38" s="20" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" s="16"/>
       <c r="C38" s="15"/>
@@ -3040,244 +3035,244 @@
     </row>
     <row r="39" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H39" s="24"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="E40" s="30" t="s">
         <v>14</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H40" s="24"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42" s="34" t="n">
         <v>2</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E42" s="35" t="s">
         <v>14</v>
       </c>
       <c r="G42" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H42" s="24"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="34" t="n">
         <v>2</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E43" s="35"/>
       <c r="G43" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H43" s="24"/>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E44" s="35"/>
       <c r="G44" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H44" s="24"/>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>23</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E45" s="31" t="s">
         <v>44</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H45" s="24"/>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>28</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E46" s="31"/>
       <c r="G46" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H46" s="24"/>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E47" s="31"/>
       <c r="G47" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H47" s="24"/>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E48" s="31"/>
       <c r="G48" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H48" s="24"/>
     </row>
     <row r="49" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E49" s="36" t="s">
         <v>118</v>
-      </c>
-      <c r="E49" s="36" t="s">
-        <v>119</v>
       </c>
       <c r="F49" s="37" t="s">
         <v>14</v>
       </c>
       <c r="G49" s="38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="28" t="s">
         <v>122</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>123</v>
       </c>
       <c r="E50" s="30" t="s">
         <v>14</v>
       </c>
       <c r="G50" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H50" s="39"/>
     </row>
@@ -3296,7 +3291,7 @@
     </row>
     <row r="54" s="46" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B54" s="41"/>
       <c r="C54" s="42"/>
@@ -3309,38 +3304,38 @@
     </row>
     <row r="55" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" s="27" t="s">
         <v>126</v>
-      </c>
-      <c r="B55" s="27" t="s">
-        <v>127</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F55" s="47"/>
       <c r="G55" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H55" s="48"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>14</v>
@@ -3351,105 +3346,105 @@
     </row>
     <row r="57" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D57" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="G57" s="23" t="s">
         <v>135</v>
-      </c>
-      <c r="G57" s="23" t="s">
-        <v>136</v>
       </c>
       <c r="H57" s="48"/>
     </row>
     <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F58" s="47"/>
       <c r="G58" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H58" s="48"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C59" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D59" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="F59" s="49"/>
       <c r="G59" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H59" s="24"/>
     </row>
     <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B60" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C60" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G60" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H60" s="48"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C61" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D61" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>14</v>
@@ -3459,35 +3454,35 @@
     </row>
     <row r="62" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C62" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F62" s="50"/>
       <c r="G62" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H62" s="48"/>
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B63" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C63" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F63" s="50"/>
       <c r="G63" s="23"/>
@@ -3495,16 +3490,16 @@
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C64" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E64" s="31" t="s">
         <v>14</v>
@@ -3515,39 +3510,39 @@
     </row>
     <row r="65" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C65" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="G65" s="23" t="s">
         <v>157</v>
-      </c>
-      <c r="G65" s="23" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="F66" s="31" t="s">
         <v>55</v>
-      </c>
-      <c r="F66" s="31" t="s">
-        <v>56</v>
       </c>
       <c r="G66" s="6" t="s">
         <v>161</v>
@@ -3556,7 +3551,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>162</v>
@@ -3568,10 +3563,10 @@
         <v>163</v>
       </c>
       <c r="E67" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F67" s="31" t="s">
         <v>55</v>
-      </c>
-      <c r="F67" s="31" t="s">
-        <v>56</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>164</v>
@@ -3579,7 +3574,7 @@
     </row>
     <row r="68" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>165</v>
@@ -3676,7 +3671,7 @@
       <c r="G73" s="23"/>
       <c r="H73" s="48"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>169</v>
       </c>
@@ -3689,38 +3684,36 @@
       <c r="D74" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E74" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="F74" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="G74" s="23"/>
+      <c r="F74" s="0"/>
+      <c r="G74" s="23" t="s">
+        <v>180</v>
+      </c>
       <c r="H74" s="24"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C75" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D75" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="E75" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E75" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="F75" s="31" t="s">
-        <v>56</v>
-      </c>
+      <c r="F75" s="0"/>
       <c r="G75" s="23"/>
       <c r="H75" s="24"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>169</v>
       </c>
@@ -3731,38 +3724,34 @@
         <v>1</v>
       </c>
       <c r="D76" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="E76" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E76" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="F76" s="31" t="s">
-        <v>56</v>
-      </c>
+      <c r="F76" s="0"/>
       <c r="G76" s="23" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H76" s="24"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C77" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="E77" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E77" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="F77" s="31" t="s">
-        <v>56</v>
-      </c>
+      <c r="F77" s="0"/>
       <c r="G77" s="23"/>
       <c r="H77" s="24"/>
     </row>
@@ -3777,16 +3766,16 @@
         <v>1</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G78" s="23" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H78" s="48"/>
     </row>
@@ -3795,115 +3784,107 @@
         <v>169</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C79" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G79" s="23" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H79" s="24"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B80" s="27" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C80" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F80" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="F80" s="0"/>
       <c r="G80" s="23" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H80" s="24"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C81" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="F81" s="0"/>
       <c r="G81" s="23" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H81" s="24"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C82" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F82" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="F82" s="0"/>
       <c r="G82" s="23" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H82" s="24"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C83" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F83" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="F83" s="0"/>
       <c r="G83" s="23" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H83" s="24"/>
     </row>
@@ -3912,41 +3893,41 @@
         <v>169</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C84" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H84" s="24"/>
     </row>
-    <row r="85" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G85" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H85" s="24"/>
     </row>
@@ -3955,67 +3936,63 @@
         <v>169</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C86" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G86" s="23" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H86" s="24"/>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C87" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F87" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="F87" s="0"/>
       <c r="G87" s="23" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H87" s="24"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C88" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F88" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="F88" s="0"/>
       <c r="G88" s="23" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H88" s="24"/>
     </row>
@@ -4024,20 +4001,20 @@
         <v>169</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C89" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F89" s="47"/>
       <c r="G89" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H89" s="48"/>
     </row>
@@ -4046,16 +4023,16 @@
         <v>169</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D90" s="28" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G90" s="23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9038,75 +9015,62 @@
     <hyperlink ref="E20" r:id="rId13" display="Amazon link"/>
     <hyperlink ref="E21" r:id="rId14" display="Amazon link"/>
     <hyperlink ref="E22" r:id="rId15" display="Amazon link"/>
-    <hyperlink ref="E23" r:id="rId16" display="MicroLab link"/>
-    <hyperlink ref="F23" r:id="rId17" display="Github Link"/>
-    <hyperlink ref="E24" r:id="rId18" display="MicroLab link"/>
-    <hyperlink ref="F24" r:id="rId19" display="Github Link"/>
-    <hyperlink ref="E25" r:id="rId20" display="MicroLab link"/>
-    <hyperlink ref="F25" r:id="rId21" display="Github Link"/>
-    <hyperlink ref="E26" r:id="rId22" display="MicroLab link"/>
-    <hyperlink ref="F26" r:id="rId23" display="Github Link"/>
-    <hyperlink ref="E27" r:id="rId24" display="Amazon link"/>
-    <hyperlink ref="E28" r:id="rId25" display="Ali Express Link"/>
-    <hyperlink ref="E29" r:id="rId26" display="Ali Express Link"/>
-    <hyperlink ref="E30" r:id="rId27" display="Amazon link"/>
-    <hyperlink ref="F30" r:id="rId28" display="Ali Express Link"/>
-    <hyperlink ref="F31" r:id="rId29" display="Amazon link"/>
-    <hyperlink ref="E32" r:id="rId30" display="Amazon link"/>
-    <hyperlink ref="E33" r:id="rId31" display="Amazon link"/>
-    <hyperlink ref="E34" r:id="rId32" display="Amazon link"/>
-    <hyperlink ref="E35" r:id="rId33" display="Amazon link"/>
-    <hyperlink ref="E39" r:id="rId34" display="Amazon link"/>
-    <hyperlink ref="E40" r:id="rId35" display="Amazon link"/>
-    <hyperlink ref="E41" r:id="rId36" display="Amazon link"/>
-    <hyperlink ref="E42" r:id="rId37" display="Amazon link"/>
-    <hyperlink ref="E45" r:id="rId38" display="Amazon link - assortment"/>
-    <hyperlink ref="F49" r:id="rId39" display="Amazon link"/>
-    <hyperlink ref="E50" r:id="rId40" display="Amazon link"/>
-    <hyperlink ref="E55" r:id="rId41" display="Amazon link"/>
-    <hyperlink ref="E56" r:id="rId42" display="Amazon link"/>
-    <hyperlink ref="E57" r:id="rId43" display="Amazon link for raw copper tubing"/>
-    <hyperlink ref="E58" r:id="rId44" display="Amazon link"/>
-    <hyperlink ref="E59" r:id="rId45" display="McMaster link"/>
-    <hyperlink ref="E60" r:id="rId46" display="Amazon link"/>
-    <hyperlink ref="E61" r:id="rId47" display="Amazon link"/>
-    <hyperlink ref="E64" r:id="rId48" display="Amazon link"/>
-    <hyperlink ref="E66" r:id="rId49" display="MicroLab link"/>
-    <hyperlink ref="F66" r:id="rId50" display="Github Link"/>
-    <hyperlink ref="E67" r:id="rId51" display="MicroLab link"/>
-    <hyperlink ref="F67" r:id="rId52" display="Github Link"/>
-    <hyperlink ref="E71" r:id="rId53" display="Amazon link"/>
-    <hyperlink ref="G71" r:id="rId54" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E72" r:id="rId55" display="Amazon link"/>
-    <hyperlink ref="E73" r:id="rId56" display="Amazon link"/>
-    <hyperlink ref="E74" r:id="rId57" display="MicroLab link"/>
-    <hyperlink ref="F74" r:id="rId58" display="Github Link"/>
-    <hyperlink ref="E75" r:id="rId59" display="MicroLab link"/>
-    <hyperlink ref="F75" r:id="rId60" display="Github Link"/>
-    <hyperlink ref="E76" r:id="rId61" display="MicroLab link"/>
-    <hyperlink ref="F76" r:id="rId62" display="Github Link"/>
-    <hyperlink ref="E77" r:id="rId63" display="MicroLab link"/>
-    <hyperlink ref="F77" r:id="rId64" display="Github Link"/>
-    <hyperlink ref="E78" r:id="rId65" display="Amazon 4oz link"/>
-    <hyperlink ref="F78" r:id="rId66" display="Amazon 6oz link"/>
-    <hyperlink ref="E79" r:id="rId67" display="Amazon link"/>
-    <hyperlink ref="E80" r:id="rId68" display="MicroLab link"/>
-    <hyperlink ref="F80" r:id="rId69" display="Github Link"/>
-    <hyperlink ref="E81" r:id="rId70" display="MicroLab link"/>
-    <hyperlink ref="F81" r:id="rId71" display="Github Link"/>
-    <hyperlink ref="E82" r:id="rId72" display="MicroLab link"/>
-    <hyperlink ref="F82" r:id="rId73" display="Github Link"/>
-    <hyperlink ref="E83" r:id="rId74" display="MicroLab link"/>
-    <hyperlink ref="F83" r:id="rId75" display="Github Link"/>
-    <hyperlink ref="E84" r:id="rId76" display="Ali Express link"/>
-    <hyperlink ref="G84" r:id="rId77" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
-    <hyperlink ref="E85" r:id="rId78" display="Amazon link"/>
-    <hyperlink ref="E86" r:id="rId79" display="Amazon link"/>
-    <hyperlink ref="E87" r:id="rId80" display="MicroLab link"/>
-    <hyperlink ref="F87" r:id="rId81" display="Github Link"/>
-    <hyperlink ref="E88" r:id="rId82" display="MicroLab link"/>
-    <hyperlink ref="F88" r:id="rId83" display="Github Link"/>
-    <hyperlink ref="E89" r:id="rId84" display="Amazon link"/>
+    <hyperlink ref="E23" r:id="rId16" display="Github Link"/>
+    <hyperlink ref="E24" r:id="rId17" display="Github Link"/>
+    <hyperlink ref="E25" r:id="rId18" display="Github Link"/>
+    <hyperlink ref="E26" r:id="rId19" display="Github Link"/>
+    <hyperlink ref="E27" r:id="rId20" display="Amazon link"/>
+    <hyperlink ref="E28" r:id="rId21" display="Ali Express Link"/>
+    <hyperlink ref="E29" r:id="rId22" display="Ali Express Link"/>
+    <hyperlink ref="E30" r:id="rId23" display="Amazon link"/>
+    <hyperlink ref="F30" r:id="rId24" display="Ali Express Link"/>
+    <hyperlink ref="F31" r:id="rId25" display="Amazon link"/>
+    <hyperlink ref="E32" r:id="rId26" display="Amazon link"/>
+    <hyperlink ref="E33" r:id="rId27" display="Amazon link"/>
+    <hyperlink ref="E34" r:id="rId28" display="Amazon link"/>
+    <hyperlink ref="E35" r:id="rId29" display="Amazon link"/>
+    <hyperlink ref="E39" r:id="rId30" display="Amazon link"/>
+    <hyperlink ref="E40" r:id="rId31" display="Amazon link"/>
+    <hyperlink ref="E41" r:id="rId32" display="Amazon link"/>
+    <hyperlink ref="E42" r:id="rId33" display="Amazon link"/>
+    <hyperlink ref="E45" r:id="rId34" display="Amazon link - assortment"/>
+    <hyperlink ref="F49" r:id="rId35" display="Amazon link"/>
+    <hyperlink ref="E50" r:id="rId36" display="Amazon link"/>
+    <hyperlink ref="E55" r:id="rId37" display="Amazon link"/>
+    <hyperlink ref="E56" r:id="rId38" display="Amazon link"/>
+    <hyperlink ref="E57" r:id="rId39" display="Amazon link for raw copper tubing"/>
+    <hyperlink ref="E58" r:id="rId40" display="Amazon link"/>
+    <hyperlink ref="E59" r:id="rId41" display="McMaster link"/>
+    <hyperlink ref="E60" r:id="rId42" display="Amazon link"/>
+    <hyperlink ref="E61" r:id="rId43" display="Amazon link"/>
+    <hyperlink ref="E64" r:id="rId44" display="Amazon link"/>
+    <hyperlink ref="E66" r:id="rId45" display="MicroLab link"/>
+    <hyperlink ref="F66" r:id="rId46" display="Github Link"/>
+    <hyperlink ref="E67" r:id="rId47" display="MicroLab link"/>
+    <hyperlink ref="F67" r:id="rId48" display="Github Link"/>
+    <hyperlink ref="E71" r:id="rId49" display="Amazon link"/>
+    <hyperlink ref="G71" r:id="rId50" display="This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
+    <hyperlink ref="E72" r:id="rId51" display="Amazon link"/>
+    <hyperlink ref="E73" r:id="rId52" display="Amazon link"/>
+    <hyperlink ref="E74" r:id="rId53" display="Github Link"/>
+    <hyperlink ref="G74" r:id="rId54" display="Craftcloud"/>
+    <hyperlink ref="E75" r:id="rId55" display="Github Link"/>
+    <hyperlink ref="E76" r:id="rId56" display="Github Link"/>
+    <hyperlink ref="E77" r:id="rId57" display="Github Link"/>
+    <hyperlink ref="E78" r:id="rId58" display="Amazon 4oz link"/>
+    <hyperlink ref="F78" r:id="rId59" display="Amazon 6oz link"/>
+    <hyperlink ref="E79" r:id="rId60" display="Amazon link"/>
+    <hyperlink ref="E80" r:id="rId61" display="Github Link"/>
+    <hyperlink ref="E81" r:id="rId62" display="Github Link"/>
+    <hyperlink ref="E82" r:id="rId63" display="Github Link"/>
+    <hyperlink ref="E83" r:id="rId64" display="Github Link"/>
+    <hyperlink ref="E84" r:id="rId65" display="Ali Express link"/>
+    <hyperlink ref="G84" r:id="rId66" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
+    <hyperlink ref="E85" r:id="rId67" display="Amazon link"/>
+    <hyperlink ref="E86" r:id="rId68" display="Amazon link"/>
+    <hyperlink ref="E87" r:id="rId69" display="Github Link"/>
+    <hyperlink ref="E88" r:id="rId70" display="Github Link"/>
+    <hyperlink ref="E89" r:id="rId71" display="Amazon link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -9129,7 +9093,7 @@
       <selection pane="topLeft" activeCell="D92" activeCellId="0" sqref="D92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.03125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="13.02"/>
@@ -9251,7 +9215,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H10" s="24"/>
     </row>
@@ -9273,7 +9237,7 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="25" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H11" s="24"/>
     </row>
@@ -9521,11 +9485,11 @@
         <v>54</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H23" s="24"/>
     </row>
@@ -9534,20 +9498,20 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H24" s="24"/>
     </row>
@@ -9556,20 +9520,20 @@
         <v>11</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H25" s="24"/>
     </row>
@@ -9578,20 +9542,20 @@
         <v>11</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H26" s="24"/>
     </row>
@@ -9600,20 +9564,20 @@
         <v>11</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="23" t="n">
         <v>2</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H27" s="24"/>
     </row>
@@ -9622,16 +9586,16 @@
         <v>11</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="23" t="n">
         <v>2</v>
       </c>
       <c r="D28" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="33" t="s">
         <v>68</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>69</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="6"/>
@@ -9642,16 +9606,16 @@
         <v>11</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C29" s="32" t="n">
         <v>2</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="32"/>
@@ -9662,16 +9626,16 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="59" t="s">
         <v>68</v>
-      </c>
-      <c r="E30" s="59" t="s">
-        <v>69</v>
       </c>
       <c r="F30" s="59"/>
       <c r="G30" s="6"/>
@@ -9682,20 +9646,20 @@
         <v>11</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C31" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H31" s="24"/>
     </row>
@@ -9704,20 +9668,20 @@
         <v>11</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E32" s="30" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H32" s="24"/>
     </row>
@@ -9728,7 +9692,7 @@
     </row>
     <row r="34" s="20" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="57"/>
       <c r="D34" s="57"/>
@@ -9739,244 +9703,244 @@
     </row>
     <row r="35" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H35" s="24"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="E36" s="30" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H36" s="24"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="C37" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C38" s="32" t="n">
         <v>2</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E38" s="35" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H38" s="24"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" s="32" t="n">
         <v>2</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E39" s="35"/>
       <c r="G39" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H39" s="24"/>
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C40" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D40" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E40" s="35"/>
       <c r="G40" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H40" s="24"/>
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C41" s="6" t="n">
         <v>23</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E41" s="26" t="s">
         <v>44</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H41" s="24"/>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C42" s="6" t="n">
         <v>28</v>
       </c>
       <c r="D42" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E42" s="26"/>
       <c r="G42" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H42" s="24"/>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C43" s="6" t="n">
         <v>5</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E43" s="26"/>
       <c r="G43" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H43" s="24"/>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C44" s="6" t="n">
         <v>5</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E44" s="26"/>
       <c r="G44" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H44" s="24"/>
     </row>
     <row r="45" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>6</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F45" s="37" t="s">
         <v>14</v>
       </c>
       <c r="G45" s="38" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="D46" s="39" t="s">
         <v>122</v>
-      </c>
-      <c r="D46" s="39" t="s">
-        <v>123</v>
       </c>
       <c r="E46" s="30" t="s">
         <v>14</v>
       </c>
       <c r="G46" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H46" s="39"/>
     </row>
@@ -9999,7 +9963,7 @@
     </row>
     <row r="50" s="46" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B50" s="60"/>
       <c r="D50" s="57"/>
@@ -10011,38 +9975,38 @@
     </row>
     <row r="51" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B51" s="39" t="s">
         <v>126</v>
-      </c>
-      <c r="B51" s="39" t="s">
-        <v>127</v>
       </c>
       <c r="C51" s="23" t="n">
         <v>2</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F51" s="47"/>
       <c r="G51" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H51" s="48"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C52" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D52" s="39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>14</v>
@@ -10053,105 +10017,105 @@
     </row>
     <row r="53" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C53" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D53" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="G53" s="23" t="s">
         <v>135</v>
-      </c>
-      <c r="G53" s="23" t="s">
-        <v>136</v>
       </c>
       <c r="H53" s="48"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C54" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D54" s="39" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F54" s="47"/>
       <c r="G54" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H54" s="48"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C55" s="23" t="n">
         <v>2</v>
       </c>
       <c r="D55" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="F55" s="49"/>
       <c r="G55" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H55" s="24"/>
     </row>
     <row r="56" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C56" s="23" t="n">
         <v>2</v>
       </c>
       <c r="D56" s="39" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G56" s="23" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H56" s="48"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C57" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D57" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>25</v>
@@ -10161,42 +10125,42 @@
     </row>
     <row r="58" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C58" s="23" t="n">
         <v>2</v>
       </c>
       <c r="D58" s="39" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F58" s="50"/>
       <c r="G58" s="23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H58" s="48"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C59" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D59" s="39" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H59" s="24"/>
     </row>
@@ -10210,7 +10174,7 @@
     </row>
     <row r="61" s="46" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="57" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B61" s="60"/>
       <c r="D61" s="57"/>
@@ -10222,16 +10186,16 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C62" s="5" t="n">
         <v>3</v>
       </c>
       <c r="D62" s="39" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>14</v>
@@ -10241,62 +10205,62 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D63" s="39" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G63" s="23" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H63" s="24"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D64" s="39" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G64" s="23"/>
       <c r="H64" s="24"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C65" s="23" t="n">
         <v>2</v>
       </c>
       <c r="D65" s="39" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G65" s="23" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H65" s="24"/>
     </row>
@@ -10324,13 +10288,13 @@
         <v>169</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C68" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D68" s="39" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>14</v>
@@ -10345,13 +10309,13 @@
         <v>169</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C69" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D69" s="39" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>14</v>
@@ -10366,17 +10330,17 @@
         <v>169</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C70" s="23"/>
       <c r="D70" s="39" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G70" s="23" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H70" s="48"/>
     </row>
@@ -10385,11 +10349,11 @@
         <v>169</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C71" s="23"/>
       <c r="D71" s="39" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>14</v>
@@ -10402,16 +10366,16 @@
         <v>169</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C72" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D72" s="39" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G72" s="23"/>
       <c r="H72" s="24"/>
@@ -10421,19 +10385,19 @@
         <v>169</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C73" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D73" s="39" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G73" s="23" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H73" s="24"/>
     </row>
@@ -10442,16 +10406,16 @@
         <v>169</v>
       </c>
       <c r="B74" s="39" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C74" s="23" t="n">
         <v>2</v>
       </c>
       <c r="D74" s="39" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G74" s="23"/>
       <c r="H74" s="24"/>
@@ -10467,16 +10431,16 @@
         <v>1</v>
       </c>
       <c r="D75" s="39" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G75" s="23" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H75" s="48"/>
     </row>
@@ -10485,19 +10449,19 @@
         <v>169</v>
       </c>
       <c r="B76" s="39" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C76" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D76" s="39" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G76" s="23" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H76" s="24"/>
     </row>
@@ -10506,19 +10470,19 @@
         <v>169</v>
       </c>
       <c r="B77" s="39" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C77" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D77" s="39" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G77" s="23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H77" s="24"/>
     </row>
@@ -10527,20 +10491,20 @@
         <v>169</v>
       </c>
       <c r="B78" s="39" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C78" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D78" s="39" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H78" s="24"/>
     </row>
@@ -10639,25 +10603,25 @@
         <v>176</v>
       </c>
       <c r="E94" s="28" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="39"/>
       <c r="D95" s="27" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E95" s="28" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="39"/>
       <c r="D96" s="27" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E96" s="28" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F96" s="4" t="n">
         <v>1</v>
@@ -10669,7 +10633,7 @@
         <v>170</v>
       </c>
       <c r="E97" s="28" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F97" s="4" t="n">
         <v>1</v>
@@ -10678,10 +10642,10 @@
     <row r="98" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="39"/>
       <c r="D98" s="27" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E98" s="28" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F98" s="4" t="n">
         <v>2</v>
@@ -10693,7 +10657,7 @@
         <v>178</v>
       </c>
       <c r="E99" s="28" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F99" s="4" t="n">
         <v>1</v>
@@ -10702,10 +10666,10 @@
     <row r="100" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="39"/>
       <c r="D100" s="27" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E100" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F100" s="4" t="n">
         <v>1</v>
@@ -10714,10 +10678,10 @@
     <row r="101" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="39"/>
       <c r="D101" s="27" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E101" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F101" s="4" t="n">
         <v>1</v>
@@ -10726,10 +10690,10 @@
     <row r="102" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="39"/>
       <c r="D102" s="27" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E102" s="28" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F102" s="4" t="n">
         <v>1</v>
@@ -10738,10 +10702,10 @@
     <row r="103" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="39"/>
       <c r="D103" s="27" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E103" s="28" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F103" s="4" t="n">
         <v>1</v>
@@ -10750,10 +10714,10 @@
     <row r="104" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="39"/>
       <c r="D104" s="27" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E104" s="28" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F104" s="4" t="n">
         <v>1</v>
@@ -10762,10 +10726,10 @@
     <row r="105" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="39"/>
       <c r="D105" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E105" s="28" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F105" s="4" t="n">
         <v>1</v>
@@ -10774,10 +10738,10 @@
     <row r="106" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="39"/>
       <c r="D106" s="27" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E106" s="28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F106" s="1" t="n">
         <v>3</v>
@@ -10786,10 +10750,10 @@
     <row r="107" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="39"/>
       <c r="D107" s="27" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E107" s="28" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F107" s="4" t="n">
         <v>3</v>
@@ -10798,10 +10762,10 @@
     <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="39"/>
       <c r="D108" s="27" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E108" s="28" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F108" s="4" t="n">
         <v>1</v>
@@ -10810,10 +10774,10 @@
     <row r="109" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="39"/>
       <c r="D109" s="27" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E109" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F109" s="4" t="n">
         <v>1</v>
@@ -15729,7 +15693,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.19921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.66"/>
@@ -15739,773 +15703,773 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="61" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B1" s="61" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C1" s="61" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="62" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E1" s="62" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="62" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G1" s="62" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H1" s="63" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I1" s="62" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="J1" s="62" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="61" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C2" s="61" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D2" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G2" s="62" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H2" s="63" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I2" s="65" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="62" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="61" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C3" s="61" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E3" s="66" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H3" s="63" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="I3" s="65" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="61" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D4" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F4" s="64" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H4" s="67" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I4" s="65" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="62" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K4" s="65" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="61" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D5" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="66" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H5" s="63"/>
       <c r="I5" s="65" t="n">
         <v>7.36</v>
       </c>
       <c r="J5" s="62" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="61" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D6" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="66" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H6" s="63"/>
       <c r="I6" s="65"/>
       <c r="J6" s="62" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="61" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D7" s="62" t="n">
         <v>4</v>
       </c>
       <c r="E7" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H7" s="63"/>
       <c r="I7" s="65" t="n">
         <v>9.99</v>
       </c>
       <c r="J7" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K7" s="62" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D8" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H8" s="63" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="I8" s="65" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="61" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D9" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="68" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H9" s="63"/>
       <c r="I9" s="69"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="61" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C10" s="61" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D10" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H10" s="63" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I10" s="69" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K10" s="62" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="L10" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="61" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B11" s="61" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C11" s="61" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D11" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H11" s="63" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I11" s="65" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="61" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C12" s="61" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D12" s="62"/>
       <c r="E12" s="64" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G12" s="62"/>
       <c r="H12" s="63" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="I12" s="65" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="61" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B13" s="61" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D13" s="62"/>
       <c r="E13" s="62"/>
       <c r="G13" s="62"/>
       <c r="H13" s="63" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="I13" s="69"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="61" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D14" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G14" s="62" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="H14" s="63"/>
       <c r="I14" s="65" t="n">
         <v>3.82</v>
       </c>
       <c r="J14" s="62" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="61" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D15" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H15" s="63" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="I15" s="65" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="61" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C16" s="61" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D16" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H16" s="63"/>
       <c r="I16" s="65" t="n">
         <v>10.91</v>
       </c>
       <c r="J16" s="62" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C17" s="61" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D17" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F17" s="62"/>
       <c r="H17" s="63" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I17" s="65" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="J17" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K17" s="62" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="61" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B18" s="61" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C18" s="61" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D18" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H18" s="63" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="I18" s="65" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="61" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D19" s="62" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H19" s="63" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I19" s="65" t="n">
         <v>64.08</v>
       </c>
       <c r="J19" s="62" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="61" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D20" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H20" s="63"/>
       <c r="I20" s="69"/>
       <c r="J20" s="62" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="61" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C21" s="61" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D21" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H21" s="63"/>
       <c r="I21" s="65" t="n">
         <v>26.79</v>
       </c>
       <c r="J21" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="61" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C22" s="70" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D22" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H22" s="63"/>
       <c r="I22" s="69"/>
       <c r="J22" s="62" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="61" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D23" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E23" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H23" s="63"/>
       <c r="I23" s="69"/>
       <c r="J23" s="62" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="61" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C24" s="70" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D24" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H24" s="63"/>
       <c r="I24" s="69"/>
       <c r="J24" s="62" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="61" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D25" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H25" s="63"/>
       <c r="I25" s="69"/>
       <c r="J25" s="62" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="61" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C26" s="61" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D26" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H26" s="63"/>
       <c r="I26" s="69"/>
       <c r="J26" s="62" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="61" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D27" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H27" s="63"/>
       <c r="I27" s="69"/>
       <c r="J27" s="62" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="61" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C28" s="61" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D28" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="62" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H28" s="63"/>
       <c r="I28" s="69"/>
       <c r="J28" s="62" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="61" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C29" s="61" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D29" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E29" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F29" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G29" s="62" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H29" s="63"/>
       <c r="I29" s="69" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="62" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K29" s="62" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="61" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B30" s="61" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C30" s="61" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E30" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H30" s="63" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="I30" s="65" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="J30" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K30" s="62" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="61"/>
       <c r="B31" s="61" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C31" s="61" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E31" s="68"/>
       <c r="H31" s="63"/>
@@ -16514,10 +16478,10 @@
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="61"/>
       <c r="B32" s="61" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C32" s="61" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E32" s="68"/>
       <c r="H32" s="63"/>
@@ -16526,10 +16490,10 @@
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="61"/>
       <c r="B33" s="61" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C33" s="61" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E33" s="68"/>
       <c r="H33" s="63"/>
@@ -16537,119 +16501,119 @@
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="61" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B34" s="61" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C34" s="70" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D34" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E34" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G34" s="62" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="H34" s="63"/>
       <c r="I34" s="65" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="61" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B35" s="61" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C35" s="61" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D35" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F35" s="64" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H35" s="63"/>
       <c r="I35" s="69" t="n">
         <v>7.63</v>
       </c>
       <c r="J35" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K35" s="62" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="61" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B36" s="61" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C36" s="61" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D36" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H36" s="63"/>
       <c r="I36" s="69"/>
       <c r="J36" s="62" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="61" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B37" s="61" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C37" s="61" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D37" s="62" t="n">
         <v>2</v>
       </c>
       <c r="E37" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H37" s="63" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="I37" s="65" t="n">
         <v>1.18</v>
       </c>
       <c r="J37" s="62" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="61" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B38" s="61"/>
       <c r="C38" s="61" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D38" s="62" t="n">
         <v>1</v>
@@ -16659,69 +16623,69 @@
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="61" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B39" s="61" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C39" s="61" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D39" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E39" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H39" s="63"/>
       <c r="I39" s="65" t="n">
         <v>9.35</v>
       </c>
       <c r="J39" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="71"/>
       <c r="B40" s="61" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C40" s="61" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E40" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H40" s="63" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="I40" s="65" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="71"/>
       <c r="B41" s="61" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C41" s="61" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D41" s="62" t="n">
         <v>1</v>
       </c>
       <c r="E41" s="64" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H41" s="63"/>
       <c r="I41" s="72" t="n">
         <v>8.99</v>
       </c>
       <c r="J41" s="73" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16735,7 +16699,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="62" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16743,32 +16707,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="62" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="K44" s="62" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="62" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="K45" s="62" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="62" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="I46" s="65" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="62" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="K46" s="62" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16776,24 +16740,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="62" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="K47" s="62" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="L47" s="62" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="73" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="J48" s="73" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="K48" s="73" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
A bit more detail in the parts list
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -235,7 +235,7 @@
     <t xml:space="preserve">Ali Express Link</t>
   </si>
   <si>
-    <t xml:space="preserve">Straight connectors will work best</t>
+    <t xml:space="preserve">Straight connectors will work best, shorter length (25cm) is recommended.</t>
   </si>
   <si>
     <t xml:space="preserve">CU-SDC</t>
@@ -1936,11 +1936,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.03125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -8667,7 +8667,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.19921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.66"/>

</xml_diff>

<commit_message>
Add note about peristaltics availability to parts list.
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -654,7 +654,8 @@
     <t xml:space="preserve">Alibaba Link</t>
   </si>
   <si>
-    <t xml:space="preserve">The 3 stepper motors should come with their own cable, but will need to cut in half and split between the Control Unit and the pumps box. </t>
+    <t xml:space="preserve">The 3 stepper motors should come with their own cable, but will need to cut in half and split between the Control Unit and the pumps box. 
+NOTE: Those links are likely to be sold out. There are other stepper-driven pumps, but they will not interface seamlessly with the printed parts. We’re also looking for DIY/printable designs.</t>
   </si>
   <si>
     <t xml:space="preserve">RU-SYR</t>
@@ -1936,8 +1937,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G84" activeCellId="0" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3489,7 +3490,7 @@
       </c>
       <c r="H82" s="28"/>
     </row>
-    <row r="83" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>166</v>
       </c>
@@ -8667,7 +8668,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.23828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.66"/>

</xml_diff>

<commit_message>
Update parts list to include new reactor core
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="390">
   <si>
     <t xml:space="preserve">MicroLab Parts List</t>
   </si>
@@ -549,19 +549,52 @@
     <t xml:space="preserve">RU-COR</t>
   </si>
   <si>
-    <t xml:space="preserve">Reactor manifold core (Printed)</t>
+    <t xml:space="preserve">Old Reactor manifold core (Printed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: New Reactor Core files here.</t>
   </si>
   <si>
     <t xml:space="preserve">RU-LID</t>
   </si>
   <si>
-    <t xml:space="preserve">Reactor manifold lid (Printed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stir rod mount (Printed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE: the motor mount is under development and does not exactly fit the linked motor</t>
+    <t xml:space="preserve">Old Reactor manifold lid (Printed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: This part is obsolete with the new Reactor Core design.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU-PTFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTFE Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old Stir rod mount (Printed)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NOTE: This part is obsolete with the new Reactor Core design
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NOTE: the motor mount is under development and does not exactly fit the linked motor</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">RU-RJF</t>
@@ -579,16 +612,13 @@
     <t xml:space="preserve">Amazon 6oz link</t>
   </si>
   <si>
-    <t xml:space="preserve">6oz jars are optimal but are hard to find individually</t>
+    <t xml:space="preserve">NOTE: New Reactor Core uses a GL45 250ml bottle instead!</t>
   </si>
   <si>
     <t xml:space="preserve">RU-OUT</t>
   </si>
   <si>
     <t xml:space="preserve">32oz wide mouth mason jar for outer jacket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Same jar as the temperature control units</t>
   </si>
   <si>
     <t xml:space="preserve">RU-SDH</t>
@@ -2026,8 +2056,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G73" activeCellId="0" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3327,7 +3357,9 @@
       <c r="F71" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="G71" s="27"/>
+      <c r="G71" s="12" t="s">
+        <v>174</v>
+      </c>
       <c r="H71" s="28"/>
     </row>
     <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3335,13 +3367,13 @@
         <v>163</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C72" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>55</v>
@@ -3349,45 +3381,43 @@
       <c r="F72" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="G72" s="27"/>
+      <c r="G72" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="H72" s="28"/>
     </row>
-    <row r="73" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="C73" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F73" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G73" s="27" t="s">
-        <v>177</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F73" s="34"/>
+      <c r="G73" s="12"/>
       <c r="H73" s="28"/>
     </row>
-    <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="C74" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>55</v>
@@ -3395,7 +3425,9 @@
       <c r="F74" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="G74" s="27"/>
+      <c r="G74" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="H74" s="28"/>
     </row>
     <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3403,68 +3435,64 @@
         <v>163</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C75" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75" s="31" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G75" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="H75" s="49"/>
+        <v>55</v>
+      </c>
+      <c r="F75" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G75" s="27"/>
+      <c r="H75" s="28"/>
     </row>
     <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C76" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D76" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E76" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G76" s="27" t="s">
+      <c r="F76" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="H76" s="28"/>
+      <c r="G76" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="H76" s="49"/>
     </row>
     <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C77" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D77" s="31" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G77" s="27" t="s">
-        <v>189</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G77" s="27"/>
       <c r="H77" s="28"/>
     </row>
     <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3553,53 +3581,56 @@
         <v>200</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F81" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="G81" s="27" t="s">
         <v>201</v>
       </c>
       <c r="H81" s="28"/>
     </row>
-    <row r="82" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B82" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="C82" s="1" t="n">
-        <v>3</v>
+      <c r="C82" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="D82" s="31" t="s">
         <v>203</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="F82" s="3"/>
+      <c r="G82" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="G82" s="27" t="s">
-        <v>205</v>
-      </c>
       <c r="H82" s="28"/>
     </row>
-    <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B83" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D83" s="31" t="s">
         <v>206</v>
-      </c>
-      <c r="C83" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D83" s="31" t="s">
-        <v>207</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="F83" s="55" t="s">
+        <v>207</v>
       </c>
       <c r="G83" s="27" t="s">
         <v>208</v>
@@ -3614,16 +3645,13 @@
         <v>209</v>
       </c>
       <c r="C84" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D84" s="31" t="s">
         <v>210</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G84" s="27" t="s">
         <v>211</v>
@@ -3658,28 +3686,47 @@
       <c r="A86" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="C86" s="1" t="n">
+      <c r="C86" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D86" s="31" t="s">
         <v>216</v>
       </c>
+      <c r="E86" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="G86" s="27" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G87" s="27"/>
+      <c r="H86" s="28"/>
+    </row>
+    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D87" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="G87" s="27" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D88" s="31"/>
       <c r="G88" s="27"/>
     </row>
     <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="30"/>
       <c r="D89" s="31"/>
       <c r="G89" s="27"/>
     </row>
@@ -8498,7 +8545,11 @@
       <c r="D1052" s="31"/>
       <c r="G1052" s="27"/>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1053" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1053" s="30"/>
+      <c r="D1053" s="31"/>
+      <c r="G1053" s="27"/>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -8509,7 +8560,7 @@
     <mergeCell ref="E40:E42"/>
     <mergeCell ref="E43:E46"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:C6 B27:C27 B8:C17 B36:C37 B22:C22 B89:C1052 C86:C88 H48:H50 B44:C44 C2 A2:A3 A14:A17 A50 B49:C60 B66:C71 B85 B81:C84 B73:C77 A22:A28">
+  <conditionalFormatting sqref="B6:C6 B27:C27 B8:C17 B36:C37 B22:C22 B90:C1053 C87:C89 H48:H50 B44:C44 C2 A2:A3 A14:A17 A50 B49:C60 B66:C71 B86 B82:C85 B74:C78 A22:A28">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
@@ -8579,22 +8630,22 @@
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+  <conditionalFormatting sqref="C86">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B78:C78">
+  <conditionalFormatting sqref="B79:C79">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B79:C79">
+  <conditionalFormatting sqref="B80:C80">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B80:C80">
+  <conditionalFormatting sqref="B81:C81">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
@@ -8609,7 +8660,7 @@
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B72:C72">
+  <conditionalFormatting sqref="B72:C73">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
@@ -8692,32 +8743,35 @@
     <hyperlink ref="E70" r:id="rId55" display="Amazon link"/>
     <hyperlink ref="E71" r:id="rId56" display="MicroLab link"/>
     <hyperlink ref="F71" r:id="rId57" display="Github Link"/>
-    <hyperlink ref="E72" r:id="rId58" display="MicroLab link"/>
-    <hyperlink ref="F72" r:id="rId59" display="Github Link"/>
-    <hyperlink ref="E73" r:id="rId60" display="MicroLab link"/>
-    <hyperlink ref="F73" r:id="rId61" display="Github Link"/>
+    <hyperlink ref="G71" r:id="rId58" display="New Reactor Core files here"/>
+    <hyperlink ref="E72" r:id="rId59" display="MicroLab link"/>
+    <hyperlink ref="F72" r:id="rId60" display="Github Link"/>
+    <hyperlink ref="E73" r:id="rId61" display="Amazon Link"/>
     <hyperlink ref="E74" r:id="rId62" display="MicroLab link"/>
     <hyperlink ref="F74" r:id="rId63" display="Github Link"/>
-    <hyperlink ref="E75" r:id="rId64" display="Amazon 4oz link"/>
-    <hyperlink ref="F75" r:id="rId65" display="Amazon 6oz link"/>
-    <hyperlink ref="E76" r:id="rId66" display="Amazon link"/>
-    <hyperlink ref="E77" r:id="rId67" display="MicroLab link"/>
-    <hyperlink ref="F77" r:id="rId68" display="Github Link"/>
-    <hyperlink ref="E78" r:id="rId69" display="MicroLab link"/>
-    <hyperlink ref="F78" r:id="rId70" display="Github Link"/>
-    <hyperlink ref="E79" r:id="rId71" display="MicroLab link"/>
-    <hyperlink ref="F79" r:id="rId72" display="Github Link"/>
-    <hyperlink ref="E80" r:id="rId73" display="MicroLab link"/>
-    <hyperlink ref="F80" r:id="rId74" display="Github Link"/>
-    <hyperlink ref="E81" r:id="rId75" display="Ali Express link"/>
-    <hyperlink ref="G81" r:id="rId76" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
-    <hyperlink ref="E82" r:id="rId77" display="Amazon link"/>
-    <hyperlink ref="F82" r:id="rId78" display="Alibaba Link"/>
-    <hyperlink ref="E83" r:id="rId79" display="Amazon link"/>
-    <hyperlink ref="E84" r:id="rId80" display="MicroLab link"/>
-    <hyperlink ref="F84" r:id="rId81" display="Github Link"/>
-    <hyperlink ref="E85" r:id="rId82" display="MicroLab link"/>
-    <hyperlink ref="F85" r:id="rId83" display="Github Link"/>
+    <hyperlink ref="E75" r:id="rId64" display="MicroLab link"/>
+    <hyperlink ref="F75" r:id="rId65" display="Github Link"/>
+    <hyperlink ref="E76" r:id="rId66" display="Amazon 4oz link"/>
+    <hyperlink ref="F76" r:id="rId67" display="Amazon 6oz link"/>
+    <hyperlink ref="G76" r:id="rId68" display="a GL45 250ml bottle"/>
+    <hyperlink ref="E77" r:id="rId69" display="Amazon link"/>
+    <hyperlink ref="E78" r:id="rId70" display="MicroLab link"/>
+    <hyperlink ref="F78" r:id="rId71" display="Github Link"/>
+    <hyperlink ref="E79" r:id="rId72" display="MicroLab link"/>
+    <hyperlink ref="F79" r:id="rId73" display="Github Link"/>
+    <hyperlink ref="E80" r:id="rId74" display="MicroLab link"/>
+    <hyperlink ref="F80" r:id="rId75" display="Github Link"/>
+    <hyperlink ref="E81" r:id="rId76" display="MicroLab link"/>
+    <hyperlink ref="F81" r:id="rId77" display="Github Link"/>
+    <hyperlink ref="E82" r:id="rId78" display="Ali Express link"/>
+    <hyperlink ref="G82" r:id="rId79" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
+    <hyperlink ref="E83" r:id="rId80" display="Amazon link"/>
+    <hyperlink ref="F83" r:id="rId81" display="Alibaba Link"/>
+    <hyperlink ref="E84" r:id="rId82" display="Amazon link"/>
+    <hyperlink ref="E85" r:id="rId83" display="MicroLab link"/>
+    <hyperlink ref="F85" r:id="rId84" display="Github Link"/>
+    <hyperlink ref="E86" r:id="rId85" display="MicroLab link"/>
+    <hyperlink ref="F86" r:id="rId86" display="Github Link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8750,773 +8804,773 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C1" s="57" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="57" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D2" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="H2" s="52" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I2" s="59" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="57" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E3" s="60" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="I3" s="59" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="57" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F4" s="58" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="H4" s="61" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="I4" s="59" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="K4" s="59" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="57" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H5" s="52"/>
       <c r="I5" s="59" t="n">
         <v>7.36</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="57" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="59"/>
       <c r="J6" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="57" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>4</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="59" t="n">
         <v>9.99</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="57" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H8" s="52" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="I8" s="59" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="57" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D9" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="H9" s="52"/>
       <c r="I9" s="59"/>
     </row>
     <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="57" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D10" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="58" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F10" s="58" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="H10" s="52" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="I10" s="59" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="57" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D11" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H11" s="52" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="I11" s="59" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="57" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C12" s="57" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="58" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="52" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="I12" s="59" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="57" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B13" s="57" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C13" s="57" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="52" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="I13" s="59"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="57" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B14" s="57" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C14" s="57" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D14" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="H14" s="52"/>
       <c r="I14" s="59" t="n">
         <v>3.82</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="57" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D15" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H15" s="52" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="I15" s="59" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="57" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C16" s="57" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D16" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H16" s="52"/>
       <c r="I16" s="59" t="n">
         <v>10.91</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="57" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C17" s="57" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D17" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F17" s="6"/>
       <c r="H17" s="52" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I17" s="59" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="57" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D18" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H18" s="52" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="I18" s="59" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="57" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D19" s="6" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H19" s="52" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I19" s="59" t="n">
         <v>64.08</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="57" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D20" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H20" s="52"/>
       <c r="I20" s="59"/>
       <c r="J20" s="6" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="57" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C21" s="57" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D21" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H21" s="52"/>
       <c r="I21" s="59" t="n">
         <v>26.79</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="57" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D22" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="59"/>
       <c r="J22" s="6" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="57" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D23" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H23" s="52"/>
       <c r="I23" s="59"/>
       <c r="J23" s="6" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="57" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B24" s="57" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D24" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H24" s="52"/>
       <c r="I24" s="59"/>
       <c r="J24" s="6" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="57" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D25" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H25" s="52"/>
       <c r="I25" s="59"/>
       <c r="J25" s="6" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="57" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C26" s="57" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D26" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H26" s="52"/>
       <c r="I26" s="59"/>
       <c r="J26" s="6" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="57" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D27" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H27" s="52"/>
       <c r="I27" s="59"/>
       <c r="J27" s="6" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="57" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B28" s="57" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D28" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="H28" s="52"/>
       <c r="I28" s="59"/>
       <c r="J28" s="6" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="57" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B29" s="57" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="D29" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F29" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H29" s="52"/>
       <c r="I29" s="59" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K29" s="6" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="57" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B30" s="57" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H30" s="52" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="I30" s="59" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="57"/>
       <c r="B31" s="57" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="E31" s="62"/>
       <c r="H31" s="52"/>
@@ -9525,10 +9579,10 @@
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="57"/>
       <c r="B32" s="57" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="E32" s="62"/>
       <c r="H32" s="52"/>
@@ -9537,10 +9591,10 @@
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="57"/>
       <c r="B33" s="57" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="E33" s="62"/>
       <c r="H33" s="52"/>
@@ -9548,119 +9602,119 @@
     </row>
     <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="57" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C34" s="63" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D34" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="H34" s="52"/>
       <c r="I34" s="59" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="57" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B35" s="57" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C35" s="57" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="D35" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F35" s="58" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="H35" s="52"/>
       <c r="I35" s="59" t="n">
         <v>7.63</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="K35" s="6" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="57" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B36" s="57" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C36" s="57" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D36" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H36" s="52"/>
       <c r="I36" s="59"/>
       <c r="J36" s="6" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="57" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B37" s="57" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C37" s="57" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="D37" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E37" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H37" s="52" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="I37" s="59" t="n">
         <v>1.18</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="57" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B38" s="57"/>
       <c r="C38" s="57" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="D38" s="6" t="n">
         <v>1</v>
@@ -9670,69 +9724,69 @@
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="57" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B39" s="57" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="D39" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E39" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H39" s="52"/>
       <c r="I39" s="59" t="n">
         <v>9.35</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="57"/>
       <c r="B40" s="57" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="C40" s="57" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H40" s="52" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I40" s="59" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="57"/>
       <c r="B41" s="57" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="D41" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E41" s="58" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H41" s="52"/>
       <c r="I41" s="64" t="n">
         <v>8.99</v>
       </c>
       <c r="J41" s="65" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9746,7 +9800,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9754,32 +9808,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="6" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="6" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I46" s="59" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9787,24 +9841,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="65" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="J48" s="65" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="K48" s="65" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update parts list and reactor assembly
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="366">
   <si>
     <t xml:space="preserve">MicroLab Parts List</t>
   </si>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">4-wire cable, 18 gauge</t>
   </si>
   <si>
-    <t xml:space="preserve">[Control Unit] [Pumps Box] 10 feet will be used to make cables to connect the Control Unit and the Pumps unit. Some of the rest will be used to wire components within the Control Unit. </t>
+    <t xml:space="preserve">[Control Unit] [Pumps Box] 10 feet will be used to make cables to connect the Control Unit and the Pumps unit. Some of the rest will be used to wire components within the Control Unit. You can also use wires from ethernet cables.</t>
   </si>
   <si>
     <t xml:space="preserve">SP-RBW</t>
@@ -295,7 +295,7 @@
     <t xml:space="preserve">2-wire cable, red and Black , 18 gauge</t>
   </si>
   <si>
-    <t xml:space="preserve">We won't use all of it, you may want to get a smaller amount if you can find it cheaper. </t>
+    <t xml:space="preserve">Optional and we won't use all of it, you may want to get a smaller amount if you can find it cheaper. </t>
   </si>
   <si>
     <t xml:space="preserve">SP-SWW</t>
@@ -337,10 +337,10 @@
     <t xml:space="preserve">SP-M3S-12</t>
   </si>
   <si>
-    <t xml:space="preserve">12mm M3 screws with nuts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Reactor Unit]  3 for reactor unit and 20 for reactor stand</t>
+    <t xml:space="preserve">12mm M3 screws with nuts (Optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Reactor Unit] 20 for reactor stand (Optional)</t>
   </si>
   <si>
     <t xml:space="preserve">SP-M3S-16</t>
@@ -358,7 +358,7 @@
     <t xml:space="preserve">20mm M3 screws with nuts</t>
   </si>
   <si>
-    <t xml:space="preserve">[Control Unit] [Reactor]  2 for Control Unit, 3 for Reactor Unit</t>
+    <t xml:space="preserve">[Control Unit] [Reactor]  2 for Control Unit</t>
   </si>
   <si>
     <t xml:space="preserve">SP-M3S-30</t>
@@ -411,16 +411,10 @@
 NOTE: These will actually be installed in the Pumps Unit.</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-SBH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submersible heater</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC-CTB</t>
   </si>
   <si>
-    <t xml:space="preserve">Copper tubing 1/4" OD x 3/16" ID</t>
+    <t xml:space="preserve">Copper tubing 10’ ¼" OD x 3/16" ID</t>
   </si>
   <si>
     <t xml:space="preserve">Amazon link for raw copper tubing</t>
@@ -443,30 +437,6 @@
     <t xml:space="preserve">Silicone tubing should fit snugly around the copper tubing </t>
   </si>
   <si>
-    <t xml:space="preserve">TC-JAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32oz wide mouth canning jar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A 32oz wide mouth jar will contain the heating coils and the copper coils. Link is to a multi-pack but single jars are not easy to find and buying in bulk is often cheaper. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-REL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switchable power supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-INS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insulation for jars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Although you could use a knit hat or any other insulator for this, we find that upcycling the foil bubblewrap bags used for shipping cold things is a light and convenient way to insulate the jars</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC-TAP</t>
   </si>
   <si>
@@ -489,31 +459,13 @@
       </t>
   </si>
   <si>
-    <t xml:space="preserve">TC-CUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooling Unit Lid (Printed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lid for the  jar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-HUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heating Unit Lid (Printed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lid for the jar </t>
-  </si>
-  <si>
     <t xml:space="preserve">TC-LIQ</t>
   </si>
   <si>
-    <t xml:space="preserve">Liquid, water or other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We have been using water for this version, but other liquids may be more effective for the temperature control.</t>
+    <t xml:space="preserve">Liquid, propylene glycol, water, or other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have been using propylene glycol which support temperature ranges as high and as low as the MicroLab supports.</t>
   </si>
   <si>
     <t xml:space="preserve">REACTOR UNIT</t>
@@ -546,67 +498,22 @@
     <t xml:space="preserve">Stir rod coupler 4mm-to-5mm</t>
   </si>
   <si>
+    <t xml:space="preserve">RU-PTFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTFE Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU-RJF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jar Flanges (Printed)</t>
+  </si>
+  <si>
     <t xml:space="preserve">RU-COR</t>
   </si>
   <si>
-    <t xml:space="preserve">Old Reactor manifold core (Printed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE: New Reactor Core files here.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU-LID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Old Reactor manifold lid (Printed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE: This part is obsolete with the new Reactor Core design.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU-PTFE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTFE Sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Old Stir rod mount (Printed)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NOTE: This part is obsolete with the new Reactor Core design
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NOTE: the motor mount is under development and does not exactly fit the linked motor</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RU-RJF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jar Flanges (Printed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 oz regular mouth mason jar for core chamber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon 4oz link</t>
+    <t xml:space="preserve">250ml GL45 Borosilicate Glass Bottles</t>
   </si>
   <si>
     <t xml:space="preserve">Amazon 6oz link</t>
@@ -2056,8 +1963,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G73" activeCellId="0" sqref="G73"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2743,7 +2650,7 @@
       </c>
       <c r="H37" s="28"/>
     </row>
-    <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
@@ -2891,7 +2798,7 @@
         <v>109</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D45" s="31" t="s">
         <v>110</v>
@@ -3013,7 +2920,7 @@
       </c>
       <c r="H53" s="49"/>
     </row>
-    <row r="54" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>124</v>
       </c>
@@ -3021,65 +2928,62 @@
         <v>128</v>
       </c>
       <c r="C54" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" s="31" t="s">
         <v>129</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F54" s="48"/>
-      <c r="G54" s="27"/>
+        <v>130</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G54" s="27" t="s">
+        <v>132</v>
+      </c>
       <c r="H54" s="49"/>
     </row>
-    <row r="55" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C55" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>133</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F55" s="48"/>
       <c r="G55" s="27" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H55" s="49"/>
     </row>
-    <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F56" s="48"/>
-      <c r="G56" s="27" t="s">
         <v>137</v>
       </c>
+      <c r="F56" s="50"/>
+      <c r="G56" s="27"/>
       <c r="H56" s="49"/>
     </row>
-    <row r="57" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>124</v>
       </c>
@@ -3087,199 +2991,200 @@
         <v>138</v>
       </c>
       <c r="C57" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G57" s="27" t="s">
-        <v>140</v>
-      </c>
+      <c r="F57" s="51"/>
+      <c r="G57" s="27"/>
       <c r="H57" s="49"/>
     </row>
-    <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D58" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="G58" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G58" s="27"/>
-      <c r="H58" s="49"/>
-    </row>
-    <row r="59" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="59" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C59" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D59" s="31" t="s">
+      <c r="C59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F59" s="50"/>
-      <c r="G59" s="27" t="s">
+      <c r="F59" s="34"/>
+      <c r="G59" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="H59" s="49"/>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B60" s="30" t="s">
+      <c r="B60" s="30"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="31"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="28"/>
+    </row>
+    <row r="61" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C60" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D60" s="31" t="s">
+      <c r="B61" s="42"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="46"/>
+      <c r="AMJ61" s="6"/>
+    </row>
+    <row r="62" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F60" s="50"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="49"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B61" s="30" t="s">
+      <c r="B62" s="30" t="s">
         <v>148</v>
-      </c>
-      <c r="C61" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D61" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="E61" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F61" s="51"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="49"/>
-    </row>
-    <row r="62" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>150</v>
       </c>
       <c r="C62" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="H62" s="28"/>
+    </row>
+    <row r="63" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="G62" s="27" t="s">
+      <c r="C63" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" s="31" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="E63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="C63" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="H63" s="28"/>
+      <c r="H63" s="49"/>
     </row>
     <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B64" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G64" s="27"/>
+      <c r="H64" s="49"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="C64" s="1" t="n">
+      <c r="C65" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E65" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" s="34"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="28"/>
+    </row>
+    <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C66" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D66" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F64" s="34" t="s">
+      <c r="F66" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="G64" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F65" s="34"/>
-      <c r="G65" s="52" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="30"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="31"/>
       <c r="G66" s="27"/>
       <c r="H66" s="28"/>
     </row>
-    <row r="67" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="18" t="s">
+    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B67" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B67" s="42"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="53"/>
-      <c r="G67" s="45"/>
-      <c r="H67" s="46"/>
-      <c r="AMJ67" s="6"/>
-    </row>
-    <row r="68" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G67" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H67" s="49"/>
+    </row>
+    <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B68" s="30" t="s">
         <v>164</v>
@@ -3293,54 +3198,60 @@
       <c r="E68" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G68" s="54" t="s">
+      <c r="G68" s="27"/>
+      <c r="H68" s="28"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" s="30" t="s">
         <v>166</v>
-      </c>
-      <c r="H68" s="28"/>
-    </row>
-    <row r="69" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B69" s="30" t="s">
-        <v>167</v>
       </c>
       <c r="C69" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D69" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G69" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G69" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="H69" s="49"/>
+      <c r="H69" s="28"/>
     </row>
     <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C70" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D70" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G70" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G70" s="27"/>
-      <c r="H70" s="49"/>
+      <c r="H70" s="28"/>
     </row>
     <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B71" s="30" t="s">
         <v>172</v>
@@ -3354,17 +3265,17 @@
       <c r="E71" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F71" s="34" t="s">
+      <c r="F71" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G71" s="12" t="s">
+      <c r="G71" s="27" t="s">
         <v>174</v>
       </c>
       <c r="H71" s="28"/>
     </row>
     <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B72" s="30" t="s">
         <v>175</v>
@@ -3378,17 +3289,17 @@
       <c r="E72" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F72" s="34" t="s">
+      <c r="F72" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G72" s="12" t="s">
+      <c r="G72" s="27" t="s">
         <v>177</v>
       </c>
       <c r="H72" s="28"/>
     </row>
     <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B73" s="30" t="s">
         <v>178</v>
@@ -3400,333 +3311,173 @@
         <v>179</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F73" s="34"/>
-      <c r="G73" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="F73" s="3"/>
+      <c r="G73" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="H73" s="28"/>
     </row>
-    <row r="74" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="C74" s="4" t="n">
-        <v>1</v>
+        <v>181</v>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F74" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>181</v>
+        <v>14</v>
+      </c>
+      <c r="F74" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="G74" s="27" t="s">
+        <v>184</v>
       </c>
       <c r="H74" s="28"/>
     </row>
     <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C75" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D75" s="31" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F75" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G75" s="27"/>
+        <v>14</v>
+      </c>
+      <c r="G75" s="27" t="s">
+        <v>187</v>
+      </c>
       <c r="H75" s="28"/>
     </row>
     <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C76" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D76" s="31" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>185</v>
+        <v>55</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="H76" s="49"/>
+        <v>56</v>
+      </c>
+      <c r="G76" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="H76" s="28"/>
     </row>
     <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C77" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D77" s="31" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G77" s="27"/>
+        <v>55</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G77" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="H77" s="28"/>
     </row>
     <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B78" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="C78" s="4" t="n">
+        <v>147</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C78" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D78" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>56</v>
+        <v>195</v>
       </c>
       <c r="G78" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="H78" s="28"/>
-    </row>
-    <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B79" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="C79" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D79" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G79" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="H79" s="28"/>
-    </row>
-    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B80" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="C80" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D80" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G80" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="H80" s="28"/>
-    </row>
-    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B81" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="C81" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D81" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G81" s="27" t="s">
-        <v>201</v>
-      </c>
-      <c r="H81" s="28"/>
-    </row>
-    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B82" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="C82" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D82" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F82" s="3"/>
-      <c r="G82" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="H82" s="28"/>
-    </row>
-    <row r="83" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B83" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="C83" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D83" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F83" s="55" t="s">
-        <v>207</v>
-      </c>
-      <c r="G83" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="H83" s="28"/>
-    </row>
-    <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B84" s="30" t="s">
-        <v>209</v>
-      </c>
-      <c r="C84" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D84" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G84" s="27" t="s">
-        <v>211</v>
-      </c>
-      <c r="H84" s="28"/>
-    </row>
-    <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B85" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="C85" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D85" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G85" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="H85" s="28"/>
-    </row>
-    <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B86" s="30" t="s">
-        <v>215</v>
-      </c>
-      <c r="C86" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D86" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G86" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="H86" s="28"/>
-    </row>
-    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C87" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D87" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="G87" s="27" t="s">
-        <v>220</v>
-      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G79" s="27"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D80" s="31"/>
+      <c r="G80" s="27"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="30"/>
+      <c r="D81" s="31"/>
+      <c r="G81" s="27"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="30"/>
+      <c r="D82" s="31"/>
+      <c r="G82" s="27"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="30"/>
+      <c r="D83" s="31"/>
+      <c r="G83" s="27"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="30"/>
+      <c r="D84" s="31"/>
+      <c r="G84" s="27"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="30"/>
+      <c r="D85" s="31"/>
+      <c r="G85" s="27"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="30"/>
+      <c r="D86" s="31"/>
+      <c r="G86" s="27"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="30"/>
+      <c r="D87" s="31"/>
+      <c r="G87" s="27"/>
     </row>
     <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="30"/>
+      <c r="D88" s="31"/>
       <c r="G88" s="27"/>
     </row>
     <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="30"/>
       <c r="D89" s="31"/>
       <c r="G89" s="27"/>
     </row>
@@ -8505,51 +8256,15 @@
       <c r="D1044" s="31"/>
       <c r="G1044" s="27"/>
     </row>
-    <row r="1045" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1045" s="30"/>
-      <c r="D1045" s="31"/>
-      <c r="G1045" s="27"/>
-    </row>
-    <row r="1046" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1046" s="30"/>
-      <c r="D1046" s="31"/>
-      <c r="G1046" s="27"/>
-    </row>
-    <row r="1047" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1047" s="30"/>
-      <c r="D1047" s="31"/>
-      <c r="G1047" s="27"/>
-    </row>
-    <row r="1048" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1048" s="30"/>
-      <c r="D1048" s="31"/>
-      <c r="G1048" s="27"/>
-    </row>
-    <row r="1049" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1049" s="30"/>
-      <c r="D1049" s="31"/>
-      <c r="G1049" s="27"/>
-    </row>
-    <row r="1050" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1050" s="30"/>
-      <c r="D1050" s="31"/>
-      <c r="G1050" s="27"/>
-    </row>
-    <row r="1051" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1051" s="30"/>
-      <c r="D1051" s="31"/>
-      <c r="G1051" s="27"/>
-    </row>
-    <row r="1052" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1052" s="30"/>
-      <c r="D1052" s="31"/>
-      <c r="G1052" s="27"/>
-    </row>
-    <row r="1053" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1053" s="30"/>
-      <c r="D1053" s="31"/>
-      <c r="G1053" s="27"/>
-    </row>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -8560,7 +8275,7 @@
     <mergeCell ref="E40:E42"/>
     <mergeCell ref="E43:E46"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:C6 B27:C27 B8:C17 B36:C37 B22:C22 B90:C1053 C87:C89 H48:H50 B44:C44 C2 A2:A3 A14:A17 A50 B49:C60 B66:C71 B86 B82:C85 B74:C78 A22:A28">
+  <conditionalFormatting sqref="B6:C6 B27:C27 B8:C17 B36:C37 B22:C22 B81:C1044 C78:C80 H48:H50 B44:C44 C2 A2:A3 A14:A17 A50 B49:C56 B60:C64 B77 B73:C76 B66:C69 A22:A28">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
@@ -8630,37 +8345,37 @@
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C86">
+  <conditionalFormatting sqref="C77">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B79:C79">
+  <conditionalFormatting sqref="B70:C70">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B80:C80">
+  <conditionalFormatting sqref="B71:C71">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B81:C81">
+  <conditionalFormatting sqref="B72:C72">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61:C61">
+  <conditionalFormatting sqref="B57:C57">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62:C62">
+  <conditionalFormatting sqref="B58:C58">
     <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B72:C73">
+  <conditionalFormatting sqref="B65:C65">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>LEN(TRIM(#ref!))&gt;0</formula>
     </cfRule>
@@ -8726,52 +8441,37 @@
     <hyperlink ref="F47" r:id="rId38" display="Amazon link"/>
     <hyperlink ref="E48" r:id="rId39" display="Amazon link"/>
     <hyperlink ref="E53" r:id="rId40" display="Amazon link"/>
-    <hyperlink ref="E54" r:id="rId41" display="Amazon link"/>
-    <hyperlink ref="E55" r:id="rId42" display="Amazon link for raw copper tubing"/>
-    <hyperlink ref="F55" r:id="rId43" display="Amazon link for aluminum cooler"/>
-    <hyperlink ref="E56" r:id="rId44" display="Amazon link"/>
-    <hyperlink ref="E57" r:id="rId45" display="Amazon link"/>
-    <hyperlink ref="E58" r:id="rId46" display="Amazon link"/>
-    <hyperlink ref="E61" r:id="rId47" display="Amazon link"/>
-    <hyperlink ref="E63" r:id="rId48" display="MicroLab link"/>
-    <hyperlink ref="F63" r:id="rId49" display="Github Link"/>
-    <hyperlink ref="E64" r:id="rId50" display="MicroLab link"/>
-    <hyperlink ref="F64" r:id="rId51" display="Github Link"/>
-    <hyperlink ref="E68" r:id="rId52" display="Amazon link"/>
-    <hyperlink ref="G68" r:id="rId53" display="Amazon link  This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E69" r:id="rId54" display="Amazon link"/>
-    <hyperlink ref="E70" r:id="rId55" display="Amazon link"/>
-    <hyperlink ref="E71" r:id="rId56" display="MicroLab link"/>
-    <hyperlink ref="F71" r:id="rId57" display="Github Link"/>
-    <hyperlink ref="G71" r:id="rId58" display="New Reactor Core files here"/>
-    <hyperlink ref="E72" r:id="rId59" display="MicroLab link"/>
-    <hyperlink ref="F72" r:id="rId60" display="Github Link"/>
-    <hyperlink ref="E73" r:id="rId61" display="Amazon Link"/>
-    <hyperlink ref="E74" r:id="rId62" display="MicroLab link"/>
-    <hyperlink ref="F74" r:id="rId63" display="Github Link"/>
-    <hyperlink ref="E75" r:id="rId64" display="MicroLab link"/>
-    <hyperlink ref="F75" r:id="rId65" display="Github Link"/>
-    <hyperlink ref="E76" r:id="rId66" display="Amazon 4oz link"/>
-    <hyperlink ref="F76" r:id="rId67" display="Amazon 6oz link"/>
-    <hyperlink ref="G76" r:id="rId68" display="a GL45 250ml bottle"/>
-    <hyperlink ref="E77" r:id="rId69" display="Amazon link"/>
-    <hyperlink ref="E78" r:id="rId70" display="MicroLab link"/>
-    <hyperlink ref="F78" r:id="rId71" display="Github Link"/>
-    <hyperlink ref="E79" r:id="rId72" display="MicroLab link"/>
-    <hyperlink ref="F79" r:id="rId73" display="Github Link"/>
-    <hyperlink ref="E80" r:id="rId74" display="MicroLab link"/>
-    <hyperlink ref="F80" r:id="rId75" display="Github Link"/>
-    <hyperlink ref="E81" r:id="rId76" display="MicroLab link"/>
-    <hyperlink ref="F81" r:id="rId77" display="Github Link"/>
-    <hyperlink ref="E82" r:id="rId78" display="Ali Express link"/>
-    <hyperlink ref="G82" r:id="rId79" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
-    <hyperlink ref="E83" r:id="rId80" display="Amazon link"/>
-    <hyperlink ref="F83" r:id="rId81" display="Alibaba Link"/>
-    <hyperlink ref="E84" r:id="rId82" display="Amazon link"/>
-    <hyperlink ref="E85" r:id="rId83" display="MicroLab link"/>
-    <hyperlink ref="F85" r:id="rId84" display="Github Link"/>
-    <hyperlink ref="E86" r:id="rId85" display="MicroLab link"/>
-    <hyperlink ref="F86" r:id="rId86" display="Github Link"/>
+    <hyperlink ref="E54" r:id="rId41" display="Amazon link for raw copper tubing"/>
+    <hyperlink ref="F54" r:id="rId42" display="Amazon link for aluminum cooler"/>
+    <hyperlink ref="E55" r:id="rId43" display="Amazon link"/>
+    <hyperlink ref="E57" r:id="rId44" display="Amazon link"/>
+    <hyperlink ref="E62" r:id="rId45" display="Amazon link"/>
+    <hyperlink ref="G62" r:id="rId46" display="Amazon link  This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
+    <hyperlink ref="E63" r:id="rId47" display="Amazon link"/>
+    <hyperlink ref="E64" r:id="rId48" display="Amazon link"/>
+    <hyperlink ref="E65" r:id="rId49" display="Amazon Link"/>
+    <hyperlink ref="E66" r:id="rId50" display="MicroLab link"/>
+    <hyperlink ref="F66" r:id="rId51" display="Github Link"/>
+    <hyperlink ref="F67" r:id="rId52" display="Amazon 6oz link"/>
+    <hyperlink ref="G67" r:id="rId53" display="NOTE: New Reactor Core uses a GL45 250ml bottle instead!"/>
+    <hyperlink ref="E68" r:id="rId54" display="Amazon link"/>
+    <hyperlink ref="E69" r:id="rId55" display="MicroLab link"/>
+    <hyperlink ref="F69" r:id="rId56" display="Github Link"/>
+    <hyperlink ref="E70" r:id="rId57" display="MicroLab link"/>
+    <hyperlink ref="F70" r:id="rId58" display="Github Link"/>
+    <hyperlink ref="E71" r:id="rId59" display="MicroLab link"/>
+    <hyperlink ref="F71" r:id="rId60" display="Github Link"/>
+    <hyperlink ref="E72" r:id="rId61" display="MicroLab link"/>
+    <hyperlink ref="F72" r:id="rId62" display="Github Link"/>
+    <hyperlink ref="E73" r:id="rId63" display="Ali Express link"/>
+    <hyperlink ref="G73" r:id="rId64" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
+    <hyperlink ref="E74" r:id="rId65" display="Amazon link"/>
+    <hyperlink ref="F74" r:id="rId66" display="Alibaba Link"/>
+    <hyperlink ref="E75" r:id="rId67" display="Amazon link"/>
+    <hyperlink ref="E76" r:id="rId68" display="MicroLab link"/>
+    <hyperlink ref="F76" r:id="rId69" display="Github Link"/>
+    <hyperlink ref="E77" r:id="rId70" display="MicroLab link"/>
+    <hyperlink ref="F77" r:id="rId71" display="Github Link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8804,773 +8504,773 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="C1" s="57" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="57" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="D2" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="H2" s="52" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="I2" s="59" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="57" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="E3" s="60" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="I3" s="59" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="57" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="F4" s="58" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="H4" s="61" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="I4" s="59" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="K4" s="59" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="57" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H5" s="52"/>
       <c r="I5" s="59" t="n">
         <v>7.36</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="57" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="59"/>
       <c r="J6" s="6" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="57" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>4</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="59" t="n">
         <v>9.99</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="57" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H8" s="52" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="I8" s="59" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="57" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="D9" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="H9" s="52"/>
       <c r="I9" s="59"/>
     </row>
     <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="57" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="D10" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="58" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="F10" s="58" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="H10" s="52" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="I10" s="59" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="57" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="D11" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H11" s="52" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="I11" s="59" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="57" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="C12" s="57" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="58" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="52" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="I12" s="59" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="57" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="B13" s="57" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="C13" s="57" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="52" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="I13" s="59"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="57" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="B14" s="57" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="C14" s="57" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="D14" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="H14" s="52"/>
       <c r="I14" s="59" t="n">
         <v>3.82</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="57" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="D15" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H15" s="52" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="I15" s="59" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="57" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="C16" s="57" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="D16" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H16" s="52"/>
       <c r="I16" s="59" t="n">
         <v>10.91</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="57" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="C17" s="57" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="D17" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="F17" s="6"/>
       <c r="H17" s="52" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="I17" s="59" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="57" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="D18" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H18" s="52" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="I18" s="59" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="57" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="D19" s="6" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H19" s="52" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="I19" s="59" t="n">
         <v>64.08</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="57" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="D20" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H20" s="52"/>
       <c r="I20" s="59"/>
       <c r="J20" s="6" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="57" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="C21" s="57" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="D21" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H21" s="52"/>
       <c r="I21" s="59" t="n">
         <v>26.79</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="57" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="D22" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="59"/>
       <c r="J22" s="6" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="57" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="D23" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H23" s="52"/>
       <c r="I23" s="59"/>
       <c r="J23" s="6" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="57" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="B24" s="57" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="D24" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H24" s="52"/>
       <c r="I24" s="59"/>
       <c r="J24" s="6" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="57" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="D25" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H25" s="52"/>
       <c r="I25" s="59"/>
       <c r="J25" s="6" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="57" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="C26" s="57" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="D26" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H26" s="52"/>
       <c r="I26" s="59"/>
       <c r="J26" s="6" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="57" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="D27" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H27" s="52"/>
       <c r="I27" s="59"/>
       <c r="J27" s="6" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="57" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="B28" s="57" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="D28" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="H28" s="52"/>
       <c r="I28" s="59"/>
       <c r="J28" s="6" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="57" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="B29" s="57" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="D29" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="F29" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="H29" s="52"/>
       <c r="I29" s="59" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="K29" s="6" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="57" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="B30" s="57" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H30" s="52" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="I30" s="59" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="57"/>
       <c r="B31" s="57" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="E31" s="62"/>
       <c r="H31" s="52"/>
@@ -9579,10 +9279,10 @@
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="57"/>
       <c r="B32" s="57" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="E32" s="62"/>
       <c r="H32" s="52"/>
@@ -9591,10 +9291,10 @@
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="57"/>
       <c r="B33" s="57" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="E33" s="62"/>
       <c r="H33" s="52"/>
@@ -9602,119 +9302,119 @@
     </row>
     <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="57" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="C34" s="63" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="D34" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="H34" s="52"/>
       <c r="I34" s="59" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="57" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="B35" s="57" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="C35" s="57" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="D35" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="F35" s="58" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="H35" s="52"/>
       <c r="I35" s="59" t="n">
         <v>7.63</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="K35" s="6" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="57" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="B36" s="57" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="C36" s="57" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="D36" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H36" s="52"/>
       <c r="I36" s="59"/>
       <c r="J36" s="6" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="57" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="B37" s="57" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="C37" s="57" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="D37" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E37" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H37" s="52" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="I37" s="59" t="n">
         <v>1.18</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="57" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="B38" s="57"/>
       <c r="C38" s="57" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="D38" s="6" t="n">
         <v>1</v>
@@ -9724,69 +9424,69 @@
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="57" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="B39" s="57" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="D39" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E39" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H39" s="52"/>
       <c r="I39" s="59" t="n">
         <v>9.35</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="57"/>
       <c r="B40" s="57" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="C40" s="57" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H40" s="52" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="I40" s="59" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="57"/>
       <c r="B41" s="57" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="D41" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E41" s="58" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H41" s="52"/>
       <c r="I41" s="64" t="n">
         <v>8.99</v>
       </c>
       <c r="J41" s="65" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9800,7 +9500,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9808,32 +9508,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="6" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="6" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="I46" s="59" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9841,24 +9541,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="65" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="J48" s="65" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="K48" s="65" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
docs: photos and docs update
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="366">
   <si>
     <t xml:space="preserve">MicroLab Parts List</t>
   </si>
@@ -295,7 +295,7 @@
     <t xml:space="preserve">2-wire cable, red and Black , 18 gauge</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional and we won't use all of it, you may want to get a smaller amount if you can find it cheaper. </t>
+    <t xml:space="preserve">Optional and we won't use all of it, you may want to get a smaller amount if you can find it cheaper. Or just use ethernet cable.</t>
   </si>
   <si>
     <t xml:space="preserve">SP-SWW</t>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t xml:space="preserve">12-pin connector, panel-mount screw terminal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ali Express  link</t>
   </si>
   <si>
     <t xml:space="preserve">[Control Unit] [Pumps Box]  connector has three pieces: plug, mount plate and socket</t>
@@ -514,9 +517,6 @@
   </si>
   <si>
     <t xml:space="preserve">250ml GL45 Borosilicate Glass Bottles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon 6oz link</t>
   </si>
   <si>
     <t xml:space="preserve">NOTE: New Reactor Core uses a GL45 250ml bottle instead!</t>
@@ -1963,8 +1963,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2705,10 +2705,10 @@
         <v>95</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H40" s="28"/>
     </row>
@@ -2717,17 +2717,17 @@
         <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C41" s="36" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E41" s="37"/>
       <c r="G41" s="27" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H41" s="28"/>
     </row>
@@ -2736,17 +2736,17 @@
         <v>82</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E42" s="37"/>
       <c r="G42" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H42" s="28"/>
     </row>
@@ -2755,19 +2755,19 @@
         <v>82</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>23</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E43" s="34" t="s">
         <v>44</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H43" s="28"/>
     </row>
@@ -2776,17 +2776,17 @@
         <v>82</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>28</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E44" s="34"/>
       <c r="G44" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H44" s="28"/>
     </row>
@@ -2795,17 +2795,17 @@
         <v>82</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E45" s="34"/>
       <c r="G45" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H45" s="28"/>
     </row>
@@ -2814,17 +2814,17 @@
         <v>82</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E46" s="34"/>
       <c r="G46" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H46" s="28"/>
     </row>
@@ -2833,22 +2833,20 @@
         <v>82</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E47" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="F47" s="39" t="s">
-        <v>14</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F47" s="39"/>
       <c r="G47" s="40" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2856,19 +2854,19 @@
         <v>82</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E48" s="33" t="s">
         <v>14</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H48" s="41"/>
     </row>
@@ -2887,7 +2885,7 @@
     </row>
     <row r="52" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="43"/>
@@ -2900,84 +2898,84 @@
     </row>
     <row r="53" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F53" s="48"/>
       <c r="G53" s="27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H53" s="49"/>
     </row>
     <row r="54" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C54" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H54" s="49"/>
     </row>
     <row r="55" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F55" s="48"/>
       <c r="G55" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H55" s="49"/>
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F56" s="50"/>
       <c r="G56" s="27"/>
@@ -2985,16 +2983,16 @@
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E57" s="34" t="s">
         <v>14</v>
@@ -3005,37 +3003,37 @@
     </row>
     <row r="58" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G58" s="27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F59" s="34"/>
       <c r="G59" s="52" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3047,7 +3045,7 @@
     </row>
     <row r="61" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="43"/>
@@ -3060,58 +3058,58 @@
     </row>
     <row r="62" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C62" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G62" s="54" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H62" s="28"/>
     </row>
     <row r="63" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C63" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G63" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H63" s="49"/>
     </row>
     <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C64" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>14</v>
@@ -3121,16 +3119,16 @@
     </row>
     <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C65" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>25</v>
@@ -3141,16 +3139,16 @@
     </row>
     <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C66" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>55</v>
@@ -3163,19 +3161,19 @@
     </row>
     <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>162</v>
+        <v>14</v>
       </c>
       <c r="G67" s="12" t="s">
         <v>163</v>
@@ -3184,7 +3182,7 @@
     </row>
     <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B68" s="30" t="s">
         <v>164</v>
@@ -3203,7 +3201,7 @@
     </row>
     <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B69" s="30" t="s">
         <v>166</v>
@@ -3227,7 +3225,7 @@
     </row>
     <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B70" s="30" t="s">
         <v>169</v>
@@ -3251,7 +3249,7 @@
     </row>
     <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="30" t="s">
         <v>172</v>
@@ -3275,7 +3273,7 @@
     </row>
     <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B72" s="30" t="s">
         <v>175</v>
@@ -3299,7 +3297,7 @@
     </row>
     <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B73" s="30" t="s">
         <v>178</v>
@@ -3321,7 +3319,7 @@
     </row>
     <row r="74" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B74" s="30" t="s">
         <v>181</v>
@@ -3345,7 +3343,7 @@
     </row>
     <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B75" s="30" t="s">
         <v>185</v>
@@ -3366,7 +3364,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B76" s="30" t="s">
         <v>188</v>
@@ -3390,7 +3388,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B77" s="30" t="s">
         <v>191</v>
@@ -3414,7 +3412,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>194</v>
@@ -8436,42 +8434,41 @@
     <hyperlink ref="E37" r:id="rId33" display="Amazon link"/>
     <hyperlink ref="E38" r:id="rId34" display="Amazon link"/>
     <hyperlink ref="E39" r:id="rId35" display="Amazon link"/>
-    <hyperlink ref="E40" r:id="rId36" display="Amazon link"/>
+    <hyperlink ref="E40" r:id="rId36" display="Ali Express  link"/>
     <hyperlink ref="E43" r:id="rId37" display="Amazon link - assortment"/>
-    <hyperlink ref="F47" r:id="rId38" display="Amazon link"/>
-    <hyperlink ref="E48" r:id="rId39" display="Amazon link"/>
-    <hyperlink ref="E53" r:id="rId40" display="Amazon link"/>
-    <hyperlink ref="E54" r:id="rId41" display="Amazon link for raw copper tubing"/>
-    <hyperlink ref="F54" r:id="rId42" display="Amazon link for aluminum cooler"/>
-    <hyperlink ref="E55" r:id="rId43" display="Amazon link"/>
-    <hyperlink ref="E57" r:id="rId44" display="Amazon link"/>
-    <hyperlink ref="E62" r:id="rId45" display="Amazon link"/>
-    <hyperlink ref="G62" r:id="rId46" display="Amazon link  This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E63" r:id="rId47" display="Amazon link"/>
-    <hyperlink ref="E64" r:id="rId48" display="Amazon link"/>
-    <hyperlink ref="E65" r:id="rId49" display="Amazon Link"/>
-    <hyperlink ref="E66" r:id="rId50" display="MicroLab link"/>
-    <hyperlink ref="F66" r:id="rId51" display="Github Link"/>
-    <hyperlink ref="F67" r:id="rId52" display="Amazon 6oz link"/>
-    <hyperlink ref="G67" r:id="rId53" display="NOTE: New Reactor Core uses a GL45 250ml bottle instead!"/>
-    <hyperlink ref="E68" r:id="rId54" display="Amazon link"/>
-    <hyperlink ref="E69" r:id="rId55" display="MicroLab link"/>
-    <hyperlink ref="F69" r:id="rId56" display="Github Link"/>
-    <hyperlink ref="E70" r:id="rId57" display="MicroLab link"/>
-    <hyperlink ref="F70" r:id="rId58" display="Github Link"/>
-    <hyperlink ref="E71" r:id="rId59" display="MicroLab link"/>
-    <hyperlink ref="F71" r:id="rId60" display="Github Link"/>
-    <hyperlink ref="E72" r:id="rId61" display="MicroLab link"/>
-    <hyperlink ref="F72" r:id="rId62" display="Github Link"/>
-    <hyperlink ref="E73" r:id="rId63" display="Ali Express link"/>
-    <hyperlink ref="G73" r:id="rId64" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
-    <hyperlink ref="E74" r:id="rId65" display="Amazon link"/>
-    <hyperlink ref="F74" r:id="rId66" display="Alibaba Link"/>
-    <hyperlink ref="E75" r:id="rId67" display="Amazon link"/>
-    <hyperlink ref="E76" r:id="rId68" display="MicroLab link"/>
-    <hyperlink ref="F76" r:id="rId69" display="Github Link"/>
-    <hyperlink ref="E77" r:id="rId70" display="MicroLab link"/>
-    <hyperlink ref="F77" r:id="rId71" display="Github Link"/>
+    <hyperlink ref="E48" r:id="rId38" display="Amazon link"/>
+    <hyperlink ref="E53" r:id="rId39" display="Amazon link"/>
+    <hyperlink ref="E54" r:id="rId40" display="Amazon link for raw copper tubing"/>
+    <hyperlink ref="F54" r:id="rId41" display="Amazon link for aluminum cooler"/>
+    <hyperlink ref="E55" r:id="rId42" display="Amazon link"/>
+    <hyperlink ref="E57" r:id="rId43" display="Amazon link"/>
+    <hyperlink ref="E62" r:id="rId44" display="Amazon link"/>
+    <hyperlink ref="G62" r:id="rId45" display="Amazon link  This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
+    <hyperlink ref="E63" r:id="rId46" display="Amazon link"/>
+    <hyperlink ref="E64" r:id="rId47" display="Amazon link"/>
+    <hyperlink ref="E65" r:id="rId48" display="Amazon Link"/>
+    <hyperlink ref="E66" r:id="rId49" display="MicroLab link"/>
+    <hyperlink ref="F66" r:id="rId50" display="Github Link"/>
+    <hyperlink ref="F67" r:id="rId51" display="Amazon link"/>
+    <hyperlink ref="G67" r:id="rId52" display="NOTE: New Reactor Core uses a GL45 250ml bottle instead!"/>
+    <hyperlink ref="E68" r:id="rId53" display="Amazon link"/>
+    <hyperlink ref="E69" r:id="rId54" display="MicroLab link"/>
+    <hyperlink ref="F69" r:id="rId55" display="Github Link"/>
+    <hyperlink ref="E70" r:id="rId56" display="MicroLab link"/>
+    <hyperlink ref="F70" r:id="rId57" display="Github Link"/>
+    <hyperlink ref="E71" r:id="rId58" display="MicroLab link"/>
+    <hyperlink ref="F71" r:id="rId59" display="Github Link"/>
+    <hyperlink ref="E72" r:id="rId60" display="MicroLab link"/>
+    <hyperlink ref="F72" r:id="rId61" display="Github Link"/>
+    <hyperlink ref="E73" r:id="rId62" display="Ali Express link"/>
+    <hyperlink ref="G73" r:id="rId63" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
+    <hyperlink ref="E74" r:id="rId64" display="Amazon link"/>
+    <hyperlink ref="F74" r:id="rId65" display="Alibaba Link"/>
+    <hyperlink ref="E75" r:id="rId66" display="Amazon link"/>
+    <hyperlink ref="E76" r:id="rId67" display="MicroLab link"/>
+    <hyperlink ref="F76" r:id="rId68" display="Github Link"/>
+    <hyperlink ref="E77" r:id="rId69" display="MicroLab link"/>
+    <hyperlink ref="F77" r:id="rId70" display="Github Link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Update screen docs and stirring gif
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -81,7 +81,8 @@
     <t xml:space="preserve">Touchscreen for Raspberry Pi</t>
   </si>
   <si>
-    <t xml:space="preserve">Touchscreen for Raspberry Pi (CU-RPI). </t>
+    <t xml:space="preserve">Touchscreen for Raspberry Pi (CU-RPI). 
+Minimum recommended screen resolution is 640 x 480.</t>
   </si>
   <si>
     <t xml:space="preserve">CU-SD32</t>
@@ -1963,8 +1964,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2105,7 +2106,7 @@
       </c>
       <c r="H10" s="28"/>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Move parts list to parts-list.md
</commit_message>
<xml_diff>
--- a/docs/microlab-parts-list.xlsx
+++ b/docs/microlab-parts-list.xlsx
@@ -21,9 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="367">
   <si>
     <t xml:space="preserve">MicroLab Parts List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE 0: THIS PARTS LIST IS DEPRECATED. DO NOT UPDATE IT. DO NOT USE IT. USE AND UPDATE THE parts-list.md FILE INSTEAD. THIS FILE IS TO KEEP LINKS ALIVE ONLY.</t>
   </si>
   <si>
     <t xml:space="preserve">NOTE 1: We link to places that have the parts that we used. They aren't picked for best price or universal availability</t>
@@ -1363,7 +1366,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1390,12 +1393,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1964,8 +1967,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1988,7 +1991,9 @@
       </c>
     </row>
     <row r="2" s="13" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8"/>
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -1999,7 +2004,7 @@
     </row>
     <row r="3" s="13" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -2010,19 +2015,19 @@
       <c r="AMJ3" s="6"/>
     </row>
     <row r="4" s="13" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>2</v>
+      <c r="A4" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
       <c r="AMJ4" s="6"/>
     </row>
     <row r="5" s="13" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="1"/>
@@ -2032,25 +2037,25 @@
     </row>
     <row r="6" s="22" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AMJ6" s="6"/>
     </row>
@@ -2062,7 +2067,7 @@
     </row>
     <row r="8" s="13" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="1"/>
@@ -2072,7 +2077,7 @@
     </row>
     <row r="9" s="22" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="17"/>
@@ -2084,171 +2089,171 @@
     </row>
     <row r="10" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H10" s="28"/>
     </row>
     <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H11" s="28"/>
     </row>
     <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H12" s="28"/>
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H14" s="28"/>
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H15" s="28"/>
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H16" s="28"/>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="3"/>
@@ -2257,19 +2262,19 @@
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="27"/>
@@ -2277,271 +2282,271 @@
     </row>
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H19" s="28"/>
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="27" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H20" s="28"/>
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G21" s="35"/>
     </row>
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H22" s="28"/>
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H23" s="28"/>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H24" s="28"/>
     </row>
     <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H26" s="28"/>
     </row>
     <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H27" s="28"/>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H28" s="28"/>
     </row>
     <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H29" s="28"/>
     </row>
     <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E30" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30" s="35"/>
@@ -2549,19 +2554,19 @@
     </row>
     <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="35"/>
@@ -2569,19 +2574,19 @@
     </row>
     <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F32" s="33"/>
       <c r="G32" s="35"/>
@@ -2589,19 +2594,19 @@
     </row>
     <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="35"/>
@@ -2620,7 +2625,7 @@
     </row>
     <row r="36" s="22" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="17"/>
@@ -2632,242 +2637,242 @@
     </row>
     <row r="37" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H37" s="28"/>
     </row>
     <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H38" s="28"/>
     </row>
     <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C40" s="36" t="n">
         <v>2</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H40" s="28"/>
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C41" s="36" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E41" s="37"/>
       <c r="G41" s="27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H41" s="28"/>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E42" s="37"/>
       <c r="G42" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H42" s="28"/>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>23</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E43" s="34" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H43" s="28"/>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>28</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E44" s="34"/>
       <c r="G44" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H44" s="28"/>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E45" s="34"/>
       <c r="G45" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H45" s="28"/>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E46" s="34"/>
       <c r="G46" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H46" s="28"/>
     </row>
     <row r="47" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E47" s="38" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F47" s="39"/>
       <c r="G47" s="40" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H48" s="41"/>
     </row>
@@ -2886,7 +2891,7 @@
     </row>
     <row r="52" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="43"/>
@@ -2899,84 +2904,84 @@
     </row>
     <row r="53" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F53" s="48"/>
       <c r="G53" s="27" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H53" s="49"/>
     </row>
     <row r="54" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C54" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H54" s="49"/>
     </row>
     <row r="55" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F55" s="48"/>
       <c r="G55" s="27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H55" s="49"/>
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F56" s="50"/>
       <c r="G56" s="27"/>
@@ -2984,19 +2989,19 @@
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E57" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F57" s="51"/>
       <c r="G57" s="27"/>
@@ -3004,37 +3009,37 @@
     </row>
     <row r="58" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G58" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F59" s="34"/>
       <c r="G59" s="52" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3046,7 +3051,7 @@
     </row>
     <row r="61" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="43"/>
@@ -3059,80 +3064,80 @@
     </row>
     <row r="62" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C62" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G62" s="54" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H62" s="28"/>
     </row>
     <row r="63" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C63" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G63" s="27" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H63" s="49"/>
     </row>
     <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C64" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G64" s="27"/>
       <c r="H64" s="49"/>
     </row>
     <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C65" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F65" s="34"/>
       <c r="G65" s="12"/>
@@ -3140,292 +3145,292 @@
     </row>
     <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C66" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F66" s="34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G66" s="27"/>
       <c r="H66" s="28"/>
     </row>
     <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H67" s="49"/>
     </row>
     <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G68" s="27"/>
       <c r="H68" s="28"/>
     </row>
     <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C69" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G69" s="27" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H69" s="28"/>
     </row>
     <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C70" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G70" s="27" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H70" s="28"/>
     </row>
     <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C71" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G71" s="27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H71" s="28"/>
     </row>
     <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C72" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G72" s="27" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H72" s="28"/>
     </row>
     <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C73" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="27" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H73" s="28"/>
     </row>
     <row r="74" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F74" s="55" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G74" s="27" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H74" s="28"/>
     </row>
     <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C75" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D75" s="31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G75" s="27" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H75" s="28"/>
     </row>
     <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C76" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D76" s="31" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G76" s="27" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H76" s="28"/>
     </row>
     <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C77" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D77" s="31" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G77" s="27" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H77" s="28"/>
     </row>
     <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D78" s="31" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G78" s="27" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8400,76 +8405,77 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" display="Amazon link"/>
-    <hyperlink ref="F10" r:id="rId2" display="Amazon Le Potato link2"/>
-    <hyperlink ref="E11" r:id="rId3" display="Amazon link"/>
-    <hyperlink ref="E12" r:id="rId4" display="Amazon link"/>
-    <hyperlink ref="E13" r:id="rId5" display="Amazon Link"/>
-    <hyperlink ref="E14" r:id="rId6" display="Ali Express link (kit)&#10;- be sure to pick option with UNO board"/>
-    <hyperlink ref="F14" r:id="rId7" display="Amazon link"/>
-    <hyperlink ref="F15" r:id="rId8" display="Amazon Link (Kit)"/>
-    <hyperlink ref="F16" r:id="rId9" display="Amazon Link"/>
-    <hyperlink ref="E18" r:id="rId10" display="Amazon link"/>
-    <hyperlink ref="E19" r:id="rId11" display="Ali Express link"/>
-    <hyperlink ref="F19" r:id="rId12" display="Amazon link - assortment"/>
-    <hyperlink ref="E20" r:id="rId13" display="Amazon link"/>
-    <hyperlink ref="E21" r:id="rId14" display="Amazon link"/>
-    <hyperlink ref="E22" r:id="rId15" display="Amazon link"/>
-    <hyperlink ref="E23" r:id="rId16" display="MicroLab link"/>
-    <hyperlink ref="F23" r:id="rId17" display="Github Link"/>
-    <hyperlink ref="E24" r:id="rId18" display="MicroLab link"/>
-    <hyperlink ref="F24" r:id="rId19" display="Github Link"/>
-    <hyperlink ref="E25" r:id="rId20" display="MicroLab link"/>
-    <hyperlink ref="F25" r:id="rId21" display="Github Link"/>
-    <hyperlink ref="E26" r:id="rId22" display="MicroLab link"/>
-    <hyperlink ref="F26" r:id="rId23" display="Github Link"/>
-    <hyperlink ref="E27" r:id="rId24" display="Amazon link"/>
-    <hyperlink ref="E28" r:id="rId25" display="Ali Express Link"/>
-    <hyperlink ref="F28" r:id="rId26" display="Amazon Link"/>
-    <hyperlink ref="E29" r:id="rId27" display="Amazon link"/>
-    <hyperlink ref="F29" r:id="rId28" display="Ali Express Link"/>
-    <hyperlink ref="E30" r:id="rId29" display="Amazon link"/>
-    <hyperlink ref="E31" r:id="rId30" display="Amazon link"/>
-    <hyperlink ref="E32" r:id="rId31" display="Amazon link"/>
-    <hyperlink ref="E33" r:id="rId32" display="Amazon link"/>
-    <hyperlink ref="E37" r:id="rId33" display="Amazon link"/>
-    <hyperlink ref="E38" r:id="rId34" display="Amazon link"/>
-    <hyperlink ref="E39" r:id="rId35" display="Amazon link"/>
-    <hyperlink ref="E40" r:id="rId36" display="Ali Express  link"/>
-    <hyperlink ref="E43" r:id="rId37" display="Amazon link - assortment"/>
-    <hyperlink ref="E48" r:id="rId38" display="Amazon link"/>
-    <hyperlink ref="E53" r:id="rId39" display="Amazon link"/>
-    <hyperlink ref="E54" r:id="rId40" display="Amazon link for raw copper tubing"/>
-    <hyperlink ref="F54" r:id="rId41" display="Amazon link for aluminum cooler"/>
-    <hyperlink ref="E55" r:id="rId42" display="Amazon link"/>
-    <hyperlink ref="E57" r:id="rId43" display="Amazon link"/>
-    <hyperlink ref="E62" r:id="rId44" display="Amazon link"/>
-    <hyperlink ref="G62" r:id="rId45" display="Amazon link  This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
-    <hyperlink ref="E63" r:id="rId46" display="Amazon link"/>
-    <hyperlink ref="E64" r:id="rId47" display="Amazon link"/>
-    <hyperlink ref="E65" r:id="rId48" display="Amazon Link"/>
-    <hyperlink ref="E66" r:id="rId49" display="MicroLab link"/>
-    <hyperlink ref="F66" r:id="rId50" display="Github Link"/>
-    <hyperlink ref="F67" r:id="rId51" display="Amazon link"/>
-    <hyperlink ref="G67" r:id="rId52" display="NOTE: New Reactor Core uses a GL45 250ml bottle instead!"/>
-    <hyperlink ref="E68" r:id="rId53" display="Amazon link"/>
-    <hyperlink ref="E69" r:id="rId54" display="MicroLab link"/>
-    <hyperlink ref="F69" r:id="rId55" display="Github Link"/>
-    <hyperlink ref="E70" r:id="rId56" display="MicroLab link"/>
-    <hyperlink ref="F70" r:id="rId57" display="Github Link"/>
-    <hyperlink ref="E71" r:id="rId58" display="MicroLab link"/>
-    <hyperlink ref="F71" r:id="rId59" display="Github Link"/>
-    <hyperlink ref="E72" r:id="rId60" display="MicroLab link"/>
-    <hyperlink ref="F72" r:id="rId61" display="Github Link"/>
-    <hyperlink ref="E73" r:id="rId62" display="Ali Express link"/>
-    <hyperlink ref="G73" r:id="rId63" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
-    <hyperlink ref="E74" r:id="rId64" display="Amazon link"/>
-    <hyperlink ref="F74" r:id="rId65" display="Alibaba Link"/>
-    <hyperlink ref="E75" r:id="rId66" display="Amazon link"/>
-    <hyperlink ref="E76" r:id="rId67" display="MicroLab link"/>
-    <hyperlink ref="F76" r:id="rId68" display="Github Link"/>
-    <hyperlink ref="E77" r:id="rId69" display="MicroLab link"/>
-    <hyperlink ref="F77" r:id="rId70" display="Github Link"/>
+    <hyperlink ref="A2" r:id="rId1" display="NOTE 0: THIS PARTS LIST IS DEPRECATED. DO NOT UPDATE IT. DO NOT USE IT. USE AND UPDATE THE parts-list.md FILE INSTEAD. THIS FILE IS TO KEEP LINKS ALIVE ONLY."/>
+    <hyperlink ref="E10" r:id="rId2" display="Amazon link"/>
+    <hyperlink ref="F10" r:id="rId3" display="Amazon Le Potato link2"/>
+    <hyperlink ref="E11" r:id="rId4" display="Amazon link"/>
+    <hyperlink ref="E12" r:id="rId5" display="Amazon link"/>
+    <hyperlink ref="E13" r:id="rId6" display="Amazon Link"/>
+    <hyperlink ref="E14" r:id="rId7" display="Ali Express link (kit)&#10;- be sure to pick option with UNO board"/>
+    <hyperlink ref="F14" r:id="rId8" display="Amazon link"/>
+    <hyperlink ref="F15" r:id="rId9" display="Amazon Link (Kit)"/>
+    <hyperlink ref="F16" r:id="rId10" display="Amazon Link"/>
+    <hyperlink ref="E18" r:id="rId11" display="Amazon link"/>
+    <hyperlink ref="E19" r:id="rId12" display="Ali Express link"/>
+    <hyperlink ref="F19" r:id="rId13" display="Amazon link - assortment"/>
+    <hyperlink ref="E20" r:id="rId14" display="Amazon link"/>
+    <hyperlink ref="E21" r:id="rId15" display="Amazon link"/>
+    <hyperlink ref="E22" r:id="rId16" display="Amazon link"/>
+    <hyperlink ref="E23" r:id="rId17" display="MicroLab link"/>
+    <hyperlink ref="F23" r:id="rId18" display="Github Link"/>
+    <hyperlink ref="E24" r:id="rId19" display="MicroLab link"/>
+    <hyperlink ref="F24" r:id="rId20" display="Github Link"/>
+    <hyperlink ref="E25" r:id="rId21" display="MicroLab link"/>
+    <hyperlink ref="F25" r:id="rId22" display="Github Link"/>
+    <hyperlink ref="E26" r:id="rId23" display="MicroLab link"/>
+    <hyperlink ref="F26" r:id="rId24" display="Github Link"/>
+    <hyperlink ref="E27" r:id="rId25" display="Amazon link"/>
+    <hyperlink ref="E28" r:id="rId26" display="Ali Express Link"/>
+    <hyperlink ref="F28" r:id="rId27" display="Amazon Link"/>
+    <hyperlink ref="E29" r:id="rId28" display="Amazon link"/>
+    <hyperlink ref="F29" r:id="rId29" display="Ali Express Link"/>
+    <hyperlink ref="E30" r:id="rId30" display="Amazon link"/>
+    <hyperlink ref="E31" r:id="rId31" display="Amazon link"/>
+    <hyperlink ref="E32" r:id="rId32" display="Amazon link"/>
+    <hyperlink ref="E33" r:id="rId33" display="Amazon link"/>
+    <hyperlink ref="E37" r:id="rId34" display="Amazon link"/>
+    <hyperlink ref="E38" r:id="rId35" display="Amazon link"/>
+    <hyperlink ref="E39" r:id="rId36" display="Amazon link"/>
+    <hyperlink ref="E40" r:id="rId37" display="Ali Express  link"/>
+    <hyperlink ref="E43" r:id="rId38" display="Amazon link - assortment"/>
+    <hyperlink ref="E48" r:id="rId39" display="Amazon link"/>
+    <hyperlink ref="E53" r:id="rId40" display="Amazon link"/>
+    <hyperlink ref="E54" r:id="rId41" display="Amazon link for raw copper tubing"/>
+    <hyperlink ref="F54" r:id="rId42" display="Amazon link for aluminum cooler"/>
+    <hyperlink ref="E55" r:id="rId43" display="Amazon link"/>
+    <hyperlink ref="E57" r:id="rId44" display="Amazon link"/>
+    <hyperlink ref="E62" r:id="rId45" display="Amazon link"/>
+    <hyperlink ref="G62" r:id="rId46" display="Amazon link  This link is to a 100 RPM 12v motor. You can also buy a faster motor and use a PWM controller to adjust the speed manually."/>
+    <hyperlink ref="E63" r:id="rId47" display="Amazon link"/>
+    <hyperlink ref="E64" r:id="rId48" display="Amazon link"/>
+    <hyperlink ref="E65" r:id="rId49" display="Amazon Link"/>
+    <hyperlink ref="E66" r:id="rId50" display="MicroLab link"/>
+    <hyperlink ref="F66" r:id="rId51" display="Github Link"/>
+    <hyperlink ref="F67" r:id="rId52" display="Amazon link"/>
+    <hyperlink ref="G67" r:id="rId53" display="NOTE: New Reactor Core uses a GL45 250ml bottle instead!"/>
+    <hyperlink ref="E68" r:id="rId54" display="Amazon link"/>
+    <hyperlink ref="E69" r:id="rId55" display="MicroLab link"/>
+    <hyperlink ref="F69" r:id="rId56" display="Github Link"/>
+    <hyperlink ref="E70" r:id="rId57" display="MicroLab link"/>
+    <hyperlink ref="F70" r:id="rId58" display="Github Link"/>
+    <hyperlink ref="E71" r:id="rId59" display="MicroLab link"/>
+    <hyperlink ref="F71" r:id="rId60" display="Github Link"/>
+    <hyperlink ref="E72" r:id="rId61" display="MicroLab link"/>
+    <hyperlink ref="F72" r:id="rId62" display="Github Link"/>
+    <hyperlink ref="E73" r:id="rId63" display="Ali Express link"/>
+    <hyperlink ref="G73" r:id="rId64" display="Used to monitor the temperature in the reaction chamber. This is a link to a USB DS18B20 "/>
+    <hyperlink ref="E74" r:id="rId65" display="Amazon link"/>
+    <hyperlink ref="F74" r:id="rId66" display="Alibaba Link"/>
+    <hyperlink ref="E75" r:id="rId67" display="Amazon link"/>
+    <hyperlink ref="E76" r:id="rId68" display="MicroLab link"/>
+    <hyperlink ref="F76" r:id="rId69" display="Github Link"/>
+    <hyperlink ref="E77" r:id="rId70" display="MicroLab link"/>
+    <hyperlink ref="F77" r:id="rId71" display="Github Link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8502,773 +8508,773 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="57" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D2" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H2" s="52" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I2" s="59" t="n">
         <v>7.1</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="57" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E3" s="60" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I3" s="59" t="n">
         <v>5.49</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="57" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F4" s="58" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H4" s="61" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I4" s="59" t="n">
         <v>25.9</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K4" s="59" t="n">
         <v>47.98</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="57" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H5" s="52"/>
       <c r="I5" s="59" t="n">
         <v>7.36</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="57" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="59"/>
       <c r="J6" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="57" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>4</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="59" t="n">
         <v>9.99</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="57" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H8" s="52" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I8" s="59" t="n">
         <v>8.99</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="57" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D9" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H9" s="52"/>
       <c r="I9" s="59"/>
     </row>
     <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="57" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D10" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="58" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F10" s="58" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H10" s="52" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I10" s="59" t="n">
         <v>25.99</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="57" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D11" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H11" s="52" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I11" s="59" t="n">
         <v>5.99</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="57" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C12" s="57" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="58" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="52" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I12" s="59" t="n">
         <v>13.99</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="57" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B13" s="57" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C13" s="57" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="52" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I13" s="59"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="57" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B14" s="57" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C14" s="57" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D14" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H14" s="52"/>
       <c r="I14" s="59" t="n">
         <v>3.82</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="57" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D15" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H15" s="52" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I15" s="59" t="n">
         <v>36.99</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="57" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C16" s="57" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D16" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H16" s="52"/>
       <c r="I16" s="59" t="n">
         <v>10.91</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="57" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C17" s="57" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D17" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F17" s="6"/>
       <c r="H17" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I17" s="59" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="57" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D18" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H18" s="52" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="I18" s="59" t="n">
         <v>13.25</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="57" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D19" s="6" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H19" s="52" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I19" s="59" t="n">
         <v>64.08</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="57" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D20" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H20" s="52"/>
       <c r="I20" s="59"/>
       <c r="J20" s="6" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="57" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C21" s="57" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D21" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H21" s="52"/>
       <c r="I21" s="59" t="n">
         <v>26.79</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="57" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D22" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="59"/>
       <c r="J22" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="57" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D23" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H23" s="52"/>
       <c r="I23" s="59"/>
       <c r="J23" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="57" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B24" s="57" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D24" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H24" s="52"/>
       <c r="I24" s="59"/>
       <c r="J24" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="57" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D25" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H25" s="52"/>
       <c r="I25" s="59"/>
       <c r="J25" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="57" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C26" s="57" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D26" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H26" s="52"/>
       <c r="I26" s="59"/>
       <c r="J26" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="57" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D27" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H27" s="52"/>
       <c r="I27" s="59"/>
       <c r="J27" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="57" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B28" s="57" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D28" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H28" s="52"/>
       <c r="I28" s="59"/>
       <c r="J28" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="57" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B29" s="57" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D29" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F29" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H29" s="52"/>
       <c r="I29" s="59" t="n">
         <v>13.7</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K29" s="6" t="n">
         <v>13.99</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="57" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B30" s="57" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H30" s="52" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="I30" s="59" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="57"/>
       <c r="B31" s="57" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E31" s="62"/>
       <c r="H31" s="52"/>
@@ -9277,10 +9283,10 @@
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="57"/>
       <c r="B32" s="57" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E32" s="62"/>
       <c r="H32" s="52"/>
@@ -9289,10 +9295,10 @@
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="57"/>
       <c r="B33" s="57" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E33" s="62"/>
       <c r="H33" s="52"/>
@@ -9300,119 +9306,119 @@
     </row>
     <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="57" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C34" s="63" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D34" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H34" s="52"/>
       <c r="I34" s="59" t="n">
         <v>11.98</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="57" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B35" s="57" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C35" s="57" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D35" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F35" s="58" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="H35" s="52"/>
       <c r="I35" s="59" t="n">
         <v>7.63</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K35" s="6" t="n">
         <v>19.99</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="57" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B36" s="57" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C36" s="57" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D36" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H36" s="52"/>
       <c r="I36" s="59"/>
       <c r="J36" s="6" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="57" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B37" s="57" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C37" s="57" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D37" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E37" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H37" s="52" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="I37" s="59" t="n">
         <v>1.18</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="57" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B38" s="57"/>
       <c r="C38" s="57" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D38" s="6" t="n">
         <v>1</v>
@@ -9422,69 +9428,69 @@
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="57" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B39" s="57" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D39" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E39" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H39" s="52"/>
       <c r="I39" s="59" t="n">
         <v>9.35</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="57"/>
       <c r="B40" s="57" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C40" s="57" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H40" s="52" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="I40" s="59" t="n">
         <v>16.99</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="57"/>
       <c r="B41" s="57" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D41" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E41" s="58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H41" s="52"/>
       <c r="I41" s="64" t="n">
         <v>8.99</v>
       </c>
       <c r="J41" s="65" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9498,7 +9504,7 @@
         <v>37</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9506,32 +9512,32 @@
         <v>3.9</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J45" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="6" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="I46" s="59" t="n">
         <v>4</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9539,24 +9545,24 @@
         <v>9.85</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="65" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="J48" s="65" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K48" s="65" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>